<commit_message>
Pew Dataset Processing - summary statistics wireframing and australia case study info
</commit_message>
<xml_diff>
--- a/data_processing/pew/pewQVDict.xlsx
+++ b/data_processing/pew/pewQVDict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natalie_kraft/Documents/LAS/bridash/data_processing/pew/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34FA372E-37AF-994C-BDF9-0FF63FE9DBDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB4D722-EB00-244E-BFFA-F03D2806787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36500" yWindow="-16260" windowWidth="34640" windowHeight="20320" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6276" uniqueCount="4208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6276" uniqueCount="4209">
   <si>
     <t>variable_name</t>
   </si>
@@ -12688,6 +12688,9 @@
   </si>
   <si>
     <t>econ_ties_usch: How do you view current economic ties between the U.S. and China?</t>
+  </si>
+  <si>
+    <t>qdate</t>
   </si>
 </sst>
 </file>
@@ -12948,9 +12951,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -12996,6 +12996,9 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -37572,38 +37575,38 @@
     <col min="13" max="16384" width="10.83203125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="14" customFormat="1" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="12">
+    <row r="1" spans="1:13" s="13" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="34">
         <v>2021</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34">
         <v>2020</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12">
+      <c r="D1" s="34"/>
+      <c r="E1" s="34">
         <v>2019</v>
       </c>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12">
+      <c r="F1" s="34"/>
+      <c r="G1" s="34">
         <v>2018</v>
       </c>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12">
+      <c r="H1" s="34"/>
+      <c r="I1" s="34">
         <v>2017</v>
       </c>
-      <c r="J1" s="12"/>
-      <c r="K1" s="14" t="s">
+      <c r="J1" s="34"/>
+      <c r="K1" s="13" t="s">
         <v>4023</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="13" t="s">
         <v>4024</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="13" t="s">
         <v>4025</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
@@ -37636,529 +37639,529 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="23" t="s">
         <v>226</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
         <v>1380</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="15" t="s">
         <v>226</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="18" t="s">
         <v>452</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="15" t="s">
         <v>226</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="18" t="s">
         <v>1380</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="15" t="s">
         <v>226</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="18" t="s">
         <v>2396</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="15" t="s">
         <v>227</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="J3" s="18" t="s">
         <v>2397</v>
       </c>
-      <c r="K3" s="26" t="s">
+      <c r="K3" s="25" t="s">
         <v>4035</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="23" t="s">
         <v>227</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="19" t="s">
         <v>1381</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="15" t="s">
         <v>227</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="18" t="s">
         <v>453</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="15" t="s">
         <v>227</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="18" t="s">
         <v>1381</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="15" t="s">
         <v>227</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="18" t="s">
         <v>2397</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="15" t="s">
         <v>226</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="J4" s="18" t="s">
         <v>2396</v>
       </c>
-      <c r="K4" s="26" t="s">
+      <c r="K4" s="25" t="s">
         <v>4036</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="23" t="s">
         <v>677</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="19" t="s">
         <v>1191</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="18" t="s">
         <v>338</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="15" t="s">
         <v>677</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="18" t="s">
         <v>1191</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="18" t="s">
         <v>2208</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="J5" s="18" t="s">
         <v>3400</v>
       </c>
-      <c r="K5" s="26" t="s">
+      <c r="K5" s="25" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="23" t="s">
         <v>678</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="19" t="s">
         <v>1192</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="18" t="s">
         <v>339</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="15" t="s">
         <v>678</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="18" t="s">
         <v>1192</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="H6" s="18" t="s">
         <v>339</v>
       </c>
-      <c r="I6" s="16" t="s">
+      <c r="I6" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="J6" s="19" t="s">
+      <c r="J6" s="18" t="s">
         <v>3401</v>
       </c>
-      <c r="K6" s="26" t="s">
+      <c r="K6" s="25" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="16"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="26" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="25" t="s">
         <v>188</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="18" t="s">
         <v>414</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="15" t="s">
         <v>823</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="18" t="s">
         <v>1352</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="18" t="s">
         <v>2362</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="I7" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="J7" s="19" t="s">
+      <c r="J7" s="18" t="s">
         <v>3590</v>
       </c>
-      <c r="K7" s="26" t="s">
+      <c r="K7" s="25" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="23" t="s">
         <v>3814</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="19" t="s">
         <v>3930</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="18" t="s">
         <v>415</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="15" t="s">
         <v>824</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="F8" s="18" t="s">
         <v>1353</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G8" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="H8" s="18" t="s">
         <v>2363</v>
       </c>
-      <c r="I8" s="16" t="s">
+      <c r="I8" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="J8" s="19" t="s">
+      <c r="J8" s="18" t="s">
         <v>3591</v>
       </c>
-      <c r="K8" s="26" t="s">
+      <c r="K8" s="25" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="17" t="s">
         <v>228</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="F9" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="H9" s="19" t="s">
+      <c r="H9" s="18" t="s">
         <v>1929</v>
       </c>
-      <c r="I9" s="16" t="s">
+      <c r="I9" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="J9" s="19" t="s">
+      <c r="J9" s="18" t="s">
         <v>1929</v>
       </c>
-      <c r="K9" s="26" t="s">
+      <c r="K9" s="25" t="s">
         <v>4029</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="16"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="16" t="s">
+      <c r="A10" s="15"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="18" t="s">
         <v>230</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="F10" s="18" t="s">
         <v>230</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="15" t="s">
         <v>1463</v>
       </c>
-      <c r="H10" s="19" t="s">
+      <c r="H10" s="18" t="s">
         <v>230</v>
       </c>
-      <c r="I10" s="16" t="s">
+      <c r="I10" s="15" t="s">
         <v>230</v>
       </c>
-      <c r="J10" s="19" t="s">
+      <c r="J10" s="18" t="s">
         <v>230</v>
       </c>
-      <c r="K10" s="16" t="s">
+      <c r="K10" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="23" t="s">
         <v>456</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="19" t="s">
         <v>3854</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="18" t="s">
         <v>240</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="15" t="s">
         <v>456</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="F11" s="18" t="s">
         <v>930</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="19" t="s">
+      <c r="H11" s="18" t="s">
         <v>1931</v>
       </c>
-      <c r="I11" s="16" t="s">
+      <c r="I11" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="J11" s="19" t="s">
+      <c r="J11" s="18" t="s">
         <v>3000</v>
       </c>
-      <c r="K11" s="26" t="s">
+      <c r="K11" s="25" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="23" t="s">
         <v>457</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="19" t="s">
         <v>3855</v>
       </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="16" t="s">
+      <c r="D12" s="18"/>
+      <c r="E12" s="15" t="s">
         <v>457</v>
       </c>
-      <c r="F12" s="19" t="s">
+      <c r="F12" s="18" t="s">
         <v>931</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="G12" s="15" t="s">
         <v>1465</v>
       </c>
-      <c r="H12" s="19" t="s">
+      <c r="H12" s="18" t="s">
         <v>1932</v>
       </c>
-      <c r="I12" s="16" t="s">
+      <c r="I12" s="15" t="s">
         <v>1465</v>
       </c>
-      <c r="J12" s="19" t="s">
+      <c r="J12" s="18" t="s">
         <v>3003</v>
       </c>
-      <c r="K12" s="26" t="s">
+      <c r="K12" s="25" t="s">
         <v>4030</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="23" t="s">
         <v>461</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="19" t="s">
         <v>3857</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="18" t="s">
         <v>242</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="F13" s="19" t="s">
+      <c r="F13" s="18" t="s">
         <v>935</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="19" t="s">
+      <c r="H13" s="18" t="s">
         <v>1943</v>
       </c>
-      <c r="I13" s="16" t="s">
+      <c r="I13" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="J13" s="19" t="s">
+      <c r="J13" s="18" t="s">
         <v>3007</v>
       </c>
-      <c r="K13" s="26" t="s">
+      <c r="K13" s="25" t="s">
         <v>4031</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="23" t="s">
         <v>462</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="19" t="s">
         <v>3858</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="18" t="s">
         <v>243</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="15" t="s">
         <v>462</v>
       </c>
-      <c r="F14" s="19" t="s">
+      <c r="F14" s="18" t="s">
         <v>936</v>
       </c>
-      <c r="G14" s="16" t="s">
+      <c r="G14" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H14" s="19" t="s">
+      <c r="H14" s="18" t="s">
         <v>1944</v>
       </c>
-      <c r="I14" s="16" t="s">
+      <c r="I14" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="J14" s="19" t="s">
+      <c r="J14" s="18" t="s">
         <v>3009</v>
       </c>
-      <c r="K14" s="26" t="s">
+      <c r="K14" s="25" t="s">
         <v>4032</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B15" s="19"/>
-      <c r="C15" s="26" t="s">
+      <c r="B15" s="18"/>
+      <c r="C15" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="18" t="s">
         <v>244</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="15" t="s">
         <v>463</v>
       </c>
-      <c r="F15" s="19" t="s">
+      <c r="F15" s="18" t="s">
         <v>937</v>
       </c>
-      <c r="G15" s="16" t="s">
+      <c r="G15" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="H15" s="19" t="s">
+      <c r="H15" s="18" t="s">
         <v>1945</v>
       </c>
-      <c r="I15" s="16" t="s">
+      <c r="I15" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="J15" s="19" t="s">
+      <c r="J15" s="18" t="s">
         <v>3011</v>
       </c>
-      <c r="K15" s="26" t="s">
+      <c r="K15" s="25" t="s">
         <v>4033</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="26" t="s">
+      <c r="B16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="25" t="s">
         <v>455</v>
       </c>
-      <c r="F16" s="19" t="s">
+      <c r="F16" s="18" t="s">
         <v>929</v>
       </c>
-      <c r="G16" s="16" t="s">
+      <c r="G16" s="15" t="s">
         <v>1464</v>
       </c>
-      <c r="H16" s="19" t="s">
+      <c r="H16" s="18" t="s">
         <v>1930</v>
       </c>
-      <c r="I16" s="16" t="s">
+      <c r="I16" s="15" t="s">
         <v>1464</v>
       </c>
-      <c r="J16" s="19" t="s">
+      <c r="J16" s="18" t="s">
         <v>929</v>
       </c>
-      <c r="K16" s="26" t="s">
+      <c r="K16" s="25" t="s">
         <v>1464</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="23" t="s">
         <v>458</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="19" t="s">
         <v>3856</v>
       </c>
-      <c r="D17" s="19"/>
-      <c r="E17" s="16" t="s">
+      <c r="D17" s="18"/>
+      <c r="E17" s="15" t="s">
         <v>458</v>
       </c>
-      <c r="F17" s="19" t="s">
+      <c r="F17" s="18" t="s">
         <v>932</v>
       </c>
-      <c r="G17" s="16" t="s">
+      <c r="G17" s="15" t="s">
         <v>1466</v>
       </c>
-      <c r="H17" s="19" t="s">
+      <c r="H17" s="18" t="s">
         <v>1933</v>
       </c>
-      <c r="I17" s="16" t="s">
+      <c r="I17" s="15" t="s">
         <v>1466</v>
       </c>
-      <c r="J17" s="19" t="s">
+      <c r="J17" s="18" t="s">
         <v>3004</v>
       </c>
-      <c r="K17" s="26" t="s">
+      <c r="K17" s="25" t="s">
         <v>1466</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="12" t="s">
         <v>3785</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="19" t="s">
         <v>3895</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="18" t="s">
         <v>326</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="E18" s="15" t="s">
         <v>604</v>
       </c>
-      <c r="F18" s="19" t="s">
+      <c r="F18" s="18" t="s">
         <v>1118</v>
       </c>
-      <c r="G18" s="16" t="s">
+      <c r="G18" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="H18" s="19" t="s">
+      <c r="H18" s="18" t="s">
         <v>2085</v>
       </c>
-      <c r="I18" s="16" t="s">
+      <c r="I18" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="J18" s="19" t="s">
+      <c r="J18" s="18" t="s">
         <v>3102</v>
       </c>
-      <c r="K18" s="26" t="s">
+      <c r="K18" s="25" t="s">
         <v>4026</v>
       </c>
       <c r="M18" s="10" t="s">
@@ -38166,137 +38169,137 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="23" t="s">
         <v>605</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="19" t="s">
         <v>3896</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="18" t="s">
         <v>327</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="E19" s="15" t="s">
         <v>605</v>
       </c>
-      <c r="F19" s="19" t="s">
+      <c r="F19" s="18" t="s">
         <v>1119</v>
       </c>
-      <c r="G19" s="16" t="s">
+      <c r="G19" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="H19" s="19" t="s">
+      <c r="H19" s="18" t="s">
         <v>2086</v>
       </c>
-      <c r="I19" s="16" t="s">
+      <c r="I19" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="J19" s="19" t="s">
+      <c r="J19" s="18" t="s">
         <v>3103</v>
       </c>
-      <c r="K19" s="26" t="s">
+      <c r="K19" s="25" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="24" t="s">
+      <c r="A20" s="23" t="s">
         <v>606</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="19" t="s">
         <v>3897</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="18" t="s">
         <v>328</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="15" t="s">
         <v>606</v>
       </c>
-      <c r="F20" s="19" t="s">
+      <c r="F20" s="18" t="s">
         <v>1120</v>
       </c>
-      <c r="G20" s="16" t="s">
+      <c r="G20" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="H20" s="19" t="s">
+      <c r="H20" s="18" t="s">
         <v>2087</v>
       </c>
-      <c r="I20" s="16" t="s">
+      <c r="I20" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="J20" s="19" t="s">
+      <c r="J20" s="18" t="s">
         <v>3104</v>
       </c>
-      <c r="K20" s="26" t="s">
+      <c r="K20" s="25" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="23" t="s">
         <v>742</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="19" t="s">
         <v>3927</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="18" t="s">
         <v>358</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E21" s="15" t="s">
         <v>742</v>
       </c>
-      <c r="F21" s="19" t="s">
+      <c r="F21" s="18" t="s">
         <v>1258</v>
       </c>
-      <c r="G21" s="16" t="s">
+      <c r="G21" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="H21" s="19" t="s">
+      <c r="H21" s="18" t="s">
         <v>2257</v>
       </c>
-      <c r="I21" s="16" t="s">
+      <c r="I21" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="J21" s="19" t="s">
+      <c r="J21" s="18" t="s">
         <v>3484</v>
       </c>
-      <c r="K21" s="26" t="s">
+      <c r="K21" s="25" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B22" s="19"/>
-      <c r="C22" s="26" t="s">
+      <c r="B22" s="18"/>
+      <c r="C22" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="18" t="s">
         <v>325</v>
       </c>
-      <c r="E22" s="16" t="s">
+      <c r="E22" s="15" t="s">
         <v>598</v>
       </c>
-      <c r="F22" s="19" t="s">
+      <c r="F22" s="18" t="s">
         <v>1112</v>
       </c>
-      <c r="G22" s="16" t="s">
+      <c r="G22" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="H22" s="19" t="s">
+      <c r="H22" s="18" t="s">
         <v>2067</v>
       </c>
-      <c r="I22" s="16" t="s">
+      <c r="I22" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="J22" s="19" t="s">
+      <c r="J22" s="18" t="s">
         <v>3084</v>
       </c>
-      <c r="K22" s="26"/>
+      <c r="K22" s="25"/>
       <c r="L22" s="10" t="s">
         <v>4057</v>
       </c>
@@ -38305,170 +38308,170 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="23" t="s">
         <v>3758</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="19" t="s">
         <v>3866</v>
       </c>
-      <c r="D23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="16" t="s">
+      <c r="D23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="15" t="s">
         <v>1590</v>
       </c>
-      <c r="H23" s="19" t="s">
+      <c r="H23" s="18" t="s">
         <v>2068</v>
       </c>
-      <c r="I23" s="16" t="s">
+      <c r="I23" s="15" t="s">
         <v>1590</v>
       </c>
-      <c r="J23" s="19" t="s">
+      <c r="J23" s="18" t="s">
         <v>3088</v>
       </c>
-      <c r="K23" s="26" t="s">
+      <c r="K23" s="25" t="s">
         <v>1590</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="23" t="s">
         <v>3759</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="19" t="s">
         <v>3867</v>
       </c>
-      <c r="D24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="16" t="s">
+      <c r="D24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="15" t="s">
         <v>1591</v>
       </c>
-      <c r="H24" s="19" t="s">
+      <c r="H24" s="18" t="s">
         <v>2069</v>
       </c>
-      <c r="I24" s="16" t="s">
+      <c r="I24" s="15" t="s">
         <v>1591</v>
       </c>
-      <c r="J24" s="19" t="s">
+      <c r="J24" s="18" t="s">
         <v>3089</v>
       </c>
-      <c r="K24" s="26" t="s">
+      <c r="K24" s="25" t="s">
         <v>1591</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B25" s="19"/>
-      <c r="C25" s="16" t="s">
+      <c r="B25" s="18"/>
+      <c r="C25" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="19" t="s">
+      <c r="D25" s="18" t="s">
         <v>241</v>
       </c>
-      <c r="F25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="16" t="s">
+      <c r="F25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J25" s="19" t="s">
+      <c r="J25" s="18" t="s">
         <v>3001</v>
       </c>
-      <c r="K25" s="26" t="s">
+      <c r="K25" s="25" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B26" s="19"/>
-      <c r="C26" s="16" t="s">
+      <c r="B26" s="18"/>
+      <c r="C26" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="D26" s="19" t="s">
+      <c r="D26" s="18" t="s">
         <v>318</v>
       </c>
-      <c r="G26" s="16" t="s">
+      <c r="G26" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="H26" s="19" t="s">
+      <c r="H26" s="18" t="s">
         <v>2061</v>
       </c>
-      <c r="I26" s="16" t="s">
+      <c r="I26" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="J26" s="19" t="s">
+      <c r="J26" s="18" t="s">
         <v>3078</v>
       </c>
-      <c r="K26" s="26" t="s">
+      <c r="K26" s="25" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="16" t="s">
+      <c r="B27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="15" t="s">
         <v>621</v>
       </c>
-      <c r="F27" s="19" t="s">
+      <c r="F27" s="18" t="s">
         <v>1135</v>
       </c>
-      <c r="I27" s="16" t="s">
+      <c r="I27" s="15" t="s">
         <v>2567</v>
       </c>
-      <c r="J27" s="19" t="s">
+      <c r="J27" s="18" t="s">
         <v>3154</v>
       </c>
-      <c r="K27" s="26" t="s">
+      <c r="K27" s="25" t="s">
         <v>2567</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="16" t="s">
+      <c r="B28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="15" t="s">
         <v>622</v>
       </c>
-      <c r="F28" s="19" t="s">
+      <c r="F28" s="18" t="s">
         <v>1136</v>
       </c>
-      <c r="I28" s="16" t="s">
+      <c r="I28" s="15" t="s">
         <v>2568</v>
       </c>
-      <c r="J28" s="19" t="s">
+      <c r="J28" s="18" t="s">
         <v>3155</v>
       </c>
-      <c r="K28" s="26" t="s">
+      <c r="K28" s="25" t="s">
         <v>2568</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="12" t="s">
         <v>3784</v>
       </c>
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="19" t="s">
         <v>3893</v>
       </c>
-      <c r="D29" s="19"/>
-      <c r="E29" s="16" t="s">
+      <c r="D29" s="18"/>
+      <c r="E29" s="15" t="s">
         <v>601</v>
       </c>
-      <c r="F29" s="19" t="s">
+      <c r="F29" s="18" t="s">
         <v>1115</v>
       </c>
-      <c r="K29" s="26" t="s">
+      <c r="K29" s="25" t="s">
         <v>4034</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A30" s="13" t="s">
+      <c r="A30" s="12" t="s">
         <v>599</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="19" t="s">
         <v>3894</v>
       </c>
-      <c r="D30" s="19"/>
-      <c r="E30" s="16" t="s">
+      <c r="D30" s="18"/>
+      <c r="E30" s="15" t="s">
         <v>599</v>
       </c>
-      <c r="F30" s="19" t="s">
+      <c r="F30" s="18" t="s">
         <v>1113</v>
       </c>
-      <c r="K30" s="16"/>
+      <c r="K30" s="15"/>
       <c r="L30" s="10" t="s">
         <v>4056</v>
       </c>
@@ -38477,34 +38480,34 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="12" t="s">
         <v>3774</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="19" t="s">
         <v>3883</v>
       </c>
-      <c r="I31" s="17"/>
-      <c r="J31" s="19"/>
-      <c r="K31" s="17" t="s">
+      <c r="I31" s="16"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="16" t="s">
         <v>4058</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="22"/>
-      <c r="B32" s="20"/>
-      <c r="E32" s="16" t="s">
+      <c r="A32" s="21"/>
+      <c r="B32" s="19"/>
+      <c r="E32" s="15" t="s">
         <v>625</v>
       </c>
-      <c r="F32" s="19" t="s">
+      <c r="F32" s="18" t="s">
         <v>1139</v>
       </c>
-      <c r="G32" s="16" t="s">
+      <c r="G32" s="15" t="s">
         <v>1682</v>
       </c>
-      <c r="H32" s="19" t="s">
+      <c r="H32" s="18" t="s">
         <v>2165</v>
       </c>
-      <c r="K32" s="26" t="s">
+      <c r="K32" s="25" t="s">
         <v>4038</v>
       </c>
       <c r="M32" s="10" t="s">
@@ -38512,25 +38515,25 @@
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="E33" s="16" t="s">
+      <c r="E33" s="15" t="s">
         <v>626</v>
       </c>
-      <c r="F33" s="19" t="s">
+      <c r="F33" s="18" t="s">
         <v>1140</v>
       </c>
-      <c r="G33" s="16" t="s">
+      <c r="G33" s="15" t="s">
         <v>1580</v>
       </c>
-      <c r="H33" s="19" t="s">
+      <c r="H33" s="18" t="s">
         <v>2054</v>
       </c>
-      <c r="I33" s="16" t="s">
+      <c r="I33" s="15" t="s">
         <v>1580</v>
       </c>
-      <c r="J33" s="19" t="s">
+      <c r="J33" s="18" t="s">
         <v>3071</v>
       </c>
-      <c r="K33" s="26" t="s">
+      <c r="K33" s="25" t="s">
         <v>4039</v>
       </c>
       <c r="M33" s="10" t="s">
@@ -38538,19 +38541,19 @@
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="E34" s="16" t="s">
+      <c r="E34" s="15" t="s">
         <v>623</v>
       </c>
-      <c r="F34" s="19" t="s">
+      <c r="F34" s="18" t="s">
         <v>1137</v>
       </c>
-      <c r="G34" s="16" t="s">
+      <c r="G34" s="15" t="s">
         <v>1681</v>
       </c>
-      <c r="H34" s="19" t="s">
+      <c r="H34" s="18" t="s">
         <v>2164</v>
       </c>
-      <c r="K34" s="26" t="s">
+      <c r="K34" s="25" t="s">
         <v>4040</v>
       </c>
       <c r="M34" s="10" t="s">
@@ -38558,26 +38561,26 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="17"/>
-      <c r="E35" s="16" t="s">
+      <c r="A35" s="16"/>
+      <c r="E35" s="15" t="s">
         <v>624</v>
       </c>
-      <c r="F35" s="19" t="s">
+      <c r="F35" s="18" t="s">
         <v>1138</v>
       </c>
-      <c r="G35" s="16" t="s">
+      <c r="G35" s="15" t="s">
         <v>1581</v>
       </c>
-      <c r="H35" s="19" t="s">
+      <c r="H35" s="18" t="s">
         <v>2055</v>
       </c>
-      <c r="I35" s="16" t="s">
+      <c r="I35" s="15" t="s">
         <v>2508</v>
       </c>
-      <c r="J35" s="19" t="s">
+      <c r="J35" s="18" t="s">
         <v>3072</v>
       </c>
-      <c r="K35" s="26" t="s">
+      <c r="K35" s="25" t="s">
         <v>4041</v>
       </c>
       <c r="M35" s="10" t="s">
@@ -38585,39 +38588,39 @@
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A36" s="17"/>
-      <c r="G36" s="16" t="s">
+      <c r="A36" s="16"/>
+      <c r="G36" s="15" t="s">
         <v>1582</v>
       </c>
-      <c r="H36" s="19" t="s">
+      <c r="H36" s="18" t="s">
         <v>2056</v>
       </c>
-      <c r="I36" s="16" t="s">
+      <c r="I36" s="15" t="s">
         <v>1582</v>
       </c>
-      <c r="J36" s="19" t="s">
+      <c r="J36" s="18" t="s">
         <v>3073</v>
       </c>
-      <c r="K36" s="26" t="s">
+      <c r="K36" s="25" t="s">
         <v>4042</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="22"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="16" t="s">
+      <c r="A37" s="21"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="D37" s="19" t="s">
+      <c r="D37" s="18" t="s">
         <v>333</v>
       </c>
-      <c r="I37" s="16" t="s">
+      <c r="I37" s="15" t="s">
         <v>2745</v>
       </c>
-      <c r="J37" s="19" t="s">
+      <c r="J37" s="18" t="s">
         <v>3357</v>
       </c>
-      <c r="K37" s="26" t="s">
+      <c r="K37" s="25" t="s">
         <v>4044</v>
       </c>
       <c r="M37" s="10" t="s">
@@ -38625,596 +38628,596 @@
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B38" s="19"/>
-      <c r="I38" s="16" t="s">
+      <c r="B38" s="18"/>
+      <c r="I38" s="15" t="s">
         <v>2520</v>
       </c>
-      <c r="J38" s="19" t="s">
+      <c r="J38" s="18" t="s">
         <v>3092</v>
       </c>
-      <c r="K38" s="26" t="s">
+      <c r="K38" s="25" t="s">
         <v>2520</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="I39" s="16" t="s">
+      <c r="I39" s="15" t="s">
         <v>2521</v>
       </c>
-      <c r="J39" s="19" t="s">
+      <c r="J39" s="18" t="s">
         <v>3093</v>
       </c>
-      <c r="K39" s="26" t="s">
+      <c r="K39" s="25" t="s">
         <v>2521</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B40" s="19"/>
-      <c r="I40" s="16" t="s">
+      <c r="B40" s="18"/>
+      <c r="I40" s="15" t="s">
         <v>2523</v>
       </c>
-      <c r="J40" s="19" t="s">
+      <c r="J40" s="18" t="s">
         <v>3095</v>
       </c>
-      <c r="K40" s="26" t="s">
+      <c r="K40" s="25" t="s">
         <v>2523</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B41" s="19"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="19"/>
-      <c r="I41" s="16" t="s">
+      <c r="B41" s="18"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="18"/>
+      <c r="I41" s="15" t="s">
         <v>2524</v>
       </c>
-      <c r="J41" s="19" t="s">
+      <c r="J41" s="18" t="s">
         <v>3096</v>
       </c>
-      <c r="K41" s="26" t="s">
+      <c r="K41" s="25" t="s">
         <v>2524</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B42" s="19"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="19"/>
-      <c r="I42" s="16" t="s">
+      <c r="B42" s="18"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="18"/>
+      <c r="I42" s="15" t="s">
         <v>1609</v>
       </c>
-      <c r="J42" s="19" t="s">
+      <c r="J42" s="18" t="s">
         <v>3125</v>
       </c>
-      <c r="K42" s="26" t="s">
+      <c r="K42" s="25" t="s">
         <v>1609</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="E43" s="17"/>
-      <c r="I43" s="16" t="s">
+      <c r="E43" s="16"/>
+      <c r="I43" s="15" t="s">
         <v>1610</v>
       </c>
-      <c r="J43" s="19" t="s">
+      <c r="J43" s="18" t="s">
         <v>3126</v>
       </c>
-      <c r="K43" s="26" t="s">
+      <c r="K43" s="25" t="s">
         <v>1610</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="I44" s="16" t="s">
+      <c r="I44" s="15" t="s">
         <v>1612</v>
       </c>
-      <c r="J44" s="19" t="s">
+      <c r="J44" s="18" t="s">
         <v>3128</v>
       </c>
-      <c r="K44" s="26" t="s">
+      <c r="K44" s="25" t="s">
         <v>1612</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="I45" s="16" t="s">
+      <c r="I45" s="15" t="s">
         <v>1613</v>
       </c>
-      <c r="J45" s="19" t="s">
+      <c r="J45" s="18" t="s">
         <v>3129</v>
       </c>
-      <c r="K45" s="26" t="s">
+      <c r="K45" s="25" t="s">
         <v>1613</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="I46" s="16" t="s">
+      <c r="I46" s="15" t="s">
         <v>1614</v>
       </c>
-      <c r="J46" s="19" t="s">
+      <c r="J46" s="18" t="s">
         <v>3130</v>
       </c>
-      <c r="K46" s="26" t="s">
+      <c r="K46" s="25" t="s">
         <v>1614</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="I47" s="16" t="s">
+      <c r="I47" s="15" t="s">
         <v>1615</v>
       </c>
-      <c r="J47" s="19" t="s">
+      <c r="J47" s="18" t="s">
         <v>3131</v>
       </c>
-      <c r="K47" s="26" t="s">
+      <c r="K47" s="25" t="s">
         <v>1615</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="I48" s="16" t="s">
+      <c r="I48" s="15" t="s">
         <v>2570</v>
       </c>
-      <c r="J48" s="19" t="s">
+      <c r="J48" s="18" t="s">
         <v>3158</v>
       </c>
-      <c r="K48" s="26" t="s">
+      <c r="K48" s="25" t="s">
         <v>2570</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A49" s="22"/>
-      <c r="B49" s="23"/>
-      <c r="D49" s="19"/>
-      <c r="G49" s="16" t="s">
+      <c r="A49" s="21"/>
+      <c r="B49" s="22"/>
+      <c r="D49" s="18"/>
+      <c r="G49" s="15" t="s">
         <v>1620</v>
       </c>
-      <c r="H49" s="19" t="s">
+      <c r="H49" s="18" t="s">
         <v>2103</v>
       </c>
-      <c r="I49" s="16" t="s">
+      <c r="I49" s="15" t="s">
         <v>1620</v>
       </c>
-      <c r="J49" s="19" t="s">
+      <c r="J49" s="18" t="s">
         <v>3157</v>
       </c>
-      <c r="K49" s="26" t="s">
+      <c r="K49" s="25" t="s">
         <v>4054</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D50" s="19"/>
-      <c r="G50" s="16" t="s">
+      <c r="D50" s="18"/>
+      <c r="G50" s="15" t="s">
         <v>1592</v>
       </c>
-      <c r="H50" s="19" t="s">
+      <c r="H50" s="18" t="s">
         <v>2070</v>
       </c>
-      <c r="K50" s="26" t="s">
+      <c r="K50" s="25" t="s">
         <v>4055</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D51" s="19"/>
-      <c r="G51" s="16" t="s">
+      <c r="D51" s="18"/>
+      <c r="G51" s="15" t="s">
         <v>1593</v>
       </c>
-      <c r="H51" s="19" t="s">
+      <c r="H51" s="18" t="s">
         <v>2071</v>
       </c>
-      <c r="K51" s="26" t="s">
+      <c r="K51" s="25" t="s">
         <v>1593</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D52" s="19"/>
-      <c r="G52" s="16" t="s">
+      <c r="D52" s="18"/>
+      <c r="G52" s="15" t="s">
         <v>1594</v>
       </c>
-      <c r="H52" s="19" t="s">
+      <c r="H52" s="18" t="s">
         <v>2072</v>
       </c>
-      <c r="K52" s="26" t="s">
+      <c r="K52" s="25" t="s">
         <v>1594</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A53" s="22"/>
-      <c r="B53" s="20"/>
-      <c r="D53" s="19"/>
-      <c r="G53" s="16" t="s">
+      <c r="A53" s="21"/>
+      <c r="B53" s="19"/>
+      <c r="D53" s="18"/>
+      <c r="G53" s="15" t="s">
         <v>1617</v>
       </c>
-      <c r="H53" s="19" t="s">
+      <c r="H53" s="18" t="s">
         <v>2100</v>
       </c>
-      <c r="K53" s="26" t="s">
+      <c r="K53" s="25" t="s">
         <v>4053</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B54" s="19"/>
-      <c r="D54" s="19"/>
-      <c r="G54" s="16" t="s">
+      <c r="B54" s="18"/>
+      <c r="D54" s="18"/>
+      <c r="G54" s="15" t="s">
         <v>1618</v>
       </c>
-      <c r="H54" s="19" t="s">
+      <c r="H54" s="18" t="s">
         <v>2101</v>
       </c>
-      <c r="I54" s="17"/>
-      <c r="J54" s="19"/>
-      <c r="K54" s="26" t="s">
+      <c r="I54" s="16"/>
+      <c r="J54" s="18"/>
+      <c r="K54" s="25" t="s">
         <v>1618</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B55" s="19"/>
-      <c r="D55" s="19"/>
-      <c r="F55" s="19"/>
-      <c r="G55" s="16" t="s">
+      <c r="B55" s="18"/>
+      <c r="D55" s="18"/>
+      <c r="F55" s="18"/>
+      <c r="G55" s="15" t="s">
         <v>1680</v>
       </c>
-      <c r="H55" s="19" t="s">
+      <c r="H55" s="18" t="s">
         <v>2163</v>
       </c>
-      <c r="K55" s="26" t="s">
+      <c r="K55" s="25" t="s">
         <v>1680</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A56" s="17"/>
-      <c r="B56" s="21"/>
-      <c r="C56" s="17"/>
-      <c r="D56" s="21"/>
-      <c r="G56" s="16" t="s">
+      <c r="A56" s="16"/>
+      <c r="B56" s="20"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="20"/>
+      <c r="G56" s="15" t="s">
         <v>1619</v>
       </c>
-      <c r="H56" s="19" t="s">
+      <c r="H56" s="18" t="s">
         <v>2102</v>
       </c>
-      <c r="K56" s="26" t="s">
+      <c r="K56" s="25" t="s">
         <v>1619</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A57" s="17"/>
-      <c r="B57" s="21"/>
-      <c r="C57" s="17"/>
-      <c r="D57" s="21"/>
-      <c r="G57" s="27" t="s">
+      <c r="A57" s="16"/>
+      <c r="B57" s="20"/>
+      <c r="C57" s="16"/>
+      <c r="D57" s="20"/>
+      <c r="G57" s="26" t="s">
         <v>1671</v>
       </c>
-      <c r="H57" s="28" t="s">
+      <c r="H57" s="27" t="s">
         <v>2154</v>
       </c>
-      <c r="I57" s="27"/>
-      <c r="J57" s="27"/>
-      <c r="K57" s="27" t="s">
+      <c r="I57" s="26"/>
+      <c r="J57" s="26"/>
+      <c r="K57" s="26" t="s">
         <v>1671</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A58" s="17"/>
-      <c r="B58" s="21"/>
-      <c r="C58" s="17"/>
-      <c r="D58" s="21"/>
-      <c r="G58" s="27" t="s">
+      <c r="A58" s="16"/>
+      <c r="B58" s="20"/>
+      <c r="C58" s="16"/>
+      <c r="D58" s="20"/>
+      <c r="G58" s="26" t="s">
         <v>1672</v>
       </c>
-      <c r="H58" s="28" t="s">
+      <c r="H58" s="27" t="s">
         <v>2155</v>
       </c>
-      <c r="I58" s="27"/>
-      <c r="J58" s="27"/>
-      <c r="K58" s="27" t="s">
+      <c r="I58" s="26"/>
+      <c r="J58" s="26"/>
+      <c r="K58" s="26" t="s">
         <v>1672</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A59" s="22"/>
-      <c r="B59" s="23"/>
-      <c r="C59" s="17"/>
-      <c r="D59" s="21"/>
-      <c r="G59" s="27" t="s">
+      <c r="A59" s="21"/>
+      <c r="B59" s="22"/>
+      <c r="C59" s="16"/>
+      <c r="D59" s="20"/>
+      <c r="G59" s="26" t="s">
         <v>1673</v>
       </c>
-      <c r="H59" s="28" t="s">
+      <c r="H59" s="27" t="s">
         <v>2156</v>
       </c>
-      <c r="I59" s="27"/>
-      <c r="J59" s="27"/>
-      <c r="K59" s="27" t="s">
+      <c r="I59" s="26"/>
+      <c r="J59" s="26"/>
+      <c r="K59" s="26" t="s">
         <v>1673</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A60" s="17"/>
-      <c r="B60" s="17"/>
-      <c r="C60" s="17"/>
-      <c r="D60" s="17"/>
-      <c r="E60" s="17"/>
-      <c r="F60" s="17"/>
-      <c r="G60" s="27" t="s">
+      <c r="A60" s="16"/>
+      <c r="B60" s="16"/>
+      <c r="C60" s="16"/>
+      <c r="D60" s="16"/>
+      <c r="E60" s="16"/>
+      <c r="F60" s="16"/>
+      <c r="G60" s="26" t="s">
         <v>1675</v>
       </c>
-      <c r="H60" s="28" t="s">
+      <c r="H60" s="27" t="s">
         <v>2158</v>
       </c>
-      <c r="I60" s="27"/>
-      <c r="J60" s="27"/>
-      <c r="K60" s="27" t="s">
+      <c r="I60" s="26"/>
+      <c r="J60" s="26"/>
+      <c r="K60" s="26" t="s">
         <v>1675</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="G61" s="27" t="s">
+      <c r="G61" s="26" t="s">
         <v>1676</v>
       </c>
-      <c r="H61" s="28" t="s">
+      <c r="H61" s="27" t="s">
         <v>2159</v>
       </c>
-      <c r="I61" s="27"/>
-      <c r="J61" s="27"/>
-      <c r="K61" s="27" t="s">
+      <c r="I61" s="26"/>
+      <c r="J61" s="26"/>
+      <c r="K61" s="26" t="s">
         <v>1676</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="G62" s="27" t="s">
+      <c r="G62" s="26" t="s">
         <v>1677</v>
       </c>
-      <c r="H62" s="28" t="s">
+      <c r="H62" s="27" t="s">
         <v>2160</v>
       </c>
-      <c r="I62" s="27"/>
-      <c r="J62" s="27"/>
-      <c r="K62" s="27" t="s">
+      <c r="I62" s="26"/>
+      <c r="J62" s="26"/>
+      <c r="K62" s="26" t="s">
         <v>1677</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A63" s="17"/>
-      <c r="B63" s="17"/>
-      <c r="C63" s="17"/>
-      <c r="D63" s="17"/>
-      <c r="E63" s="17"/>
-      <c r="F63" s="17"/>
-      <c r="G63" s="27" t="s">
+      <c r="A63" s="16"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="16"/>
+      <c r="D63" s="16"/>
+      <c r="E63" s="16"/>
+      <c r="F63" s="16"/>
+      <c r="G63" s="26" t="s">
         <v>1678</v>
       </c>
-      <c r="H63" s="28" t="s">
+      <c r="H63" s="27" t="s">
         <v>2161</v>
       </c>
-      <c r="I63" s="27"/>
-      <c r="J63" s="27"/>
-      <c r="K63" s="27" t="s">
+      <c r="I63" s="26"/>
+      <c r="J63" s="26"/>
+      <c r="K63" s="26" t="s">
         <v>1678</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A64" s="17"/>
-      <c r="B64" s="17"/>
-      <c r="C64" s="17"/>
-      <c r="D64" s="17"/>
-      <c r="E64" s="17"/>
-      <c r="F64" s="17"/>
-      <c r="G64" s="27" t="s">
+      <c r="A64" s="16"/>
+      <c r="B64" s="16"/>
+      <c r="C64" s="16"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="16"/>
+      <c r="G64" s="26" t="s">
         <v>1679</v>
       </c>
-      <c r="H64" s="28" t="s">
+      <c r="H64" s="27" t="s">
         <v>2162</v>
       </c>
-      <c r="I64" s="27"/>
-      <c r="J64" s="27"/>
-      <c r="K64" s="27" t="s">
+      <c r="I64" s="26"/>
+      <c r="J64" s="26"/>
+      <c r="K64" s="26" t="s">
         <v>1679</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E65" s="17"/>
-      <c r="F65" s="17"/>
-      <c r="G65" s="27" t="s">
+      <c r="E65" s="16"/>
+      <c r="F65" s="16"/>
+      <c r="G65" s="26" t="s">
         <v>1690</v>
       </c>
-      <c r="H65" s="28" t="s">
+      <c r="H65" s="27" t="s">
         <v>2173</v>
       </c>
-      <c r="I65" s="27"/>
-      <c r="J65" s="27"/>
-      <c r="K65" s="27" t="s">
+      <c r="I65" s="26"/>
+      <c r="J65" s="26"/>
+      <c r="K65" s="26" t="s">
         <v>1690</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A66" s="17"/>
-      <c r="B66" s="17"/>
-      <c r="E66" s="26" t="s">
+      <c r="A66" s="16"/>
+      <c r="B66" s="16"/>
+      <c r="E66" s="25" t="s">
         <v>603</v>
       </c>
-      <c r="F66" s="19" t="s">
+      <c r="F66" s="18" t="s">
         <v>1117</v>
       </c>
-      <c r="G66" s="17"/>
-      <c r="H66" s="17"/>
-      <c r="K66" s="26" t="s">
+      <c r="G66" s="16"/>
+      <c r="H66" s="16"/>
+      <c r="K66" s="25" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A67" s="17"/>
-      <c r="B67" s="17"/>
-      <c r="E67" s="26" t="s">
+      <c r="A67" s="16"/>
+      <c r="B67" s="16"/>
+      <c r="E67" s="25" t="s">
         <v>602</v>
       </c>
-      <c r="F67" s="19" t="s">
+      <c r="F67" s="18" t="s">
         <v>1116</v>
       </c>
-      <c r="G67" s="17"/>
-      <c r="H67" s="17"/>
-      <c r="J67" s="17"/>
-      <c r="K67" s="26" t="s">
+      <c r="G67" s="16"/>
+      <c r="H67" s="16"/>
+      <c r="J67" s="16"/>
+      <c r="K67" s="25" t="s">
         <v>4051</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A68" s="17"/>
-      <c r="B68" s="17"/>
-      <c r="C68" s="17"/>
-      <c r="D68" s="17"/>
-      <c r="E68" s="26" t="s">
+      <c r="A68" s="16"/>
+      <c r="B68" s="16"/>
+      <c r="C68" s="16"/>
+      <c r="D68" s="16"/>
+      <c r="E68" s="25" t="s">
         <v>587</v>
       </c>
-      <c r="F68" s="19" t="s">
+      <c r="F68" s="18" t="s">
         <v>1101</v>
       </c>
-      <c r="G68" s="17"/>
-      <c r="H68" s="17"/>
-      <c r="J68" s="17"/>
-      <c r="K68" s="26" t="s">
+      <c r="G68" s="16"/>
+      <c r="H68" s="16"/>
+      <c r="J68" s="16"/>
+      <c r="K68" s="25" t="s">
         <v>4059</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A69" s="17"/>
-      <c r="B69" s="17"/>
-      <c r="C69" s="17"/>
-      <c r="D69" s="17"/>
-      <c r="E69" s="26" t="s">
+      <c r="A69" s="16"/>
+      <c r="B69" s="16"/>
+      <c r="C69" s="16"/>
+      <c r="D69" s="16"/>
+      <c r="E69" s="25" t="s">
         <v>588</v>
       </c>
-      <c r="F69" s="19" t="s">
+      <c r="F69" s="18" t="s">
         <v>1102</v>
       </c>
-      <c r="G69" s="17"/>
-      <c r="H69" s="17"/>
-      <c r="J69" s="17"/>
-      <c r="K69" s="26" t="s">
+      <c r="G69" s="16"/>
+      <c r="H69" s="16"/>
+      <c r="J69" s="16"/>
+      <c r="K69" s="25" t="s">
         <v>4060</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A70" s="17"/>
-      <c r="B70" s="17"/>
-      <c r="C70" s="17"/>
-      <c r="D70" s="17"/>
-      <c r="E70" s="26" t="s">
+      <c r="A70" s="16"/>
+      <c r="B70" s="16"/>
+      <c r="C70" s="16"/>
+      <c r="D70" s="16"/>
+      <c r="E70" s="25" t="s">
         <v>591</v>
       </c>
-      <c r="F70" s="19" t="s">
+      <c r="F70" s="18" t="s">
         <v>1105</v>
       </c>
-      <c r="J70" s="17"/>
-      <c r="K70" s="26" t="s">
+      <c r="J70" s="16"/>
+      <c r="K70" s="25" t="s">
         <v>4049</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A71" s="17"/>
-      <c r="B71" s="17"/>
-      <c r="C71" s="17"/>
-      <c r="D71" s="17"/>
-      <c r="E71" s="26" t="s">
+      <c r="A71" s="16"/>
+      <c r="B71" s="16"/>
+      <c r="C71" s="16"/>
+      <c r="D71" s="16"/>
+      <c r="E71" s="25" t="s">
         <v>592</v>
       </c>
-      <c r="F71" s="19" t="s">
+      <c r="F71" s="18" t="s">
         <v>1106</v>
       </c>
-      <c r="I71" s="17"/>
-      <c r="J71" s="17"/>
-      <c r="K71" s="26" t="s">
+      <c r="I71" s="16"/>
+      <c r="J71" s="16"/>
+      <c r="K71" s="25" t="s">
         <v>4050</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A72" s="17"/>
-      <c r="B72" s="17"/>
-      <c r="C72" s="17"/>
-      <c r="D72" s="17"/>
-      <c r="E72" s="26" t="s">
+      <c r="A72" s="16"/>
+      <c r="B72" s="16"/>
+      <c r="C72" s="16"/>
+      <c r="D72" s="16"/>
+      <c r="E72" s="25" t="s">
         <v>593</v>
       </c>
-      <c r="F72" s="19" t="s">
+      <c r="F72" s="18" t="s">
         <v>1107</v>
       </c>
-      <c r="J72" s="17"/>
-      <c r="K72" s="26" t="s">
+      <c r="J72" s="16"/>
+      <c r="K72" s="25" t="s">
         <v>4048</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A73" s="17"/>
-      <c r="B73" s="17"/>
-      <c r="C73" s="17"/>
-      <c r="D73" s="17"/>
-      <c r="E73" s="26" t="s">
+      <c r="A73" s="16"/>
+      <c r="B73" s="16"/>
+      <c r="C73" s="16"/>
+      <c r="D73" s="16"/>
+      <c r="E73" s="25" t="s">
         <v>564</v>
       </c>
-      <c r="F73" s="19" t="s">
+      <c r="F73" s="18" t="s">
         <v>1078</v>
       </c>
-      <c r="J73" s="17"/>
-      <c r="K73" s="26" t="s">
+      <c r="J73" s="16"/>
+      <c r="K73" s="25" t="s">
         <v>4047</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A74" s="17"/>
-      <c r="B74" s="17"/>
-      <c r="C74" s="17"/>
-      <c r="D74" s="21"/>
-      <c r="E74" s="26" t="s">
+      <c r="A74" s="16"/>
+      <c r="B74" s="16"/>
+      <c r="C74" s="16"/>
+      <c r="D74" s="20"/>
+      <c r="E74" s="25" t="s">
         <v>600</v>
       </c>
-      <c r="F74" s="19" t="s">
+      <c r="F74" s="18" t="s">
         <v>1114</v>
       </c>
-      <c r="J74" s="17"/>
-      <c r="K74" s="26" t="s">
+      <c r="J74" s="16"/>
+      <c r="K74" s="25" t="s">
         <v>4052</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A75" s="17"/>
-      <c r="B75" s="17"/>
-      <c r="C75" s="17"/>
-      <c r="D75" s="21"/>
-      <c r="E75" s="26" t="s">
+      <c r="A75" s="16"/>
+      <c r="B75" s="16"/>
+      <c r="C75" s="16"/>
+      <c r="D75" s="20"/>
+      <c r="E75" s="25" t="s">
         <v>594</v>
       </c>
-      <c r="F75" s="19" t="s">
+      <c r="F75" s="18" t="s">
         <v>1108</v>
       </c>
-      <c r="J75" s="17"/>
-      <c r="K75" s="26" t="s">
+      <c r="J75" s="16"/>
+      <c r="K75" s="25" t="s">
         <v>4046</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A76" s="17"/>
-      <c r="B76" s="17"/>
-      <c r="C76" s="26" t="s">
+      <c r="A76" s="16"/>
+      <c r="B76" s="16"/>
+      <c r="C76" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="D76" s="19" t="s">
+      <c r="D76" s="18" t="s">
         <v>334</v>
       </c>
-      <c r="J76" s="17"/>
-      <c r="K76" s="26" t="s">
+      <c r="J76" s="16"/>
+      <c r="K76" s="25" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C77" s="26" t="s">
+      <c r="C77" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="D77" s="19" t="s">
+      <c r="D77" s="18" t="s">
         <v>332</v>
       </c>
-      <c r="J77" s="17"/>
-      <c r="K77" s="26" t="s">
+      <c r="J77" s="16"/>
+      <c r="K77" s="25" t="s">
         <v>4206</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A78" s="24" t="s">
+      <c r="A78" s="23" t="s">
         <v>3772</v>
       </c>
-      <c r="B78" s="20" t="s">
+      <c r="B78" s="19" t="s">
         <v>3881</v>
       </c>
-      <c r="K78" s="26" t="s">
+      <c r="K78" s="25" t="s">
         <v>4043</v>
       </c>
     </row>
@@ -39853,480 +39856,480 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB360FDB-9222-4846-8C29-B1EE5CE081EB}">
   <dimension ref="A1:J104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.33203125" style="29" customWidth="1"/>
-    <col min="2" max="2" width="54.5" style="29" customWidth="1"/>
-    <col min="3" max="4" width="10.83203125" style="29"/>
-    <col min="5" max="5" width="23.1640625" style="29" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="29"/>
+    <col min="1" max="1" width="37.33203125" style="28" customWidth="1"/>
+    <col min="2" max="2" width="54.5" style="28" customWidth="1"/>
+    <col min="3" max="4" width="10.83203125" style="28"/>
+    <col min="5" max="5" width="23.1640625" style="28" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="28" t="s">
         <v>4061</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="28" t="s">
         <v>4064</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="28" t="s">
         <v>4130</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="28" t="s">
         <v>4096</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="28" t="s">
         <v>4171</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="30" t="s">
         <v>4075</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="28" t="s">
         <v>4076</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="28" t="s">
         <v>4071</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="28" t="s">
         <v>4022</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="28" t="s">
         <v>4165</v>
       </c>
-      <c r="F2" s="17"/>
+      <c r="F2" s="16"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="28" t="s">
         <v>4077</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="28" t="s">
         <v>4166</v>
       </c>
-      <c r="F3" s="17"/>
+      <c r="F3" s="16"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="30" t="s">
         <v>4029</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="28" t="s">
         <v>4124</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="28" t="s">
         <v>4071</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="28" t="s">
         <v>4124</v>
       </c>
-      <c r="F4" s="17"/>
+      <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="30" t="s">
         <v>4122</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="28" t="s">
         <v>4123</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="28" t="s">
         <v>4071</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="28" t="s">
         <v>4167</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="16"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="30" t="s">
         <v>4120</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="28" t="s">
         <v>4121</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="28" t="s">
         <v>4168</v>
       </c>
-      <c r="F6" s="17"/>
+      <c r="F6" s="16"/>
     </row>
     <row r="7" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="31" t="s">
-        <v>4036</v>
-      </c>
-      <c r="B7" s="30" t="s">
+      <c r="A7" s="30" t="s">
+        <v>4208</v>
+      </c>
+      <c r="B7" s="29" t="s">
         <v>4095</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="28" t="s">
         <v>4062</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="28" t="s">
         <v>4022</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="18" t="s">
         <v>2396</v>
       </c>
-      <c r="F7" s="17"/>
+      <c r="F7" s="16"/>
     </row>
     <row r="8" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="28" t="s">
         <v>1191</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E8" s="29" t="s">
+      <c r="E8" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="F8" s="17"/>
+      <c r="F8" s="16"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="30" t="s">
         <v>4065</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="28" t="s">
         <v>4066</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="28" t="s">
         <v>4067</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="28" t="s">
         <v>4068</v>
       </c>
-      <c r="E9" s="29" t="s">
+      <c r="E9" s="28" t="s">
         <v>4066</v>
       </c>
-      <c r="F9" s="17"/>
+      <c r="F9" s="16"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="30" t="s">
         <v>113</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>4070</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="28" t="s">
         <v>4071</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="D10" s="28" t="s">
         <v>4068</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="18" t="s">
         <v>3401</v>
       </c>
-      <c r="F10" s="17"/>
+      <c r="F10" s="16"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="30" t="s">
         <v>188</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="28" t="s">
         <v>4072</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="28" t="s">
         <v>4071</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="28" t="s">
         <v>4022</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="18" t="s">
         <v>3590</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="16" t="s">
         <v>4097</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="30" t="s">
         <v>189</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="28" t="s">
         <v>4073</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="28" t="s">
         <v>4074</v>
       </c>
-      <c r="D12" s="29" t="s">
+      <c r="D12" s="28" t="s">
         <v>4022</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="18" t="s">
         <v>3591</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="16" t="s">
         <v>4097</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="165" x14ac:dyDescent="0.2">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="30" t="s">
         <v>4111</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>4112</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="28" t="s">
         <v>4067</v>
       </c>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="28" t="s">
         <v>4022</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>405</v>
       </c>
-      <c r="F13" s="17"/>
+      <c r="F13" s="16"/>
     </row>
     <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.2">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="30" t="s">
         <v>4113</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="28" t="s">
         <v>4114</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D14" s="29" t="s">
+      <c r="D14" s="28" t="s">
         <v>4069</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>425</v>
       </c>
-      <c r="F14" s="17"/>
+      <c r="F14" s="16"/>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="30" t="s">
         <v>4115</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="28" t="s">
         <v>4116</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="28" t="s">
         <v>4069</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>340</v>
       </c>
-      <c r="F15" s="17"/>
+      <c r="F15" s="16"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="28" t="s">
         <v>4125</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="28" t="s">
         <v>4071</v>
       </c>
-      <c r="D16" s="29" t="s">
+      <c r="D16" s="28" t="s">
         <v>4022</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="18" t="s">
         <v>1258</v>
       </c>
-      <c r="F16" s="17"/>
+      <c r="F16" s="16"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="18" t="s">
         <v>4193</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="E17" s="18" t="s">
         <v>1258</v>
       </c>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17" t="s">
+      <c r="F17" s="16"/>
+      <c r="G17" s="16" t="s">
         <v>4099</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="75" x14ac:dyDescent="0.2">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="30" t="s">
         <v>4117</v>
       </c>
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="28" t="s">
         <v>4118</v>
       </c>
-      <c r="C18" s="29" t="s">
+      <c r="C18" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D18" s="29" t="s">
+      <c r="D18" s="28" t="s">
         <v>4119</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>362</v>
       </c>
-      <c r="F18" s="17"/>
+      <c r="F18" s="16"/>
     </row>
     <row r="19" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="30" t="s">
         <v>4086</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="28" t="s">
         <v>4083</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="28" t="s">
         <v>4071</v>
       </c>
-      <c r="D19" s="29" t="s">
+      <c r="D19" s="28" t="s">
         <v>4022</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="E19" s="18" t="s">
         <v>4169</v>
       </c>
-      <c r="F19" s="17"/>
+      <c r="F19" s="16"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="30" t="s">
         <v>4085</v>
       </c>
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="28" t="s">
         <v>4084</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="28" t="s">
         <v>4071</v>
       </c>
-      <c r="D20" s="29" t="s">
+      <c r="D20" s="28" t="s">
         <v>4022</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="E20" s="18" t="s">
         <v>4169</v>
       </c>
-      <c r="F20" s="17"/>
+      <c r="F20" s="16"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="30" t="s">
         <v>4089</v>
       </c>
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="28" t="s">
         <v>4090</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="C21" s="28" t="s">
         <v>4071</v>
       </c>
-      <c r="D21" s="29" t="s">
+      <c r="D21" s="28" t="s">
         <v>4022</v>
       </c>
-      <c r="E21" s="19" t="s">
+      <c r="E21" s="18" t="s">
         <v>4169</v>
       </c>
-      <c r="F21" s="17"/>
+      <c r="F21" s="16"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="31" t="s">
+      <c r="A22" s="30" t="s">
         <v>4091</v>
       </c>
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="28" t="s">
         <v>4092</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="C22" s="28" t="s">
         <v>4071</v>
       </c>
-      <c r="D22" s="29" t="s">
+      <c r="D22" s="28" t="s">
         <v>4022</v>
       </c>
-      <c r="E22" s="19" t="s">
+      <c r="E22" s="18" t="s">
         <v>4169</v>
       </c>
-      <c r="F22" s="17"/>
+      <c r="F22" s="16"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="30" t="s">
         <v>4087</v>
       </c>
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="28" t="s">
         <v>4088</v>
       </c>
-      <c r="C23" s="29" t="s">
+      <c r="C23" s="28" t="s">
         <v>4071</v>
       </c>
-      <c r="D23" s="29" t="s">
+      <c r="D23" s="28" t="s">
         <v>4022</v>
       </c>
-      <c r="E23" s="19" t="s">
+      <c r="E23" s="18" t="s">
         <v>4169</v>
       </c>
-      <c r="F23" s="17"/>
+      <c r="F23" s="16"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="16" t="s">
         <v>4131</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="C24" s="29" t="s">
+      <c r="C24" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D24" s="29" t="s">
+      <c r="D24" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E24" s="34" t="s">
+      <c r="E24" s="33" t="s">
         <v>3084</v>
       </c>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17" t="s">
+      <c r="F24" s="16"/>
+      <c r="G24" s="16" t="s">
         <v>4099</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="30" t="s">
         <v>14</v>
       </c>
       <c r="B25" t="s">
         <v>4082</v>
       </c>
-      <c r="C25" s="29" t="s">
+      <c r="C25" s="28" t="s">
         <v>4071</v>
       </c>
-      <c r="D25" s="29" t="s">
+      <c r="D25" s="28" t="s">
         <v>4068</v>
       </c>
-      <c r="E25" s="19" t="s">
+      <c r="E25" s="18" t="s">
         <v>3000</v>
       </c>
     </row>
@@ -40334,42 +40337,42 @@
       <c r="A26" t="s">
         <v>4132</v>
       </c>
-      <c r="B26" s="33" t="s">
+      <c r="B26" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="29" t="s">
+      <c r="C26" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D26" s="29" t="s">
+      <c r="D26" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E26" s="19" t="s">
+      <c r="E26" s="18" t="s">
         <v>3000</v>
       </c>
-      <c r="G26" s="17" t="s">
+      <c r="G26" s="16" t="s">
         <v>4099</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="30" t="s">
         <v>4100</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>4093</v>
       </c>
-      <c r="C27" s="29" t="s">
+      <c r="C27" s="28" t="s">
         <v>4067</v>
       </c>
-      <c r="D27" s="29" t="s">
+      <c r="D27" s="28" t="s">
         <v>4022</v>
       </c>
-      <c r="E27" s="19" t="s">
+      <c r="E27" s="18" t="s">
         <v>4170</v>
       </c>
-      <c r="F27" s="17"/>
+      <c r="F27" s="16"/>
     </row>
     <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="30" t="s">
         <v>4101</v>
       </c>
       <c r="B28" s="5" t="s">
@@ -40378,215 +40381,215 @@
       <c r="C28" s="9" t="s">
         <v>4067</v>
       </c>
-      <c r="D28" s="29" t="s">
+      <c r="D28" s="28" t="s">
         <v>4022</v>
       </c>
-      <c r="E28" s="19" t="s">
+      <c r="E28" s="18" t="s">
         <v>4170</v>
       </c>
-      <c r="F28" s="17"/>
+      <c r="F28" s="16"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="17" t="s">
+      <c r="A29" s="16" t="s">
         <v>4133</v>
       </c>
-      <c r="B29" s="31" t="s">
+      <c r="B29" s="30" t="s">
         <v>4098</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>4063</v>
       </c>
-      <c r="D29" s="29" t="s">
+      <c r="D29" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E29" s="19" t="s">
+      <c r="E29" s="18" t="s">
         <v>1113</v>
       </c>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17" t="s">
+      <c r="F29" s="16"/>
+      <c r="G29" s="16" t="s">
         <v>4099</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="25" t="s">
         <v>4078</v>
       </c>
-      <c r="B30" s="29" t="s">
+      <c r="B30" s="28" t="s">
         <v>4079</v>
       </c>
-      <c r="C30" s="29" t="s">
+      <c r="C30" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D30" s="29" t="s">
+      <c r="D30" s="28" t="s">
         <v>4022</v>
       </c>
-      <c r="F30" s="17"/>
+      <c r="F30" s="16"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="26" t="s">
+      <c r="A31" s="25" t="s">
         <v>4080</v>
       </c>
-      <c r="B31" s="29" t="s">
+      <c r="B31" s="28" t="s">
         <v>4081</v>
       </c>
-      <c r="C31" s="29" t="s">
+      <c r="C31" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D31" s="29" t="s">
+      <c r="D31" s="28" t="s">
         <v>4022</v>
       </c>
-      <c r="F31" s="17"/>
+      <c r="F31" s="16"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="30" t="s">
         <v>4030</v>
       </c>
       <c r="B32" t="s">
         <v>4102</v>
       </c>
-      <c r="C32" s="29" t="s">
+      <c r="C32" s="28" t="s">
         <v>4071</v>
       </c>
-      <c r="D32" s="29" t="s">
+      <c r="D32" s="28" t="s">
         <v>4022</v>
       </c>
-      <c r="F32" s="17"/>
+      <c r="F32" s="16"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="30" t="s">
         <v>4031</v>
       </c>
       <c r="B33" t="s">
         <v>4103</v>
       </c>
-      <c r="C33" s="29" t="s">
+      <c r="C33" s="28" t="s">
         <v>4071</v>
       </c>
-      <c r="D33" s="29" t="s">
+      <c r="D33" s="28" t="s">
         <v>4022</v>
       </c>
-      <c r="F33" s="17"/>
+      <c r="F33" s="16"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="31" t="s">
+      <c r="A34" s="30" t="s">
         <v>4032</v>
       </c>
       <c r="B34" t="s">
         <v>4104</v>
       </c>
-      <c r="C34" s="29" t="s">
+      <c r="C34" s="28" t="s">
         <v>4071</v>
       </c>
-      <c r="D34" s="29" t="s">
+      <c r="D34" s="28" t="s">
         <v>4022</v>
       </c>
-      <c r="F34" s="17"/>
+      <c r="F34" s="16"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="31" t="s">
+      <c r="A35" s="30" t="s">
         <v>4033</v>
       </c>
-      <c r="B35" s="32" t="s">
+      <c r="B35" s="31" t="s">
         <v>4105</v>
       </c>
-      <c r="C35" s="29" t="s">
+      <c r="C35" s="28" t="s">
         <v>4071</v>
       </c>
-      <c r="D35" s="29" t="s">
+      <c r="D35" s="28" t="s">
         <v>4022</v>
       </c>
-      <c r="F35" s="17"/>
+      <c r="F35" s="16"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="31" t="s">
+      <c r="A36" s="30" t="s">
         <v>1464</v>
       </c>
       <c r="B36" t="s">
         <v>4107</v>
       </c>
-      <c r="C36" s="29" t="s">
+      <c r="C36" s="28" t="s">
         <v>4071</v>
       </c>
-      <c r="D36" s="29" t="s">
+      <c r="D36" s="28" t="s">
         <v>4022</v>
       </c>
-      <c r="F36" s="17"/>
+      <c r="F36" s="16"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="31" t="s">
+      <c r="A37" s="30" t="s">
         <v>1466</v>
       </c>
       <c r="B37" t="s">
         <v>4106</v>
       </c>
-      <c r="C37" s="29" t="s">
+      <c r="C37" s="28" t="s">
         <v>4071</v>
       </c>
-      <c r="D37" s="29" t="s">
+      <c r="D37" s="28" t="s">
         <v>4022</v>
       </c>
-      <c r="F37" s="17"/>
+      <c r="F37" s="16"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="31" t="s">
+      <c r="A38" s="30" t="s">
         <v>4026</v>
       </c>
       <c r="B38" t="s">
         <v>4110</v>
       </c>
-      <c r="C38" s="29" t="s">
+      <c r="C38" s="28" t="s">
         <v>4071</v>
       </c>
-      <c r="D38" s="29" t="s">
+      <c r="D38" s="28" t="s">
         <v>4022</v>
       </c>
-      <c r="F38" s="17"/>
+      <c r="F38" s="16"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="31" t="s">
+      <c r="A39" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="B39" s="29" t="s">
+      <c r="B39" s="28" t="s">
         <v>4109</v>
       </c>
-      <c r="C39" s="29" t="s">
+      <c r="C39" s="28" t="s">
         <v>4071</v>
       </c>
-      <c r="D39" s="29" t="s">
+      <c r="D39" s="28" t="s">
         <v>4022</v>
       </c>
-      <c r="F39" s="17"/>
+      <c r="F39" s="16"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="31" t="s">
+      <c r="A40" s="30" t="s">
         <v>102</v>
       </c>
       <c r="B40" t="s">
         <v>4108</v>
       </c>
-      <c r="C40" s="29" t="s">
+      <c r="C40" s="28" t="s">
         <v>4071</v>
       </c>
-      <c r="D40" s="29" t="s">
+      <c r="D40" s="28" t="s">
         <v>4022</v>
       </c>
-      <c r="F40" s="17"/>
+      <c r="F40" s="16"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="19" t="s">
+      <c r="A41" s="18" t="s">
         <v>4134</v>
       </c>
-      <c r="B41" s="31" t="s">
+      <c r="B41" s="30" t="s">
         <v>1465</v>
       </c>
-      <c r="C41" s="29" t="s">
+      <c r="C41" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D41" s="29" t="s">
+      <c r="D41" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17" t="s">
+      <c r="F41" s="16"/>
+      <c r="G41" s="16" t="s">
         <v>4099</v>
       </c>
     </row>
@@ -40594,71 +40597,71 @@
       <c r="A42" t="s">
         <v>4135</v>
       </c>
-      <c r="B42" s="31" t="s">
+      <c r="B42" s="30" t="s">
         <v>4031</v>
       </c>
-      <c r="C42" s="29" t="s">
+      <c r="C42" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D42" s="29" t="s">
+      <c r="D42" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="F42" s="17"/>
-      <c r="G42" s="17" t="s">
+      <c r="F42" s="16"/>
+      <c r="G42" s="16" t="s">
         <v>4099</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="32" t="s">
+      <c r="A43" s="31" t="s">
         <v>4136</v>
       </c>
-      <c r="B43" s="31" t="s">
+      <c r="B43" s="30" t="s">
         <v>4032</v>
       </c>
-      <c r="C43" s="29" t="s">
+      <c r="C43" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D43" s="29" t="s">
+      <c r="D43" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="F43" s="17"/>
-      <c r="G43" s="17" t="s">
+      <c r="F43" s="16"/>
+      <c r="G43" s="16" t="s">
         <v>4099</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="32" t="s">
+      <c r="A44" s="31" t="s">
         <v>4137</v>
       </c>
-      <c r="B44" s="31" t="s">
+      <c r="B44" s="30" t="s">
         <v>4033</v>
       </c>
-      <c r="C44" s="29" t="s">
+      <c r="C44" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D44" s="29" t="s">
+      <c r="D44" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="F44" s="17"/>
-      <c r="G44" s="17" t="s">
+      <c r="F44" s="16"/>
+      <c r="G44" s="16" t="s">
         <v>4099</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="29" t="s">
+      <c r="A45" s="28" t="s">
         <v>4139</v>
       </c>
-      <c r="B45" s="31" t="s">
+      <c r="B45" s="30" t="s">
         <v>1464</v>
       </c>
-      <c r="C45" s="29" t="s">
+      <c r="C45" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D45" s="29" t="s">
+      <c r="D45" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="F45" s="17"/>
-      <c r="G45" s="17" t="s">
+      <c r="F45" s="16"/>
+      <c r="G45" s="16" t="s">
         <v>4099</v>
       </c>
     </row>
@@ -40666,17 +40669,17 @@
       <c r="A46" t="s">
         <v>4138</v>
       </c>
-      <c r="B46" s="31" t="s">
+      <c r="B46" s="30" t="s">
         <v>1466</v>
       </c>
-      <c r="C46" s="29" t="s">
+      <c r="C46" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D46" s="29" t="s">
+      <c r="D46" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="F46" s="17"/>
-      <c r="G46" s="17" t="s">
+      <c r="F46" s="16"/>
+      <c r="G46" s="16" t="s">
         <v>4099</v>
       </c>
     </row>
@@ -40684,35 +40687,35 @@
       <c r="A47" t="s">
         <v>4140</v>
       </c>
-      <c r="B47" s="31" t="s">
+      <c r="B47" s="30" t="s">
         <v>4026</v>
       </c>
-      <c r="C47" s="29" t="s">
+      <c r="C47" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D47" s="29" t="s">
+      <c r="D47" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="F47" s="17"/>
-      <c r="G47" s="17" t="s">
+      <c r="F47" s="16"/>
+      <c r="G47" s="16" t="s">
         <v>4099</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="29" t="s">
+      <c r="A48" s="28" t="s">
         <v>4141</v>
       </c>
-      <c r="B48" s="31" t="s">
+      <c r="B48" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="C48" s="29" t="s">
+      <c r="C48" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D48" s="29" t="s">
+      <c r="D48" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="F48" s="17"/>
-      <c r="G48" s="17" t="s">
+      <c r="F48" s="16"/>
+      <c r="G48" s="16" t="s">
         <v>4099</v>
       </c>
     </row>
@@ -40720,1150 +40723,1150 @@
       <c r="A49" t="s">
         <v>4142</v>
       </c>
-      <c r="B49" s="31" t="s">
+      <c r="B49" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="C49" s="29" t="s">
+      <c r="C49" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D49" s="29" t="s">
+      <c r="D49" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="F49" s="17"/>
-      <c r="G49" s="17" t="s">
+      <c r="F49" s="16"/>
+      <c r="G49" s="16" t="s">
         <v>4099</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="31" t="s">
+      <c r="A50" s="30" t="s">
         <v>1590</v>
       </c>
-      <c r="B50" s="19" t="s">
+      <c r="B50" s="18" t="s">
         <v>4126</v>
       </c>
-      <c r="C50" s="29" t="s">
+      <c r="C50" s="28" t="s">
         <v>4071</v>
       </c>
-      <c r="D50" s="29" t="s">
+      <c r="D50" s="28" t="s">
         <v>4022</v>
       </c>
-      <c r="F50" s="17"/>
+      <c r="F50" s="16"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="17" t="s">
+      <c r="A51" s="16" t="s">
         <v>4143</v>
       </c>
-      <c r="B51" s="31" t="s">
+      <c r="B51" s="30" t="s">
         <v>1590</v>
       </c>
-      <c r="C51" s="29" t="s">
+      <c r="C51" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D51" s="29" t="s">
+      <c r="D51" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="F51" s="17"/>
-      <c r="G51" s="17" t="s">
+      <c r="F51" s="16"/>
+      <c r="G51" s="16" t="s">
         <v>4099</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="31" t="s">
+      <c r="A52" s="30" t="s">
         <v>1591</v>
       </c>
-      <c r="B52" s="17" t="s">
+      <c r="B52" s="16" t="s">
         <v>4127</v>
       </c>
-      <c r="C52" s="29" t="s">
+      <c r="C52" s="28" t="s">
         <v>4071</v>
       </c>
-      <c r="D52" s="29" t="s">
+      <c r="D52" s="28" t="s">
         <v>4022</v>
       </c>
-      <c r="F52" s="17"/>
+      <c r="F52" s="16"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="17" t="s">
+      <c r="A53" s="16" t="s">
         <v>4144</v>
       </c>
-      <c r="B53" s="31" t="s">
+      <c r="B53" s="30" t="s">
         <v>1591</v>
       </c>
-      <c r="C53" s="29" t="s">
+      <c r="C53" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D53" s="29" t="s">
+      <c r="D53" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="F53" s="17"/>
-      <c r="G53" s="17" t="s">
+      <c r="F53" s="16"/>
+      <c r="G53" s="16" t="s">
         <v>4099</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" s="31" t="s">
+      <c r="A54" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B54" s="29" t="s">
+      <c r="B54" s="28" t="s">
         <v>4194</v>
       </c>
-      <c r="C54" s="29" t="s">
+      <c r="C54" s="28" t="s">
         <v>4071</v>
       </c>
-      <c r="D54" s="29" t="s">
+      <c r="D54" s="28" t="s">
         <v>4022</v>
       </c>
-      <c r="E54" s="19" t="s">
+      <c r="E54" s="18" t="s">
         <v>3001</v>
       </c>
-      <c r="F54" s="17"/>
+      <c r="F54" s="16"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" s="31" t="s">
+      <c r="A55" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="B55" s="29" t="s">
+      <c r="B55" s="28" t="s">
         <v>4195</v>
       </c>
-      <c r="C55" s="29" t="s">
+      <c r="C55" s="28" t="s">
         <v>4071</v>
       </c>
-      <c r="D55" s="29" t="s">
+      <c r="D55" s="28" t="s">
         <v>4022</v>
       </c>
-      <c r="E55" s="19" t="s">
+      <c r="E55" s="18" t="s">
         <v>3078</v>
       </c>
-      <c r="F55" s="17"/>
+      <c r="F55" s="16"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="17" t="s">
+      <c r="A56" s="16" t="s">
         <v>4197</v>
       </c>
-      <c r="B56" s="31" t="s">
+      <c r="B56" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C56" s="29" t="s">
+      <c r="C56" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D56" s="29" t="s">
+      <c r="D56" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E56" s="19" t="s">
+      <c r="E56" s="18" t="s">
         <v>3001</v>
       </c>
-      <c r="F56" s="17"/>
-      <c r="G56" s="17" t="s">
+      <c r="F56" s="16"/>
+      <c r="G56" s="16" t="s">
         <v>4099</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="17" t="s">
+      <c r="A57" s="16" t="s">
         <v>4196</v>
       </c>
-      <c r="B57" s="31" t="s">
+      <c r="B57" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="C57" s="29" t="s">
+      <c r="C57" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D57" s="29" t="s">
+      <c r="D57" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E57" s="19" t="s">
+      <c r="E57" s="18" t="s">
         <v>3078</v>
       </c>
-      <c r="F57" s="17"/>
-      <c r="G57" s="17" t="s">
+      <c r="F57" s="16"/>
+      <c r="G57" s="16" t="s">
         <v>4099</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="31" t="s">
+      <c r="A58" s="30" t="s">
         <v>2567</v>
       </c>
-      <c r="B58" s="19" t="s">
+      <c r="B58" s="18" t="s">
         <v>4202</v>
       </c>
-      <c r="C58" s="29" t="s">
+      <c r="C58" s="28" t="s">
         <v>4191</v>
       </c>
-      <c r="D58" s="29" t="s">
+      <c r="D58" s="28" t="s">
         <v>4022</v>
       </c>
-      <c r="E58" s="19" t="s">
+      <c r="E58" s="18" t="s">
         <v>3154</v>
       </c>
-      <c r="F58" s="17"/>
+      <c r="F58" s="16"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" s="31" t="s">
+      <c r="A59" s="30" t="s">
         <v>2568</v>
       </c>
-      <c r="B59" s="19" t="s">
+      <c r="B59" s="18" t="s">
         <v>4203</v>
       </c>
-      <c r="C59" s="29" t="s">
+      <c r="C59" s="28" t="s">
         <v>4191</v>
       </c>
-      <c r="D59" s="29" t="s">
+      <c r="D59" s="28" t="s">
         <v>4022</v>
       </c>
-      <c r="E59" s="19" t="s">
+      <c r="E59" s="18" t="s">
         <v>3155</v>
       </c>
-      <c r="F59" s="17"/>
+      <c r="F59" s="16"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60" s="17" t="s">
+      <c r="A60" s="16" t="s">
         <v>4204</v>
       </c>
-      <c r="B60" s="31" t="s">
+      <c r="B60" s="30" t="s">
         <v>2567</v>
       </c>
-      <c r="C60" s="29" t="s">
+      <c r="C60" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D60" s="29" t="s">
+      <c r="D60" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E60" s="19" t="s">
+      <c r="E60" s="18" t="s">
         <v>3154</v>
       </c>
-      <c r="F60" s="17"/>
-      <c r="G60" s="17" t="s">
+      <c r="F60" s="16"/>
+      <c r="G60" s="16" t="s">
         <v>4099</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A61" s="17" t="s">
+      <c r="A61" s="16" t="s">
         <v>4205</v>
       </c>
-      <c r="B61" s="31" t="s">
+      <c r="B61" s="30" t="s">
         <v>2568</v>
       </c>
-      <c r="C61" s="29" t="s">
+      <c r="C61" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D61" s="29" t="s">
+      <c r="D61" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E61" s="19" t="s">
+      <c r="E61" s="18" t="s">
         <v>3155</v>
       </c>
-      <c r="F61" s="17"/>
-      <c r="G61" s="17" t="s">
+      <c r="F61" s="16"/>
+      <c r="G61" s="16" t="s">
         <v>4099</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A62" s="31" t="s">
+      <c r="A62" s="30" t="s">
         <v>4200</v>
       </c>
-      <c r="B62" s="29" t="s">
+      <c r="B62" s="28" t="s">
         <v>4198</v>
       </c>
-      <c r="C62" s="29" t="s">
+      <c r="C62" s="28" t="s">
         <v>4071</v>
       </c>
-      <c r="D62" s="29" t="s">
+      <c r="D62" s="28" t="s">
         <v>4022</v>
       </c>
-      <c r="E62" s="20" t="s">
+      <c r="E62" s="19" t="s">
         <v>4201</v>
       </c>
-      <c r="F62" s="17"/>
+      <c r="F62" s="16"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" s="29" t="s">
+      <c r="A63" s="28" t="s">
         <v>4199</v>
       </c>
-      <c r="B63" s="31" t="s">
+      <c r="B63" s="30" t="s">
         <v>4200</v>
       </c>
-      <c r="C63" s="29" t="s">
+      <c r="C63" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D63" s="29" t="s">
+      <c r="D63" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E63" s="20" t="s">
+      <c r="E63" s="19" t="s">
         <v>4201</v>
       </c>
-      <c r="G63" s="17" t="s">
+      <c r="G63" s="16" t="s">
         <v>4099</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A64" s="31" t="s">
+      <c r="A64" s="30" t="s">
         <v>4039</v>
       </c>
-      <c r="B64" s="29" t="s">
+      <c r="B64" s="28" t="s">
         <v>4183</v>
       </c>
-      <c r="C64" s="29" t="s">
+      <c r="C64" s="28" t="s">
         <v>4191</v>
       </c>
-      <c r="D64" s="29" t="s">
+      <c r="D64" s="28" t="s">
         <v>4022</v>
       </c>
-      <c r="E64" s="19" t="s">
+      <c r="E64" s="18" t="s">
         <v>3071</v>
       </c>
-      <c r="F64" s="17"/>
+      <c r="F64" s="16"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A65" s="31" t="s">
+      <c r="A65" s="30" t="s">
         <v>4041</v>
       </c>
-      <c r="B65" s="29" t="s">
+      <c r="B65" s="28" t="s">
         <v>4182</v>
       </c>
-      <c r="C65" s="29" t="s">
+      <c r="C65" s="28" t="s">
         <v>4191</v>
       </c>
-      <c r="D65" s="29" t="s">
+      <c r="D65" s="28" t="s">
         <v>4022</v>
       </c>
-      <c r="E65" s="19" t="s">
+      <c r="E65" s="18" t="s">
         <v>3072</v>
       </c>
-      <c r="F65" s="17"/>
+      <c r="F65" s="16"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66" s="29" t="s">
+      <c r="A66" s="28" t="s">
         <v>4189</v>
       </c>
-      <c r="B66" s="31" t="s">
+      <c r="B66" s="30" t="s">
         <v>1580</v>
       </c>
-      <c r="C66" s="29" t="s">
+      <c r="C66" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D66" s="29" t="s">
+      <c r="D66" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E66" s="19" t="s">
+      <c r="E66" s="18" t="s">
         <v>3071</v>
       </c>
-      <c r="G66" s="17" t="s">
+      <c r="G66" s="16" t="s">
         <v>4099</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="29" t="s">
+      <c r="A67" s="28" t="s">
         <v>4190</v>
       </c>
-      <c r="B67" s="31" t="s">
+      <c r="B67" s="30" t="s">
         <v>4184</v>
       </c>
-      <c r="C67" s="29" t="s">
+      <c r="C67" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D67" s="29" t="s">
+      <c r="D67" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E67" s="19" t="s">
+      <c r="E67" s="18" t="s">
         <v>3072</v>
       </c>
-      <c r="G67" s="17" t="s">
+      <c r="G67" s="16" t="s">
         <v>4099</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A68" s="29" t="s">
+      <c r="A68" s="28" t="s">
         <v>4188</v>
       </c>
-      <c r="B68" s="31" t="s">
+      <c r="B68" s="30" t="s">
         <v>1682</v>
       </c>
-      <c r="C68" s="29" t="s">
+      <c r="C68" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D68" s="29" t="s">
+      <c r="D68" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E68" s="19" t="s">
+      <c r="E68" s="18" t="s">
         <v>2165</v>
       </c>
-      <c r="F68" s="17"/>
-      <c r="G68" s="17" t="s">
+      <c r="F68" s="16"/>
+      <c r="G68" s="16" t="s">
         <v>4099</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="29" t="s">
+      <c r="A69" s="28" t="s">
         <v>4187</v>
       </c>
-      <c r="B69" s="31" t="s">
+      <c r="B69" s="30" t="s">
         <v>1681</v>
       </c>
-      <c r="C69" s="29" t="s">
+      <c r="C69" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D69" s="29" t="s">
+      <c r="D69" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E69" s="19" t="s">
+      <c r="E69" s="18" t="s">
         <v>2164</v>
       </c>
-      <c r="F69" s="17"/>
-      <c r="G69" s="17" t="s">
+      <c r="F69" s="16"/>
+      <c r="G69" s="16" t="s">
         <v>4099</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A70" s="29" t="s">
+      <c r="A70" s="28" t="s">
         <v>4186</v>
       </c>
-      <c r="B70" s="31" t="s">
+      <c r="B70" s="30" t="s">
         <v>1582</v>
       </c>
-      <c r="C70" s="29" t="s">
+      <c r="C70" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D70" s="29" t="s">
+      <c r="D70" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E70" s="19" t="s">
+      <c r="E70" s="18" t="s">
         <v>3073</v>
       </c>
-      <c r="F70" s="17"/>
-      <c r="G70" s="17" t="s">
+      <c r="F70" s="16"/>
+      <c r="G70" s="16" t="s">
         <v>4099</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71" s="29" t="s">
+      <c r="A71" s="28" t="s">
         <v>4185</v>
       </c>
-      <c r="B71" s="31" t="s">
+      <c r="B71" s="30" t="s">
         <v>4044</v>
       </c>
-      <c r="C71" s="29" t="s">
+      <c r="C71" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D71" s="29" t="s">
+      <c r="D71" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E71" s="19" t="s">
+      <c r="E71" s="18" t="s">
         <v>3357</v>
       </c>
-      <c r="F71" s="17"/>
-      <c r="G71" s="17" t="s">
+      <c r="F71" s="16"/>
+      <c r="G71" s="16" t="s">
         <v>4099</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A72" s="29" t="s">
+      <c r="A72" s="28" t="s">
         <v>4145</v>
       </c>
-      <c r="B72" s="31" t="s">
+      <c r="B72" s="30" t="s">
         <v>2520</v>
       </c>
-      <c r="C72" s="29" t="s">
+      <c r="C72" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D72" s="29" t="s">
+      <c r="D72" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E72" s="19" t="s">
+      <c r="E72" s="18" t="s">
         <v>3092</v>
       </c>
-      <c r="F72" s="17"/>
-      <c r="G72" s="17" t="s">
+      <c r="F72" s="16"/>
+      <c r="G72" s="16" t="s">
         <v>4099</v>
       </c>
-      <c r="H72" s="17"/>
+      <c r="H72" s="16"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" s="29" t="s">
+      <c r="A73" s="28" t="s">
         <v>4146</v>
       </c>
-      <c r="B73" s="31" t="s">
+      <c r="B73" s="30" t="s">
         <v>2521</v>
       </c>
-      <c r="C73" s="29" t="s">
+      <c r="C73" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D73" s="29" t="s">
+      <c r="D73" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E73" s="19" t="s">
+      <c r="E73" s="18" t="s">
         <v>3093</v>
       </c>
-      <c r="F73" s="17"/>
-      <c r="G73" s="17" t="s">
+      <c r="F73" s="16"/>
+      <c r="G73" s="16" t="s">
         <v>4099</v>
       </c>
-      <c r="H73" s="17"/>
+      <c r="H73" s="16"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="29" t="s">
+      <c r="A74" s="28" t="s">
         <v>4147</v>
       </c>
-      <c r="B74" s="31" t="s">
+      <c r="B74" s="30" t="s">
         <v>2524</v>
       </c>
-      <c r="C74" s="29" t="s">
+      <c r="C74" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D74" s="29" t="s">
+      <c r="D74" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E74" s="19" t="s">
+      <c r="E74" s="18" t="s">
         <v>3096</v>
       </c>
-      <c r="F74" s="17"/>
-      <c r="G74" s="17" t="s">
+      <c r="F74" s="16"/>
+      <c r="G74" s="16" t="s">
         <v>4099</v>
       </c>
-      <c r="H74" s="17"/>
+      <c r="H74" s="16"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" s="19" t="s">
+      <c r="A75" s="18" t="s">
         <v>4172</v>
       </c>
-      <c r="B75" s="31" t="s">
+      <c r="B75" s="30" t="s">
         <v>1609</v>
       </c>
-      <c r="C75" s="29" t="s">
+      <c r="C75" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D75" s="29" t="s">
+      <c r="D75" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E75" s="19" t="s">
+      <c r="E75" s="18" t="s">
         <v>3125</v>
       </c>
-      <c r="F75" s="17"/>
-      <c r="G75" s="17" t="s">
+      <c r="F75" s="16"/>
+      <c r="G75" s="16" t="s">
         <v>4099</v>
       </c>
-      <c r="H75" s="17"/>
+      <c r="H75" s="16"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" s="19" t="s">
+      <c r="A76" s="18" t="s">
         <v>4173</v>
       </c>
-      <c r="B76" s="31" t="s">
+      <c r="B76" s="30" t="s">
         <v>1610</v>
       </c>
-      <c r="C76" s="29" t="s">
+      <c r="C76" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D76" s="29" t="s">
+      <c r="D76" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E76" s="19" t="s">
+      <c r="E76" s="18" t="s">
         <v>3126</v>
       </c>
-      <c r="F76" s="17"/>
-      <c r="G76" s="17" t="s">
+      <c r="F76" s="16"/>
+      <c r="G76" s="16" t="s">
         <v>4099</v>
       </c>
-      <c r="H76" s="17"/>
+      <c r="H76" s="16"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A77" s="19" t="s">
+      <c r="A77" s="18" t="s">
         <v>4148</v>
       </c>
-      <c r="B77" s="31" t="s">
+      <c r="B77" s="30" t="s">
         <v>1612</v>
       </c>
-      <c r="C77" s="29" t="s">
+      <c r="C77" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D77" s="29" t="s">
+      <c r="D77" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E77" s="19" t="s">
+      <c r="E77" s="18" t="s">
         <v>3128</v>
       </c>
-      <c r="F77" s="17"/>
-      <c r="G77" s="17" t="s">
+      <c r="F77" s="16"/>
+      <c r="G77" s="16" t="s">
         <v>4099</v>
       </c>
-      <c r="H77" s="17"/>
+      <c r="H77" s="16"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A78" s="29" t="s">
+      <c r="A78" s="28" t="s">
         <v>4174</v>
       </c>
-      <c r="B78" s="31" t="s">
+      <c r="B78" s="30" t="s">
         <v>1613</v>
       </c>
-      <c r="C78" s="29" t="s">
+      <c r="C78" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D78" s="29" t="s">
+      <c r="D78" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E78" s="19" t="s">
+      <c r="E78" s="18" t="s">
         <v>3129</v>
       </c>
-      <c r="F78" s="17"/>
-      <c r="G78" s="17" t="s">
+      <c r="F78" s="16"/>
+      <c r="G78" s="16" t="s">
         <v>4099</v>
       </c>
-      <c r="H78" s="17"/>
+      <c r="H78" s="16"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A79" s="29" t="s">
+      <c r="A79" s="28" t="s">
         <v>4175</v>
       </c>
-      <c r="B79" s="31" t="s">
+      <c r="B79" s="30" t="s">
         <v>1614</v>
       </c>
-      <c r="C79" s="29" t="s">
+      <c r="C79" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D79" s="29" t="s">
+      <c r="D79" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E79" s="19" t="s">
+      <c r="E79" s="18" t="s">
         <v>3130</v>
       </c>
-      <c r="F79" s="17"/>
-      <c r="G79" s="17" t="s">
+      <c r="F79" s="16"/>
+      <c r="G79" s="16" t="s">
         <v>4099</v>
       </c>
-      <c r="H79" s="17"/>
+      <c r="H79" s="16"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A80" s="29" t="s">
+      <c r="A80" s="28" t="s">
         <v>4176</v>
       </c>
-      <c r="B80" s="31" t="s">
+      <c r="B80" s="30" t="s">
         <v>1615</v>
       </c>
-      <c r="C80" s="29" t="s">
+      <c r="C80" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D80" s="29" t="s">
+      <c r="D80" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E80" s="19" t="s">
+      <c r="E80" s="18" t="s">
         <v>3131</v>
       </c>
-      <c r="F80" s="17"/>
-      <c r="G80" s="17" t="s">
+      <c r="F80" s="16"/>
+      <c r="G80" s="16" t="s">
         <v>4099</v>
       </c>
-      <c r="H80" s="17"/>
+      <c r="H80" s="16"/>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A81" s="29" t="s">
+      <c r="A81" s="28" t="s">
         <v>4149</v>
       </c>
-      <c r="B81" s="31" t="s">
+      <c r="B81" s="30" t="s">
         <v>2570</v>
       </c>
-      <c r="C81" s="29" t="s">
+      <c r="C81" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D81" s="29" t="s">
+      <c r="D81" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E81" s="19" t="s">
+      <c r="E81" s="18" t="s">
         <v>3158</v>
       </c>
-      <c r="F81" s="17"/>
-      <c r="G81" s="17" t="s">
+      <c r="F81" s="16"/>
+      <c r="G81" s="16" t="s">
         <v>4099</v>
       </c>
-      <c r="H81" s="17"/>
+      <c r="H81" s="16"/>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A82" s="29" t="s">
+      <c r="A82" s="28" t="s">
         <v>4177</v>
       </c>
-      <c r="B82" s="31" t="s">
+      <c r="B82" s="30" t="s">
         <v>4054</v>
       </c>
-      <c r="C82" s="29" t="s">
+      <c r="C82" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D82" s="29" t="s">
+      <c r="D82" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E82" s="19" t="s">
+      <c r="E82" s="18" t="s">
         <v>2103</v>
       </c>
-      <c r="F82" s="17"/>
-      <c r="G82" s="17" t="s">
+      <c r="F82" s="16"/>
+      <c r="G82" s="16" t="s">
         <v>4099</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A83" s="19" t="s">
+      <c r="A83" s="18" t="s">
         <v>4178</v>
       </c>
-      <c r="B83" s="31" t="s">
+      <c r="B83" s="30" t="s">
         <v>4055</v>
       </c>
-      <c r="C83" s="29" t="s">
+      <c r="C83" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D83" s="29" t="s">
+      <c r="D83" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E83" s="19" t="s">
+      <c r="E83" s="18" t="s">
         <v>2070</v>
       </c>
-      <c r="F83" s="17"/>
-      <c r="G83" s="17" t="s">
+      <c r="F83" s="16"/>
+      <c r="G83" s="16" t="s">
         <v>4099</v>
       </c>
-      <c r="H83" s="17"/>
+      <c r="H83" s="16"/>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A84" s="19" t="s">
+      <c r="A84" s="18" t="s">
         <v>4179</v>
       </c>
-      <c r="B84" s="31" t="s">
+      <c r="B84" s="30" t="s">
         <v>4128</v>
       </c>
-      <c r="C84" s="29" t="s">
+      <c r="C84" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D84" s="29" t="s">
+      <c r="D84" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E84" s="19" t="s">
+      <c r="E84" s="18" t="s">
         <v>2071</v>
       </c>
-      <c r="F84" s="17"/>
-      <c r="G84" s="17" t="s">
+      <c r="F84" s="16"/>
+      <c r="G84" s="16" t="s">
         <v>4099</v>
       </c>
-      <c r="H84" s="17"/>
-      <c r="I84" s="19"/>
+      <c r="H84" s="16"/>
+      <c r="I84" s="18"/>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A85" s="19" t="s">
+      <c r="A85" s="18" t="s">
         <v>4180</v>
       </c>
-      <c r="B85" s="31" t="s">
+      <c r="B85" s="30" t="s">
         <v>1594</v>
       </c>
-      <c r="C85" s="29" t="s">
+      <c r="C85" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D85" s="29" t="s">
+      <c r="D85" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E85" s="19" t="s">
+      <c r="E85" s="18" t="s">
         <v>2072</v>
       </c>
-      <c r="F85" s="17"/>
-      <c r="G85" s="17" t="s">
+      <c r="F85" s="16"/>
+      <c r="G85" s="16" t="s">
         <v>4099</v>
       </c>
-      <c r="H85" s="17"/>
-      <c r="I85" s="19"/>
+      <c r="H85" s="16"/>
+      <c r="I85" s="18"/>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A86" s="19" t="s">
+      <c r="A86" s="18" t="s">
         <v>4150</v>
       </c>
-      <c r="B86" s="31" t="s">
+      <c r="B86" s="30" t="s">
         <v>4053</v>
       </c>
-      <c r="C86" s="29" t="s">
+      <c r="C86" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D86" s="29" t="s">
+      <c r="D86" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E86" s="19" t="s">
+      <c r="E86" s="18" t="s">
         <v>2100</v>
       </c>
-      <c r="F86" s="17"/>
-      <c r="G86" s="17" t="s">
+      <c r="F86" s="16"/>
+      <c r="G86" s="16" t="s">
         <v>4099</v>
       </c>
-      <c r="H86" s="17"/>
-      <c r="I86" s="19"/>
+      <c r="H86" s="16"/>
+      <c r="I86" s="18"/>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A87" s="19" t="s">
+      <c r="A87" s="18" t="s">
         <v>4151</v>
       </c>
-      <c r="B87" s="31" t="s">
+      <c r="B87" s="30" t="s">
         <v>4129</v>
       </c>
-      <c r="C87" s="29" t="s">
+      <c r="C87" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D87" s="29" t="s">
+      <c r="D87" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E87" s="19" t="s">
+      <c r="E87" s="18" t="s">
         <v>2101</v>
       </c>
-      <c r="F87" s="17"/>
-      <c r="G87" s="17" t="s">
+      <c r="F87" s="16"/>
+      <c r="G87" s="16" t="s">
         <v>4099</v>
       </c>
-      <c r="H87" s="17"/>
-      <c r="I87" s="19"/>
+      <c r="H87" s="16"/>
+      <c r="I87" s="18"/>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A88" s="19" t="s">
+      <c r="A88" s="18" t="s">
         <v>4181</v>
       </c>
-      <c r="B88" s="31" t="s">
+      <c r="B88" s="30" t="s">
         <v>1680</v>
       </c>
-      <c r="C88" s="29" t="s">
+      <c r="C88" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D88" s="29" t="s">
+      <c r="D88" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E88" s="19" t="s">
+      <c r="E88" s="18" t="s">
         <v>2163</v>
       </c>
-      <c r="F88" s="17"/>
-      <c r="G88" s="17" t="s">
+      <c r="F88" s="16"/>
+      <c r="G88" s="16" t="s">
         <v>4099</v>
       </c>
-      <c r="H88" s="17"/>
-      <c r="I88" s="19"/>
+      <c r="H88" s="16"/>
+      <c r="I88" s="18"/>
     </row>
     <row r="89" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="19" t="s">
+      <c r="A89" s="18" t="s">
         <v>4152</v>
       </c>
-      <c r="B89" s="31" t="s">
+      <c r="B89" s="30" t="s">
         <v>1619</v>
       </c>
-      <c r="C89" s="29" t="s">
+      <c r="C89" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D89" s="29" t="s">
+      <c r="D89" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E89" s="19" t="s">
+      <c r="E89" s="18" t="s">
         <v>2102</v>
       </c>
-      <c r="F89" s="17"/>
-      <c r="G89" s="17" t="s">
+      <c r="F89" s="16"/>
+      <c r="G89" s="16" t="s">
         <v>4099</v>
       </c>
-      <c r="H89" s="17"/>
-      <c r="I89" s="19"/>
+      <c r="H89" s="16"/>
+      <c r="I89" s="18"/>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A90" s="19" t="s">
+      <c r="A90" s="18" t="s">
         <v>4153</v>
       </c>
-      <c r="B90" s="31" t="s">
+      <c r="B90" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="C90" s="29" t="s">
+      <c r="C90" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D90" s="29" t="s">
+      <c r="D90" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E90" s="19" t="s">
+      <c r="E90" s="18" t="s">
         <v>1117</v>
       </c>
-      <c r="F90" s="17"/>
-      <c r="G90" s="17" t="s">
+      <c r="F90" s="16"/>
+      <c r="G90" s="16" t="s">
         <v>4099</v>
       </c>
-      <c r="H90" s="17"/>
-      <c r="I90" s="19"/>
+      <c r="H90" s="16"/>
+      <c r="I90" s="18"/>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A91" s="19" t="s">
+      <c r="A91" s="18" t="s">
         <v>4154</v>
       </c>
-      <c r="B91" s="31" t="s">
+      <c r="B91" s="30" t="s">
         <v>4051</v>
       </c>
-      <c r="C91" s="29" t="s">
+      <c r="C91" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D91" s="29" t="s">
+      <c r="D91" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E91" s="19" t="s">
+      <c r="E91" s="18" t="s">
         <v>1116</v>
       </c>
-      <c r="F91" s="17"/>
-      <c r="G91" s="17" t="s">
+      <c r="F91" s="16"/>
+      <c r="G91" s="16" t="s">
         <v>4099</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A92" s="19" t="s">
+      <c r="A92" s="18" t="s">
         <v>4155</v>
       </c>
-      <c r="B92" s="31" t="s">
+      <c r="B92" s="30" t="s">
         <v>4059</v>
       </c>
-      <c r="C92" s="29" t="s">
+      <c r="C92" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D92" s="29" t="s">
+      <c r="D92" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E92" s="19" t="s">
+      <c r="E92" s="18" t="s">
         <v>1101</v>
       </c>
-      <c r="F92" s="17"/>
-      <c r="G92" s="17" t="s">
+      <c r="F92" s="16"/>
+      <c r="G92" s="16" t="s">
         <v>4099</v>
       </c>
-      <c r="J92" s="17"/>
+      <c r="J92" s="16"/>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A93" s="19" t="s">
+      <c r="A93" s="18" t="s">
         <v>4156</v>
       </c>
-      <c r="B93" s="31" t="s">
+      <c r="B93" s="30" t="s">
         <v>4060</v>
       </c>
-      <c r="C93" s="29" t="s">
+      <c r="C93" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D93" s="29" t="s">
+      <c r="D93" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E93" s="19" t="s">
+      <c r="E93" s="18" t="s">
         <v>1102</v>
       </c>
-      <c r="F93" s="17"/>
-      <c r="G93" s="17" t="s">
+      <c r="F93" s="16"/>
+      <c r="G93" s="16" t="s">
         <v>4099</v>
       </c>
-      <c r="J93" s="17"/>
+      <c r="J93" s="16"/>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A94" s="19" t="s">
+      <c r="A94" s="18" t="s">
         <v>4157</v>
       </c>
-      <c r="B94" s="31" t="s">
+      <c r="B94" s="30" t="s">
         <v>4049</v>
       </c>
-      <c r="C94" s="29" t="s">
+      <c r="C94" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D94" s="29" t="s">
+      <c r="D94" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E94" s="19" t="s">
+      <c r="E94" s="18" t="s">
         <v>1105</v>
       </c>
-      <c r="F94" s="17"/>
-      <c r="G94" s="17" t="s">
+      <c r="F94" s="16"/>
+      <c r="G94" s="16" t="s">
         <v>4099</v>
       </c>
-      <c r="J94" s="17"/>
+      <c r="J94" s="16"/>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A95" s="19" t="s">
+      <c r="A95" s="18" t="s">
         <v>4158</v>
       </c>
-      <c r="B95" s="31" t="s">
+      <c r="B95" s="30" t="s">
         <v>4050</v>
       </c>
-      <c r="C95" s="29" t="s">
+      <c r="C95" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D95" s="29" t="s">
+      <c r="D95" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E95" s="19" t="s">
+      <c r="E95" s="18" t="s">
         <v>1106</v>
       </c>
-      <c r="F95" s="17"/>
-      <c r="G95" s="17" t="s">
+      <c r="F95" s="16"/>
+      <c r="G95" s="16" t="s">
         <v>4099</v>
       </c>
-      <c r="J95" s="17"/>
+      <c r="J95" s="16"/>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A96" s="19" t="s">
+      <c r="A96" s="18" t="s">
         <v>4159</v>
       </c>
-      <c r="B96" s="31" t="s">
+      <c r="B96" s="30" t="s">
         <v>4048</v>
       </c>
-      <c r="C96" s="29" t="s">
+      <c r="C96" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D96" s="29" t="s">
+      <c r="D96" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E96" s="19" t="s">
+      <c r="E96" s="18" t="s">
         <v>1107</v>
       </c>
-      <c r="F96" s="17"/>
-      <c r="G96" s="17" t="s">
+      <c r="F96" s="16"/>
+      <c r="G96" s="16" t="s">
         <v>4099</v>
       </c>
-      <c r="J96" s="17"/>
+      <c r="J96" s="16"/>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A97" s="19" t="s">
+      <c r="A97" s="18" t="s">
         <v>4160</v>
       </c>
-      <c r="B97" s="31" t="s">
+      <c r="B97" s="30" t="s">
         <v>4047</v>
       </c>
-      <c r="C97" s="29" t="s">
+      <c r="C97" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D97" s="29" t="s">
+      <c r="D97" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E97" s="19" t="s">
+      <c r="E97" s="18" t="s">
         <v>1078</v>
       </c>
-      <c r="F97" s="17"/>
-      <c r="G97" s="17" t="s">
+      <c r="F97" s="16"/>
+      <c r="G97" s="16" t="s">
         <v>4099</v>
       </c>
-      <c r="J97" s="17"/>
+      <c r="J97" s="16"/>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A98" s="29" t="s">
+      <c r="A98" s="28" t="s">
         <v>4161</v>
       </c>
-      <c r="B98" s="31" t="s">
+      <c r="B98" s="30" t="s">
         <v>4052</v>
       </c>
-      <c r="C98" s="29" t="s">
+      <c r="C98" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D98" s="29" t="s">
+      <c r="D98" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E98" s="19" t="s">
+      <c r="E98" s="18" t="s">
         <v>1114</v>
       </c>
-      <c r="F98" s="17"/>
-      <c r="G98" s="17" t="s">
+      <c r="F98" s="16"/>
+      <c r="G98" s="16" t="s">
         <v>4099</v>
       </c>
-      <c r="J98" s="17"/>
+      <c r="J98" s="16"/>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A99" s="19" t="s">
+      <c r="A99" s="18" t="s">
         <v>4162</v>
       </c>
-      <c r="B99" s="31" t="s">
+      <c r="B99" s="30" t="s">
         <v>4046</v>
       </c>
-      <c r="C99" s="29" t="s">
+      <c r="C99" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D99" s="29" t="s">
+      <c r="D99" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E99" s="19" t="s">
+      <c r="E99" s="18" t="s">
         <v>1108</v>
       </c>
-      <c r="F99" s="17"/>
-      <c r="G99" s="17" t="s">
+      <c r="F99" s="16"/>
+      <c r="G99" s="16" t="s">
         <v>4099</v>
       </c>
-      <c r="J99" s="17"/>
+      <c r="J99" s="16"/>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A100" s="19" t="s">
+      <c r="A100" s="18" t="s">
         <v>4163</v>
       </c>
-      <c r="B100" s="31" t="s">
+      <c r="B100" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="C100" s="29" t="s">
+      <c r="C100" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D100" s="29" t="s">
+      <c r="D100" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E100" s="19" t="s">
+      <c r="E100" s="18" t="s">
         <v>334</v>
       </c>
-      <c r="F100" s="17"/>
-      <c r="G100" s="17" t="s">
+      <c r="F100" s="16"/>
+      <c r="G100" s="16" t="s">
         <v>4099</v>
       </c>
-      <c r="J100" s="17"/>
+      <c r="J100" s="16"/>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A101" s="19" t="s">
+      <c r="A101" s="18" t="s">
         <v>4207</v>
       </c>
-      <c r="B101" s="31" t="s">
+      <c r="B101" s="30" t="s">
         <v>4206</v>
       </c>
-      <c r="C101" s="29" t="s">
+      <c r="C101" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D101" s="29" t="s">
+      <c r="D101" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E101" s="19" t="s">
+      <c r="E101" s="18" t="s">
         <v>332</v>
       </c>
-      <c r="F101" s="17"/>
-      <c r="G101" s="17" t="s">
+      <c r="F101" s="16"/>
+      <c r="G101" s="16" t="s">
         <v>4099</v>
       </c>
-      <c r="J101" s="17"/>
+      <c r="J101" s="16"/>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A102" s="20" t="s">
+      <c r="A102" s="19" t="s">
         <v>4164</v>
       </c>
-      <c r="B102" s="31" t="s">
+      <c r="B102" s="30" t="s">
         <v>4043</v>
       </c>
-      <c r="C102" s="29" t="s">
+      <c r="C102" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D102" s="29" t="s">
+      <c r="D102" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E102" s="20" t="s">
+      <c r="E102" s="19" t="s">
         <v>3881</v>
       </c>
-      <c r="F102" s="17"/>
-      <c r="G102" s="17" t="s">
+      <c r="F102" s="16"/>
+      <c r="G102" s="16" t="s">
         <v>4099</v>
       </c>
-      <c r="J102" s="17"/>
+      <c r="J102" s="16"/>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A103" s="20" t="s">
+      <c r="A103" s="19" t="s">
         <v>4192</v>
       </c>
-      <c r="B103" s="33" t="s">
+      <c r="B103" s="32" t="s">
         <v>4058</v>
       </c>
-      <c r="C103" s="29" t="s">
+      <c r="C103" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D103" s="29" t="s">
+      <c r="D103" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E103" s="20" t="s">
+      <c r="E103" s="19" t="s">
         <v>3883</v>
       </c>
-      <c r="F103" s="17"/>
-      <c r="G103" s="17" t="s">
+      <c r="F103" s="16"/>
+      <c r="G103" s="16" t="s">
         <v>4099</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J104" s="22"/>
+      <c r="J104" s="21"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:B6 A19:A23 A30:A31 A24:B24 B25:B26 B12:B15 B18 A2:A4">

</xml_diff>

<commit_message>
Pew geocoding variables  updated; passed over to geocoder to match with ADMs
</commit_message>
<xml_diff>
--- a/data_processing/pew/pewQVDict.xlsx
+++ b/data_processing/pew/pewQVDict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natalie_kraft/Documents/LAS/bridash/data_processing/pew/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46820763-FBD3-6448-98EA-37C81861C89F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04BA2D1C-8669-4C4A-AC34-FC9D7B2FB013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="980" yWindow="500" windowWidth="34860" windowHeight="21900" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6276" uniqueCount="4209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6280" uniqueCount="4212">
   <si>
     <t>variable_name</t>
   </si>
@@ -12691,6 +12691,15 @@
   </si>
   <si>
     <t>qdate</t>
+  </si>
+  <si>
+    <t>qs8</t>
+  </si>
+  <si>
+    <t>Urban/Rural/Suburban</t>
+  </si>
+  <si>
+    <t>maybe</t>
   </si>
 </sst>
 </file>
@@ -13012,7 +13021,17 @@
     <cellStyle name="style1653674313118" xfId="7" xr:uid="{9BCB1D19-D975-B94E-A914-38E36B84D20C}"/>
     <cellStyle name="style1653674313702" xfId="8" xr:uid="{3E7AD95F-8CB5-1643-BD70-9D2DF7B58AF9}"/>
   </cellStyles>
-  <dxfs count="308">
+  <dxfs count="309">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -18596,34 +18615,34 @@
   </sheetData>
   <autoFilter ref="A1:D258" xr:uid="{ADFDCDBA-9437-2A4B-99A0-9034E1D786F7}"/>
   <conditionalFormatting sqref="A1:XFD41 A43:XFD43 A44:C44 E44:XFD44 A267:XFD1048576 A45:XFD264">
-    <cfRule type="expression" dxfId="307" priority="7">
+    <cfRule type="expression" dxfId="308" priority="7">
       <formula>$C1="Y"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="306" priority="8">
+    <cfRule type="expression" dxfId="307" priority="8">
       <formula>"$C3='Y'"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D42">
-    <cfRule type="expression" dxfId="305" priority="11">
+    <cfRule type="expression" dxfId="306" priority="11">
       <formula>$D42="Y"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="304" priority="12">
+    <cfRule type="expression" dxfId="305" priority="12">
       <formula>"$C3='Y'"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="expression" dxfId="303" priority="1">
+    <cfRule type="expression" dxfId="304" priority="1">
       <formula>$C42="Y"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="302" priority="2">
+    <cfRule type="expression" dxfId="303" priority="2">
       <formula>"$C3='Y'"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42:B42 E42:XFD42">
-    <cfRule type="expression" dxfId="301" priority="15">
+    <cfRule type="expression" dxfId="302" priority="15">
       <formula>#REF!="Y"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="300" priority="16">
+    <cfRule type="expression" dxfId="301" priority="16">
       <formula>"$C3='Y'"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20545,15 +20564,15 @@
   </sheetData>
   <autoFilter ref="A1:C227" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="C1">
-    <cfRule type="expression" dxfId="299" priority="2">
+    <cfRule type="expression" dxfId="300" priority="2">
       <formula>$C1="Y"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="298" priority="3">
+    <cfRule type="expression" dxfId="299" priority="3">
       <formula>"$C3='Y'"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="297" priority="1">
+    <cfRule type="expression" dxfId="298" priority="1">
       <formula>$C1="Y"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -25578,17 +25597,17 @@
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="A1:XFD520 A523:XFD1048576 C521:XFD521">
-    <cfRule type="expression" dxfId="296" priority="1">
+    <cfRule type="expression" dxfId="297" priority="1">
       <formula>$C1="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D522:XFD522 A522:B522 C521">
-    <cfRule type="expression" dxfId="295" priority="19">
+    <cfRule type="expression" dxfId="296" priority="19">
       <formula>$C520="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A521:B521">
-    <cfRule type="expression" dxfId="294" priority="20">
+    <cfRule type="expression" dxfId="295" priority="20">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -30313,7 +30332,7 @@
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="293" priority="1">
+    <cfRule type="expression" dxfId="294" priority="1">
       <formula>$C1="Y"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -37542,7 +37561,7 @@
   </sheetData>
   <autoFilter ref="A1:C876" xr:uid="{00000000-0001-0000-0300-000000000000}"/>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="292" priority="1">
+    <cfRule type="expression" dxfId="293" priority="1">
       <formula>$C1="Y"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -39230,621 +39249,621 @@
     <mergeCell ref="I1:J1"/>
   </mergeCells>
   <conditionalFormatting sqref="C9:J10 C11:D11 C13:D15 C37:D37 C74:D77 K76:K77 C3:D8 C18:D22 C25:D26">
-    <cfRule type="expression" dxfId="291" priority="71">
+    <cfRule type="expression" dxfId="292" priority="71">
       <formula>$C3="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:F3">
-    <cfRule type="expression" dxfId="290" priority="68">
+    <cfRule type="expression" dxfId="291" priority="68">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29:B29">
-    <cfRule type="expression" dxfId="289" priority="62">
+    <cfRule type="expression" dxfId="290" priority="62">
       <formula>#REF!="Y"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="288" priority="63">
+    <cfRule type="expression" dxfId="289" priority="63">
       <formula>"$C3='Y'"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:B23">
-    <cfRule type="expression" dxfId="287" priority="64">
+    <cfRule type="expression" dxfId="288" priority="64">
       <formula>$C15="Y"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="286" priority="65">
+    <cfRule type="expression" dxfId="287" priority="65">
       <formula>"$C3='Y'"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I25:J25">
-    <cfRule type="expression" dxfId="285" priority="83">
+    <cfRule type="expression" dxfId="286" priority="83">
       <formula>$C14="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:H4">
-    <cfRule type="expression" dxfId="284" priority="85">
+    <cfRule type="expression" dxfId="285" priority="85">
       <formula>$C3="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:B12 A4:B4 A8:B8">
-    <cfRule type="expression" dxfId="283" priority="104">
+    <cfRule type="expression" dxfId="284" priority="104">
       <formula>$C3="Y"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="282" priority="105">
+    <cfRule type="expression" dxfId="283" priority="105">
       <formula>"$C3='Y'"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:B9 A13:B14 A21:B21 A5:B6">
-    <cfRule type="expression" dxfId="281" priority="106">
+    <cfRule type="expression" dxfId="282" priority="106">
       <formula>$C5="Y"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="280" priority="107">
+    <cfRule type="expression" dxfId="281" priority="107">
       <formula>"$C3='Y'"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11:J11 E13:H13 I35:J35 J73">
-    <cfRule type="expression" dxfId="279" priority="112">
+    <cfRule type="expression" dxfId="280" priority="112">
       <formula>$C13="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:F4">
-    <cfRule type="expression" dxfId="278" priority="115">
+    <cfRule type="expression" dxfId="279" priority="115">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19:J19 E5:H6 E27:F27 I27:J28 E35:F35 E33:F33 E32:H32 G34:H34 I54:J54 I37:J37 I71 I43:J49 G55:H65 G49:H49 E7:F8 E21:F21">
-    <cfRule type="expression" dxfId="277" priority="125">
+    <cfRule type="expression" dxfId="278" priority="125">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:H12">
-    <cfRule type="expression" dxfId="276" priority="141">
+    <cfRule type="expression" dxfId="277" priority="141">
       <formula>$C13="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I26:K26">
-    <cfRule type="expression" dxfId="275" priority="145">
+    <cfRule type="expression" dxfId="276" priority="145">
       <formula>$C5="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:J4">
-    <cfRule type="expression" dxfId="274" priority="158">
+    <cfRule type="expression" dxfId="275" priority="158">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16:J16">
-    <cfRule type="expression" dxfId="273" priority="163">
+    <cfRule type="expression" dxfId="274" priority="163">
       <formula>$C11="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17:H17 G24:H24">
-    <cfRule type="expression" dxfId="272" priority="164">
+    <cfRule type="expression" dxfId="273" priority="164">
       <formula>$C14="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38:J38">
-    <cfRule type="expression" dxfId="271" priority="166">
+    <cfRule type="expression" dxfId="272" priority="166">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13:J15 J71">
-    <cfRule type="expression" dxfId="270" priority="199">
+    <cfRule type="expression" dxfId="271" priority="199">
       <formula>$C18="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32:B32">
-    <cfRule type="expression" dxfId="269" priority="202">
+    <cfRule type="expression" dxfId="270" priority="202">
       <formula>$C18="Y"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="268" priority="203">
+    <cfRule type="expression" dxfId="269" priority="203">
       <formula>"$C3='Y'"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E72:F72">
-    <cfRule type="expression" dxfId="267" priority="207">
+    <cfRule type="expression" dxfId="268" priority="207">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41:F42">
-    <cfRule type="expression" dxfId="266" priority="242">
+    <cfRule type="expression" dxfId="267" priority="242">
       <formula>$C18="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:J8">
-    <cfRule type="expression" dxfId="265" priority="250">
+    <cfRule type="expression" dxfId="266" priority="250">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23:J23">
-    <cfRule type="expression" dxfId="264" priority="259">
+    <cfRule type="expression" dxfId="265" priority="259">
       <formula>$C21="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I42:J42">
-    <cfRule type="expression" dxfId="263" priority="283">
+    <cfRule type="expression" dxfId="264" priority="283">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21:J21">
-    <cfRule type="expression" dxfId="262" priority="302">
+    <cfRule type="expression" dxfId="263" priority="302">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I37:J37">
-    <cfRule type="expression" dxfId="261" priority="307">
+    <cfRule type="expression" dxfId="262" priority="307">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30:F30">
-    <cfRule type="expression" dxfId="260" priority="309">
+    <cfRule type="expression" dxfId="261" priority="309">
       <formula>$C21="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I31:J31">
-    <cfRule type="expression" dxfId="259" priority="321">
+    <cfRule type="expression" dxfId="260" priority="321">
       <formula>$C22="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G53:H54">
-    <cfRule type="expression" dxfId="258" priority="336">
+    <cfRule type="expression" dxfId="259" priority="336">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:J20">
-    <cfRule type="expression" dxfId="257" priority="338">
+    <cfRule type="expression" dxfId="258" priority="338">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34:F34 E28:F28">
-    <cfRule type="expression" dxfId="256" priority="339">
+    <cfRule type="expression" dxfId="257" priority="339">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:B37">
-    <cfRule type="expression" dxfId="255" priority="352">
+    <cfRule type="expression" dxfId="256" priority="352">
       <formula>#REF!="Y"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="254" priority="353">
+    <cfRule type="expression" dxfId="255" priority="353">
       <formula>"$C3='Y'"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17:B17">
-    <cfRule type="expression" dxfId="253" priority="366">
+    <cfRule type="expression" dxfId="254" priority="366">
       <formula>$C25="Y"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="252" priority="367">
+    <cfRule type="expression" dxfId="253" priority="367">
       <formula>"$C3='Y'"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11:H11 I12:J12">
-    <cfRule type="expression" dxfId="251" priority="369">
+    <cfRule type="expression" dxfId="252" priority="369">
       <formula>$C25="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:H14">
-    <cfRule type="expression" dxfId="250" priority="377">
+    <cfRule type="expression" dxfId="251" priority="377">
       <formula>$C26="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24:B24">
-    <cfRule type="expression" dxfId="249" priority="378">
+    <cfRule type="expression" dxfId="250" priority="378">
       <formula>$C26="Y"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="248" priority="379">
+    <cfRule type="expression" dxfId="249" priority="379">
       <formula>"$C3='Y'"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26:H26">
-    <cfRule type="expression" dxfId="247" priority="381">
+    <cfRule type="expression" dxfId="248" priority="381">
       <formula>$C20="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19:H20 E22:F22">
-    <cfRule type="expression" dxfId="246" priority="382">
+    <cfRule type="expression" dxfId="247" priority="382">
       <formula>$C3="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:B30">
-    <cfRule type="expression" dxfId="245" priority="389">
+    <cfRule type="expression" dxfId="246" priority="389">
       <formula>$C20="Y"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="244" priority="390">
+    <cfRule type="expression" dxfId="245" priority="390">
       <formula>"$C3='Y'"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G52:H52">
-    <cfRule type="expression" dxfId="243" priority="398">
+    <cfRule type="expression" dxfId="244" priority="398">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20:F20">
-    <cfRule type="expression" dxfId="242" priority="416">
+    <cfRule type="expression" dxfId="243" priority="416">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18:J18">
-    <cfRule type="expression" dxfId="241" priority="417">
+    <cfRule type="expression" dxfId="242" priority="417">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:H3">
-    <cfRule type="expression" dxfId="240" priority="430">
+    <cfRule type="expression" dxfId="241" priority="430">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="expression" dxfId="239" priority="473">
+    <cfRule type="expression" dxfId="240" priority="473">
       <formula>$C22="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31:B31">
-    <cfRule type="expression" dxfId="238" priority="53">
+    <cfRule type="expression" dxfId="239" priority="53">
       <formula>$C29="Y"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="237" priority="54">
+    <cfRule type="expression" dxfId="238" priority="54">
       <formula>"$C3='Y'"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A78:B78">
-    <cfRule type="expression" dxfId="236" priority="51">
+    <cfRule type="expression" dxfId="237" priority="51">
       <formula>$C57="Y"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="235" priority="52">
+    <cfRule type="expression" dxfId="236" priority="52">
       <formula>"$C3='Y'"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9:K10">
-    <cfRule type="expression" dxfId="234" priority="48">
+    <cfRule type="expression" dxfId="235" priority="48">
       <formula>$C9="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11">
-    <cfRule type="expression" dxfId="233" priority="49">
+    <cfRule type="expression" dxfId="234" priority="49">
       <formula>$C13="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="expression" dxfId="232" priority="50">
+    <cfRule type="expression" dxfId="233" priority="50">
       <formula>$C26="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16">
-    <cfRule type="expression" dxfId="231" priority="45">
+    <cfRule type="expression" dxfId="232" priority="45">
       <formula>$C11="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13:K15">
-    <cfRule type="expression" dxfId="230" priority="46">
+    <cfRule type="expression" dxfId="231" priority="46">
       <formula>$C18="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K19">
-    <cfRule type="expression" dxfId="229" priority="43">
+    <cfRule type="expression" dxfId="230" priority="43">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20">
-    <cfRule type="expression" dxfId="228" priority="44">
+    <cfRule type="expression" dxfId="229" priority="44">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21">
-    <cfRule type="expression" dxfId="227" priority="41">
+    <cfRule type="expression" dxfId="228" priority="41">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K23">
-    <cfRule type="expression" dxfId="226" priority="38">
+    <cfRule type="expression" dxfId="227" priority="38">
       <formula>$C21="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K25">
-    <cfRule type="expression" dxfId="225" priority="36">
+    <cfRule type="expression" dxfId="226" priority="36">
       <formula>$C14="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K27:K28">
-    <cfRule type="expression" dxfId="224" priority="34">
+    <cfRule type="expression" dxfId="225" priority="34">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G22:H23">
-    <cfRule type="expression" dxfId="223" priority="508">
+    <cfRule type="expression" dxfId="224" priority="508">
       <formula>$C5="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29:F29">
-    <cfRule type="expression" dxfId="222" priority="509">
+    <cfRule type="expression" dxfId="223" priority="509">
       <formula>$C8="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I39:J39">
-    <cfRule type="expression" dxfId="221" priority="510">
+    <cfRule type="expression" dxfId="222" priority="510">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18:H18">
-    <cfRule type="expression" dxfId="220" priority="512">
+    <cfRule type="expression" dxfId="221" priority="512">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:F19">
-    <cfRule type="expression" dxfId="219" priority="513">
+    <cfRule type="expression" dxfId="220" priority="513">
       <formula>$C3="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59:B59">
-    <cfRule type="expression" dxfId="218" priority="514">
+    <cfRule type="expression" dxfId="219" priority="514">
       <formula>$C4="Y"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="217" priority="515">
+    <cfRule type="expression" dxfId="218" priority="515">
       <formula>"$C3='Y'"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I40:J41">
-    <cfRule type="expression" dxfId="216" priority="516">
+    <cfRule type="expression" dxfId="217" priority="516">
       <formula>$C3="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G50:H51">
-    <cfRule type="expression" dxfId="215" priority="517">
+    <cfRule type="expression" dxfId="216" priority="517">
       <formula>$C7="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I24:K24">
-    <cfRule type="expression" dxfId="214" priority="520">
+    <cfRule type="expression" dxfId="215" priority="520">
       <formula>$C7="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E66:F66">
-    <cfRule type="expression" dxfId="213" priority="523">
+    <cfRule type="expression" dxfId="214" priority="523">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E75:F75">
-    <cfRule type="expression" dxfId="212" priority="525">
+    <cfRule type="expression" dxfId="213" priority="525">
       <formula>$C5="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E74:F74">
-    <cfRule type="expression" dxfId="211" priority="526">
+    <cfRule type="expression" dxfId="212" priority="526">
       <formula>$C7="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22:K22">
-    <cfRule type="expression" dxfId="210" priority="527">
+    <cfRule type="expression" dxfId="211" priority="527">
       <formula>$C6="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5:K8">
-    <cfRule type="expression" dxfId="209" priority="33">
+    <cfRule type="expression" dxfId="210" priority="33">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E67:F67">
-    <cfRule type="expression" dxfId="208" priority="528">
+    <cfRule type="expression" dxfId="209" priority="528">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49:B49">
-    <cfRule type="expression" dxfId="207" priority="529">
+    <cfRule type="expression" dxfId="208" priority="529">
       <formula>#REF!="Y"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="206" priority="530">
+    <cfRule type="expression" dxfId="207" priority="530">
       <formula>"$C3='Y'"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53:B53">
-    <cfRule type="expression" dxfId="205" priority="531">
+    <cfRule type="expression" dxfId="206" priority="531">
       <formula>$C32="Y"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="204" priority="532">
+    <cfRule type="expression" dxfId="205" priority="532">
       <formula>"$C3='Y'"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G35:H36">
-    <cfRule type="expression" dxfId="203" priority="533">
+    <cfRule type="expression" dxfId="204" priority="533">
       <formula>$C18="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33:H33">
-    <cfRule type="expression" dxfId="202" priority="534">
+    <cfRule type="expression" dxfId="203" priority="534">
       <formula>$C22="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19:B19">
-    <cfRule type="expression" dxfId="201" priority="541">
+    <cfRule type="expression" dxfId="202" priority="541">
       <formula>$C37="Y"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="200" priority="542">
+    <cfRule type="expression" dxfId="201" priority="542">
       <formula>"$C3='Y'"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E69:F69 K69">
-    <cfRule type="expression" dxfId="199" priority="544">
+    <cfRule type="expression" dxfId="200" priority="544">
       <formula>$C75="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E71:F71">
-    <cfRule type="expression" dxfId="198" priority="545">
+    <cfRule type="expression" dxfId="199" priority="545">
       <formula>$C74="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E73:F73">
-    <cfRule type="expression" dxfId="197" priority="552">
+    <cfRule type="expression" dxfId="198" priority="552">
       <formula>$C22="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E68:F68">
-    <cfRule type="expression" dxfId="196" priority="554">
+    <cfRule type="expression" dxfId="197" priority="554">
       <formula>$C20="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E70:F70">
-    <cfRule type="expression" dxfId="195" priority="556">
+    <cfRule type="expression" dxfId="196" priority="556">
       <formula>$C37="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21:H21">
-    <cfRule type="expression" dxfId="194" priority="600">
+    <cfRule type="expression" dxfId="195" priority="600">
       <formula>$C56="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J74">
-    <cfRule type="expression" dxfId="193" priority="10">
+    <cfRule type="expression" dxfId="194" priority="10">
       <formula>$C25="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K71">
-    <cfRule type="expression" dxfId="192" priority="20">
+    <cfRule type="expression" dxfId="193" priority="20">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K75">
-    <cfRule type="expression" dxfId="191" priority="22">
+    <cfRule type="expression" dxfId="192" priority="22">
       <formula>$C5="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K73">
-    <cfRule type="expression" dxfId="190" priority="23">
+    <cfRule type="expression" dxfId="191" priority="23">
       <formula>$C7="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K72">
-    <cfRule type="expression" dxfId="189" priority="27">
+    <cfRule type="expression" dxfId="190" priority="27">
       <formula>$C22="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J68">
-    <cfRule type="expression" dxfId="188" priority="11">
+    <cfRule type="expression" dxfId="189" priority="11">
       <formula>$C7="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J77">
-    <cfRule type="expression" dxfId="187" priority="12">
+    <cfRule type="expression" dxfId="188" priority="12">
       <formula>$C6="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J76">
-    <cfRule type="expression" dxfId="186" priority="13">
+    <cfRule type="expression" dxfId="187" priority="13">
       <formula>$C8="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J69">
-    <cfRule type="expression" dxfId="185" priority="14">
+    <cfRule type="expression" dxfId="186" priority="14">
       <formula>$C21="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J75">
-    <cfRule type="expression" dxfId="184" priority="17">
+    <cfRule type="expression" dxfId="185" priority="17">
       <formula>$C23="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J70">
-    <cfRule type="expression" dxfId="183" priority="18">
+    <cfRule type="expression" dxfId="184" priority="18">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J72">
-    <cfRule type="expression" dxfId="182" priority="19">
+    <cfRule type="expression" dxfId="183" priority="19">
       <formula>$C38="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K55:K65">
-    <cfRule type="expression" dxfId="181" priority="8">
+    <cfRule type="expression" dxfId="182" priority="8">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K54">
-    <cfRule type="expression" dxfId="180" priority="9">
+    <cfRule type="expression" dxfId="181" priority="9">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K52">
-    <cfRule type="expression" dxfId="179" priority="6">
+    <cfRule type="expression" dxfId="180" priority="6">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K51">
-    <cfRule type="expression" dxfId="178" priority="7">
+    <cfRule type="expression" dxfId="179" priority="7">
       <formula>$C8="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:H8">
-    <cfRule type="expression" dxfId="177" priority="608">
+    <cfRule type="expression" dxfId="178" priority="608">
       <formula>$C57="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20:B20">
-    <cfRule type="expression" dxfId="176" priority="609">
+    <cfRule type="expression" dxfId="177" priority="609">
       <formula>$C74="Y"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="175" priority="610">
+    <cfRule type="expression" dxfId="176" priority="610">
       <formula>"$C3='Y'"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I33:J33">
-    <cfRule type="expression" dxfId="174" priority="611">
+    <cfRule type="expression" dxfId="175" priority="611">
       <formula>$C75="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18:B18">
-    <cfRule type="expression" dxfId="173" priority="612">
+    <cfRule type="expression" dxfId="174" priority="612">
       <formula>$C75="Y"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="172" priority="613">
+    <cfRule type="expression" dxfId="173" priority="613">
       <formula>"$C3='Y'"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36:J36">
-    <cfRule type="expression" dxfId="171" priority="614">
+    <cfRule type="expression" dxfId="172" priority="614">
       <formula>$C74="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K43:K48">
-    <cfRule type="expression" dxfId="170" priority="1">
+    <cfRule type="expression" dxfId="171" priority="1">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K38">
-    <cfRule type="expression" dxfId="169" priority="2">
+    <cfRule type="expression" dxfId="170" priority="2">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K42">
-    <cfRule type="expression" dxfId="168" priority="3">
+    <cfRule type="expression" dxfId="169" priority="3">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K39">
-    <cfRule type="expression" dxfId="167" priority="4">
+    <cfRule type="expression" dxfId="168" priority="4">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K40:K41">
-    <cfRule type="expression" dxfId="166" priority="5">
+    <cfRule type="expression" dxfId="167" priority="5">
       <formula>$C3="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K70">
-    <cfRule type="expression" dxfId="165" priority="617">
+    <cfRule type="expression" dxfId="166" priority="617">
       <formula>$C74="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:B3">
-    <cfRule type="expression" dxfId="164" priority="621">
+    <cfRule type="expression" dxfId="165" priority="621">
       <formula>#REF!="Y"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="163" priority="622">
+    <cfRule type="expression" dxfId="164" priority="622">
       <formula>"$C3='Y'"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17:K17">
-    <cfRule type="expression" dxfId="162" priority="623">
+    <cfRule type="expression" dxfId="163" priority="623">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:H15">
-    <cfRule type="expression" dxfId="161" priority="624">
+    <cfRule type="expression" dxfId="162" priority="624">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -39854,10 +39873,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB360FDB-9222-4846-8C29-B1EE5CE081EB}">
-  <dimension ref="A1:J104"/>
+  <dimension ref="A1:J105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A8:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -39982,160 +40001,157 @@
       </c>
       <c r="F6" s="16"/>
     </row>
-    <row r="7" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="30" t="s">
+        <v>4209</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>4210</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>4063</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>4211</v>
+      </c>
+      <c r="F7" s="16"/>
+    </row>
+    <row r="8" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="30" t="s">
         <v>4208</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B8" s="29" t="s">
         <v>4095</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C8" s="28" t="s">
         <v>4062</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D8" s="28" t="s">
         <v>4022</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E8" s="18" t="s">
         <v>2396</v>
       </c>
-      <c r="F7" s="16"/>
-    </row>
-    <row r="8" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="30" t="s">
+      <c r="F8" s="16"/>
+    </row>
+    <row r="9" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B9" s="28" t="s">
         <v>1191</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C9" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D9" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E9" s="28" t="s">
         <v>112</v>
-      </c>
-      <c r="F8" s="16"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="30" t="s">
-        <v>4065</v>
-      </c>
-      <c r="B9" s="28" t="s">
-        <v>4066</v>
-      </c>
-      <c r="C9" s="28" t="s">
-        <v>4067</v>
-      </c>
-      <c r="D9" s="28" t="s">
-        <v>4068</v>
-      </c>
-      <c r="E9" s="28" t="s">
-        <v>4066</v>
       </c>
       <c r="F9" s="16"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="30" t="s">
-        <v>113</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>4070</v>
+        <v>4065</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>4066</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>4071</v>
+        <v>4067</v>
       </c>
       <c r="D10" s="28" t="s">
         <v>4068</v>
       </c>
-      <c r="E10" s="18" t="s">
-        <v>3401</v>
+      <c r="E10" s="28" t="s">
+        <v>4066</v>
       </c>
       <c r="F10" s="16"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="30" t="s">
-        <v>188</v>
-      </c>
-      <c r="B11" s="28" t="s">
-        <v>4072</v>
+        <v>113</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>4070</v>
       </c>
       <c r="C11" s="28" t="s">
         <v>4071</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>4022</v>
+        <v>4068</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>3590</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>4097</v>
-      </c>
+        <v>3401</v>
+      </c>
+      <c r="F11" s="16"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="30" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>4073</v>
+        <v>4072</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>4074</v>
+        <v>4071</v>
       </c>
       <c r="D12" s="28" t="s">
         <v>4022</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>3591</v>
+        <v>3590</v>
       </c>
       <c r="F12" s="16" t="s">
         <v>4097</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="165" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="30" t="s">
-        <v>4111</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>4112</v>
+        <v>189</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>4073</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>4067</v>
+        <v>4074</v>
       </c>
       <c r="D13" s="28" t="s">
         <v>4022</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="18" t="s">
+        <v>3591</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>4097</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="165" x14ac:dyDescent="0.2">
+      <c r="A14" s="30" t="s">
+        <v>4111</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>4112</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>4067</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>4022</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>405</v>
       </c>
-      <c r="F13" s="16"/>
-    </row>
-    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.2">
-      <c r="A14" s="30" t="s">
+      <c r="F14" s="16"/>
+    </row>
+    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+      <c r="A15" s="30" t="s">
         <v>4113</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B15" s="28" t="s">
         <v>4114</v>
-      </c>
-      <c r="C14" s="28" t="s">
-        <v>4063</v>
-      </c>
-      <c r="D14" s="28" t="s">
-        <v>4069</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>425</v>
-      </c>
-      <c r="F14" s="16"/>
-    </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A15" s="30" t="s">
-        <v>4115</v>
-      </c>
-      <c r="B15" s="28" t="s">
-        <v>4116</v>
       </c>
       <c r="C15" s="28" t="s">
         <v>4063</v>
@@ -40144,91 +40160,91 @@
         <v>4069</v>
       </c>
       <c r="E15" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="F15" s="16"/>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+      <c r="A16" s="30" t="s">
+        <v>4115</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>4116</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>4063</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>4069</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>340</v>
       </c>
-      <c r="F15" s="16"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="30" t="s">
+      <c r="F16" s="16"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="B16" s="28" t="s">
+      <c r="B17" s="28" t="s">
         <v>4125</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C17" s="28" t="s">
         <v>4071</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="D17" s="28" t="s">
         <v>4022</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>1258</v>
-      </c>
-      <c r="F16" s="16"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="18" t="s">
-        <v>4193</v>
-      </c>
-      <c r="B17" s="30" t="s">
-        <v>132</v>
-      </c>
-      <c r="C17" s="28" t="s">
-        <v>4063</v>
-      </c>
-      <c r="D17" s="28" t="s">
-        <v>4069</v>
       </c>
       <c r="E17" s="18" t="s">
         <v>1258</v>
       </c>
       <c r="F17" s="16"/>
-      <c r="G17" s="16" t="s">
-        <v>4099</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="75" x14ac:dyDescent="0.2">
-      <c r="A18" s="30" t="s">
-        <v>4117</v>
-      </c>
-      <c r="B18" s="28" t="s">
-        <v>4118</v>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="18" t="s">
+        <v>4193</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>132</v>
       </c>
       <c r="C18" s="28" t="s">
         <v>4063</v>
       </c>
       <c r="D18" s="28" t="s">
+        <v>4069</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>1258</v>
+      </c>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16" t="s">
+        <v>4099</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="75" x14ac:dyDescent="0.2">
+      <c r="A19" s="30" t="s">
+        <v>4117</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>4118</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>4063</v>
+      </c>
+      <c r="D19" s="28" t="s">
         <v>4119</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E19" s="5" t="s">
         <v>362</v>
       </c>
-      <c r="F18" s="16"/>
-    </row>
-    <row r="19" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="30" t="s">
+      <c r="F19" s="16"/>
+    </row>
+    <row r="20" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="30" t="s">
         <v>4086</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B20" s="28" t="s">
         <v>4083</v>
-      </c>
-      <c r="C19" s="28" t="s">
-        <v>4071</v>
-      </c>
-      <c r="D19" s="28" t="s">
-        <v>4022</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>4169</v>
-      </c>
-      <c r="F19" s="16"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="30" t="s">
-        <v>4085</v>
-      </c>
-      <c r="B20" s="28" t="s">
-        <v>4084</v>
       </c>
       <c r="C20" s="28" t="s">
         <v>4071</v>
@@ -40243,10 +40259,10 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="30" t="s">
-        <v>4089</v>
+        <v>4085</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>4090</v>
+        <v>4084</v>
       </c>
       <c r="C21" s="28" t="s">
         <v>4071</v>
@@ -40261,10 +40277,10 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="30" t="s">
-        <v>4091</v>
+        <v>4089</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>4092</v>
+        <v>4090</v>
       </c>
       <c r="C22" s="28" t="s">
         <v>4071</v>
@@ -40279,10 +40295,10 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="30" t="s">
-        <v>4087</v>
+        <v>4091</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>4088</v>
+        <v>4092</v>
       </c>
       <c r="C23" s="28" t="s">
         <v>4071</v>
@@ -40296,89 +40312,89 @@
       <c r="F23" s="16"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="30" t="s">
+        <v>4087</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>4088</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>4071</v>
+      </c>
+      <c r="D24" s="28" t="s">
+        <v>4022</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>4169</v>
+      </c>
+      <c r="F24" s="16"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="16" t="s">
         <v>4131</v>
       </c>
-      <c r="B24" s="30" t="s">
+      <c r="B25" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="C24" s="28" t="s">
+      <c r="C25" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D24" s="28" t="s">
+      <c r="D25" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E24" s="33" t="s">
+      <c r="E25" s="33" t="s">
         <v>3084</v>
       </c>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16" t="s">
+      <c r="F25" s="16"/>
+      <c r="G25" s="16" t="s">
         <v>4099</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="30" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>4082</v>
       </c>
-      <c r="C25" s="28" t="s">
+      <c r="C26" s="28" t="s">
         <v>4071</v>
       </c>
-      <c r="D25" s="28" t="s">
+      <c r="D26" s="28" t="s">
         <v>4068</v>
-      </c>
-      <c r="E25" s="18" t="s">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>4132</v>
-      </c>
-      <c r="B26" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="28" t="s">
-        <v>4063</v>
-      </c>
-      <c r="D26" s="28" t="s">
-        <v>4069</v>
       </c>
       <c r="E26" s="18" t="s">
         <v>3000</v>
       </c>
-      <c r="G26" s="16" t="s">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>4132</v>
+      </c>
+      <c r="B27" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>4063</v>
+      </c>
+      <c r="D27" s="28" t="s">
+        <v>4069</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>3000</v>
+      </c>
+      <c r="G27" s="16" t="s">
         <v>4099</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A27" s="30" t="s">
-        <v>4100</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>4093</v>
-      </c>
-      <c r="C27" s="28" t="s">
-        <v>4067</v>
-      </c>
-      <c r="D27" s="28" t="s">
-        <v>4022</v>
-      </c>
-      <c r="E27" s="18" t="s">
-        <v>4170</v>
-      </c>
-      <c r="F27" s="16"/>
     </row>
     <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A28" s="30" t="s">
-        <v>4101</v>
+        <v>4100</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>4094</v>
-      </c>
-      <c r="C28" s="9" t="s">
+        <v>4093</v>
+      </c>
+      <c r="C28" s="28" t="s">
         <v>4067</v>
       </c>
       <c r="D28" s="28" t="s">
@@ -40389,48 +40405,51 @@
       </c>
       <c r="F28" s="16"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="16" t="s">
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+      <c r="A29" s="30" t="s">
+        <v>4101</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>4094</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>4067</v>
+      </c>
+      <c r="D29" s="28" t="s">
+        <v>4022</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>4170</v>
+      </c>
+      <c r="F29" s="16"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="16" t="s">
         <v>4133</v>
       </c>
-      <c r="B29" s="30" t="s">
+      <c r="B30" s="30" t="s">
         <v>4098</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C30" s="9" t="s">
         <v>4063</v>
       </c>
-      <c r="D29" s="28" t="s">
+      <c r="D30" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E29" s="18" t="s">
+      <c r="E30" s="18" t="s">
         <v>1113</v>
       </c>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16" t="s">
+      <c r="F30" s="16"/>
+      <c r="G30" s="16" t="s">
         <v>4099</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="25" t="s">
-        <v>4078</v>
-      </c>
-      <c r="B30" s="28" t="s">
-        <v>4079</v>
-      </c>
-      <c r="C30" s="28" t="s">
-        <v>4063</v>
-      </c>
-      <c r="D30" s="28" t="s">
-        <v>4022</v>
-      </c>
-      <c r="F30" s="16"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="25" t="s">
-        <v>4080</v>
+        <v>4078</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>4081</v>
+        <v>4079</v>
       </c>
       <c r="C31" s="28" t="s">
         <v>4063</v>
@@ -40441,14 +40460,14 @@
       <c r="F31" s="16"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="30" t="s">
-        <v>4030</v>
-      </c>
-      <c r="B32" t="s">
-        <v>4102</v>
+      <c r="A32" s="25" t="s">
+        <v>4080</v>
+      </c>
+      <c r="B32" s="28" t="s">
+        <v>4081</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>4071</v>
+        <v>4063</v>
       </c>
       <c r="D32" s="28" t="s">
         <v>4022</v>
@@ -40457,10 +40476,10 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="30" t="s">
-        <v>4031</v>
+        <v>4030</v>
       </c>
       <c r="B33" t="s">
-        <v>4103</v>
+        <v>4102</v>
       </c>
       <c r="C33" s="28" t="s">
         <v>4071</v>
@@ -40472,10 +40491,10 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="30" t="s">
-        <v>4032</v>
+        <v>4031</v>
       </c>
       <c r="B34" t="s">
-        <v>4104</v>
+        <v>4103</v>
       </c>
       <c r="C34" s="28" t="s">
         <v>4071</v>
@@ -40487,10 +40506,10 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="30" t="s">
-        <v>4033</v>
-      </c>
-      <c r="B35" s="31" t="s">
-        <v>4105</v>
+        <v>4032</v>
+      </c>
+      <c r="B35" t="s">
+        <v>4104</v>
       </c>
       <c r="C35" s="28" t="s">
         <v>4071</v>
@@ -40502,10 +40521,10 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="30" t="s">
-        <v>1464</v>
-      </c>
-      <c r="B36" t="s">
-        <v>4107</v>
+        <v>4033</v>
+      </c>
+      <c r="B36" s="31" t="s">
+        <v>4105</v>
       </c>
       <c r="C36" s="28" t="s">
         <v>4071</v>
@@ -40517,10 +40536,10 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="30" t="s">
-        <v>1466</v>
+        <v>1464</v>
       </c>
       <c r="B37" t="s">
-        <v>4106</v>
+        <v>4107</v>
       </c>
       <c r="C37" s="28" t="s">
         <v>4071</v>
@@ -40532,10 +40551,10 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="30" t="s">
-        <v>4026</v>
+        <v>1466</v>
       </c>
       <c r="B38" t="s">
-        <v>4110</v>
+        <v>4106</v>
       </c>
       <c r="C38" s="28" t="s">
         <v>4071</v>
@@ -40547,10 +40566,10 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="B39" s="28" t="s">
-        <v>4109</v>
+        <v>4026</v>
+      </c>
+      <c r="B39" t="s">
+        <v>4110</v>
       </c>
       <c r="C39" s="28" t="s">
         <v>4071</v>
@@ -40562,10 +40581,10 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="B40" t="s">
-        <v>4108</v>
+        <v>101</v>
+      </c>
+      <c r="B40" s="28" t="s">
+        <v>4109</v>
       </c>
       <c r="C40" s="28" t="s">
         <v>4071</v>
@@ -40576,29 +40595,26 @@
       <c r="F40" s="16"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="18" t="s">
+      <c r="A41" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="B41" t="s">
+        <v>4108</v>
+      </c>
+      <c r="C41" s="28" t="s">
+        <v>4071</v>
+      </c>
+      <c r="D41" s="28" t="s">
+        <v>4022</v>
+      </c>
+      <c r="F41" s="16"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="18" t="s">
         <v>4134</v>
       </c>
-      <c r="B41" s="30" t="s">
+      <c r="B42" s="30" t="s">
         <v>1465</v>
-      </c>
-      <c r="C41" s="28" t="s">
-        <v>4063</v>
-      </c>
-      <c r="D41" s="28" t="s">
-        <v>4069</v>
-      </c>
-      <c r="F41" s="16"/>
-      <c r="G41" s="16" t="s">
-        <v>4099</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>4135</v>
-      </c>
-      <c r="B42" s="30" t="s">
-        <v>4031</v>
       </c>
       <c r="C42" s="28" t="s">
         <v>4063</v>
@@ -40612,11 +40628,11 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="31" t="s">
-        <v>4136</v>
+      <c r="A43" t="s">
+        <v>4135</v>
       </c>
       <c r="B43" s="30" t="s">
-        <v>4032</v>
+        <v>4031</v>
       </c>
       <c r="C43" s="28" t="s">
         <v>4063</v>
@@ -40631,10 +40647,10 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="31" t="s">
-        <v>4137</v>
+        <v>4136</v>
       </c>
       <c r="B44" s="30" t="s">
-        <v>4033</v>
+        <v>4032</v>
       </c>
       <c r="C44" s="28" t="s">
         <v>4063</v>
@@ -40648,11 +40664,11 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="28" t="s">
-        <v>4139</v>
+      <c r="A45" s="31" t="s">
+        <v>4137</v>
       </c>
       <c r="B45" s="30" t="s">
-        <v>1464</v>
+        <v>4033</v>
       </c>
       <c r="C45" s="28" t="s">
         <v>4063</v>
@@ -40666,11 +40682,11 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>4138</v>
+      <c r="A46" s="28" t="s">
+        <v>4139</v>
       </c>
       <c r="B46" s="30" t="s">
-        <v>1466</v>
+        <v>1464</v>
       </c>
       <c r="C46" s="28" t="s">
         <v>4063</v>
@@ -40685,10 +40701,10 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>4140</v>
+        <v>4138</v>
       </c>
       <c r="B47" s="30" t="s">
-        <v>4026</v>
+        <v>1466</v>
       </c>
       <c r="C47" s="28" t="s">
         <v>4063</v>
@@ -40702,11 +40718,11 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="28" t="s">
-        <v>4141</v>
+      <c r="A48" t="s">
+        <v>4140</v>
       </c>
       <c r="B48" s="30" t="s">
-        <v>101</v>
+        <v>4026</v>
       </c>
       <c r="C48" s="28" t="s">
         <v>4063</v>
@@ -40720,11 +40736,11 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>4142</v>
+      <c r="A49" s="28" t="s">
+        <v>4141</v>
       </c>
       <c r="B49" s="30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C49" s="28" t="s">
         <v>4063</v>
@@ -40738,95 +40754,95 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="30" t="s">
+      <c r="A50" t="s">
+        <v>4142</v>
+      </c>
+      <c r="B50" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="C50" s="28" t="s">
+        <v>4063</v>
+      </c>
+      <c r="D50" s="28" t="s">
+        <v>4069</v>
+      </c>
+      <c r="F50" s="16"/>
+      <c r="G50" s="16" t="s">
+        <v>4099</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" s="30" t="s">
         <v>1590</v>
       </c>
-      <c r="B50" s="18" t="s">
+      <c r="B51" s="18" t="s">
         <v>4126</v>
       </c>
-      <c r="C50" s="28" t="s">
+      <c r="C51" s="28" t="s">
         <v>4071</v>
       </c>
-      <c r="D50" s="28" t="s">
+      <c r="D51" s="28" t="s">
         <v>4022</v>
       </c>
-      <c r="F50" s="16"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="16" t="s">
+      <c r="F51" s="16"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="16" t="s">
         <v>4143</v>
       </c>
-      <c r="B51" s="30" t="s">
+      <c r="B52" s="30" t="s">
         <v>1590</v>
       </c>
-      <c r="C51" s="28" t="s">
+      <c r="C52" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D51" s="28" t="s">
+      <c r="D52" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="F51" s="16"/>
-      <c r="G51" s="16" t="s">
+      <c r="F52" s="16"/>
+      <c r="G52" s="16" t="s">
         <v>4099</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="30" t="s">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" s="30" t="s">
         <v>1591</v>
       </c>
-      <c r="B52" s="16" t="s">
+      <c r="B53" s="16" t="s">
         <v>4127</v>
       </c>
-      <c r="C52" s="28" t="s">
+      <c r="C53" s="28" t="s">
         <v>4071</v>
       </c>
-      <c r="D52" s="28" t="s">
+      <c r="D53" s="28" t="s">
         <v>4022</v>
       </c>
-      <c r="F52" s="16"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="16" t="s">
+      <c r="F53" s="16"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" s="16" t="s">
         <v>4144</v>
       </c>
-      <c r="B53" s="30" t="s">
+      <c r="B54" s="30" t="s">
         <v>1591</v>
       </c>
-      <c r="C53" s="28" t="s">
+      <c r="C54" s="28" t="s">
         <v>4063</v>
       </c>
-      <c r="D53" s="28" t="s">
+      <c r="D54" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="F53" s="16"/>
-      <c r="G53" s="16" t="s">
+      <c r="F54" s="16"/>
+      <c r="G54" s="16" t="s">
         <v>4099</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="B54" s="28" t="s">
-        <v>4194</v>
-      </c>
-      <c r="C54" s="28" t="s">
-        <v>4071</v>
-      </c>
-      <c r="D54" s="28" t="s">
-        <v>4022</v>
-      </c>
-      <c r="E54" s="18" t="s">
-        <v>3001</v>
-      </c>
-      <c r="F54" s="16"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="30" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="B55" s="28" t="s">
-        <v>4195</v>
+        <v>4194</v>
       </c>
       <c r="C55" s="28" t="s">
         <v>4071</v>
@@ -40835,37 +40851,34 @@
         <v>4022</v>
       </c>
       <c r="E55" s="18" t="s">
+        <v>3001</v>
+      </c>
+      <c r="F55" s="16"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="B56" s="28" t="s">
+        <v>4195</v>
+      </c>
+      <c r="C56" s="28" t="s">
+        <v>4071</v>
+      </c>
+      <c r="D56" s="28" t="s">
+        <v>4022</v>
+      </c>
+      <c r="E56" s="18" t="s">
         <v>3078</v>
       </c>
-      <c r="F55" s="16"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="16" t="s">
-        <v>4197</v>
-      </c>
-      <c r="B56" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="C56" s="28" t="s">
-        <v>4063</v>
-      </c>
-      <c r="D56" s="28" t="s">
-        <v>4069</v>
-      </c>
-      <c r="E56" s="18" t="s">
-        <v>3001</v>
-      </c>
       <c r="F56" s="16"/>
-      <c r="G56" s="16" t="s">
-        <v>4099</v>
-      </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="16" t="s">
-        <v>4196</v>
+        <v>4197</v>
       </c>
       <c r="B57" s="30" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="C57" s="28" t="s">
         <v>4063</v>
@@ -40874,7 +40887,7 @@
         <v>4069</v>
       </c>
       <c r="E57" s="18" t="s">
-        <v>3078</v>
+        <v>3001</v>
       </c>
       <c r="F57" s="16"/>
       <c r="G57" s="16" t="s">
@@ -40882,29 +40895,32 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="30" t="s">
-        <v>2567</v>
-      </c>
-      <c r="B58" s="18" t="s">
-        <v>4202</v>
+      <c r="A58" s="16" t="s">
+        <v>4196</v>
+      </c>
+      <c r="B58" s="30" t="s">
+        <v>92</v>
       </c>
       <c r="C58" s="28" t="s">
-        <v>4191</v>
+        <v>4063</v>
       </c>
       <c r="D58" s="28" t="s">
-        <v>4022</v>
+        <v>4069</v>
       </c>
       <c r="E58" s="18" t="s">
-        <v>3154</v>
+        <v>3078</v>
       </c>
       <c r="F58" s="16"/>
+      <c r="G58" s="16" t="s">
+        <v>4099</v>
+      </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="30" t="s">
-        <v>2568</v>
+        <v>2567</v>
       </c>
       <c r="B59" s="18" t="s">
-        <v>4203</v>
+        <v>4202</v>
       </c>
       <c r="C59" s="28" t="s">
         <v>4191</v>
@@ -40913,37 +40929,34 @@
         <v>4022</v>
       </c>
       <c r="E59" s="18" t="s">
+        <v>3154</v>
+      </c>
+      <c r="F59" s="16"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" s="30" t="s">
+        <v>2568</v>
+      </c>
+      <c r="B60" s="18" t="s">
+        <v>4203</v>
+      </c>
+      <c r="C60" s="28" t="s">
+        <v>4191</v>
+      </c>
+      <c r="D60" s="28" t="s">
+        <v>4022</v>
+      </c>
+      <c r="E60" s="18" t="s">
         <v>3155</v>
       </c>
-      <c r="F59" s="16"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60" s="16" t="s">
-        <v>4204</v>
-      </c>
-      <c r="B60" s="30" t="s">
-        <v>2567</v>
-      </c>
-      <c r="C60" s="28" t="s">
-        <v>4063</v>
-      </c>
-      <c r="D60" s="28" t="s">
-        <v>4069</v>
-      </c>
-      <c r="E60" s="18" t="s">
-        <v>3154</v>
-      </c>
       <c r="F60" s="16"/>
-      <c r="G60" s="16" t="s">
-        <v>4099</v>
-      </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="16" t="s">
-        <v>4205</v>
+        <v>4204</v>
       </c>
       <c r="B61" s="30" t="s">
-        <v>2568</v>
+        <v>2567</v>
       </c>
       <c r="C61" s="28" t="s">
         <v>4063</v>
@@ -40952,7 +40965,7 @@
         <v>4069</v>
       </c>
       <c r="E61" s="18" t="s">
-        <v>3155</v>
+        <v>3154</v>
       </c>
       <c r="F61" s="16"/>
       <c r="G61" s="16" t="s">
@@ -40960,67 +40973,70 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A62" s="30" t="s">
+      <c r="A62" s="16" t="s">
+        <v>4205</v>
+      </c>
+      <c r="B62" s="30" t="s">
+        <v>2568</v>
+      </c>
+      <c r="C62" s="28" t="s">
+        <v>4063</v>
+      </c>
+      <c r="D62" s="28" t="s">
+        <v>4069</v>
+      </c>
+      <c r="E62" s="18" t="s">
+        <v>3155</v>
+      </c>
+      <c r="F62" s="16"/>
+      <c r="G62" s="16" t="s">
+        <v>4099</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" s="30" t="s">
         <v>4200</v>
       </c>
-      <c r="B62" s="28" t="s">
+      <c r="B63" s="28" t="s">
         <v>4198</v>
       </c>
-      <c r="C62" s="28" t="s">
+      <c r="C63" s="28" t="s">
         <v>4071</v>
       </c>
-      <c r="D62" s="28" t="s">
+      <c r="D63" s="28" t="s">
         <v>4022</v>
-      </c>
-      <c r="E62" s="19" t="s">
-        <v>4201</v>
-      </c>
-      <c r="F62" s="16"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" s="28" t="s">
-        <v>4199</v>
-      </c>
-      <c r="B63" s="30" t="s">
-        <v>4200</v>
-      </c>
-      <c r="C63" s="28" t="s">
-        <v>4063</v>
-      </c>
-      <c r="D63" s="28" t="s">
-        <v>4069</v>
       </c>
       <c r="E63" s="19" t="s">
         <v>4201</v>
       </c>
-      <c r="G63" s="16" t="s">
+      <c r="F63" s="16"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" s="28" t="s">
+        <v>4199</v>
+      </c>
+      <c r="B64" s="30" t="s">
+        <v>4200</v>
+      </c>
+      <c r="C64" s="28" t="s">
+        <v>4063</v>
+      </c>
+      <c r="D64" s="28" t="s">
+        <v>4069</v>
+      </c>
+      <c r="E64" s="19" t="s">
+        <v>4201</v>
+      </c>
+      <c r="G64" s="16" t="s">
         <v>4099</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A64" s="30" t="s">
-        <v>4039</v>
-      </c>
-      <c r="B64" s="28" t="s">
-        <v>4183</v>
-      </c>
-      <c r="C64" s="28" t="s">
-        <v>4191</v>
-      </c>
-      <c r="D64" s="28" t="s">
-        <v>4022</v>
-      </c>
-      <c r="E64" s="18" t="s">
-        <v>3071</v>
-      </c>
-      <c r="F64" s="16"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="30" t="s">
-        <v>4041</v>
+        <v>4039</v>
       </c>
       <c r="B65" s="28" t="s">
-        <v>4182</v>
+        <v>4183</v>
       </c>
       <c r="C65" s="28" t="s">
         <v>4191</v>
@@ -41029,36 +41045,34 @@
         <v>4022</v>
       </c>
       <c r="E65" s="18" t="s">
+        <v>3071</v>
+      </c>
+      <c r="F65" s="16"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="30" t="s">
+        <v>4041</v>
+      </c>
+      <c r="B66" s="28" t="s">
+        <v>4182</v>
+      </c>
+      <c r="C66" s="28" t="s">
+        <v>4191</v>
+      </c>
+      <c r="D66" s="28" t="s">
+        <v>4022</v>
+      </c>
+      <c r="E66" s="18" t="s">
         <v>3072</v>
       </c>
-      <c r="F65" s="16"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66" s="28" t="s">
+      <c r="F66" s="16"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="28" t="s">
         <v>4189</v>
       </c>
-      <c r="B66" s="30" t="s">
+      <c r="B67" s="30" t="s">
         <v>1580</v>
-      </c>
-      <c r="C66" s="28" t="s">
-        <v>4063</v>
-      </c>
-      <c r="D66" s="28" t="s">
-        <v>4069</v>
-      </c>
-      <c r="E66" s="18" t="s">
-        <v>3071</v>
-      </c>
-      <c r="G66" s="16" t="s">
-        <v>4099</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="28" t="s">
-        <v>4190</v>
-      </c>
-      <c r="B67" s="30" t="s">
-        <v>4184</v>
       </c>
       <c r="C67" s="28" t="s">
         <v>4063</v>
@@ -41067,18 +41081,18 @@
         <v>4069</v>
       </c>
       <c r="E67" s="18" t="s">
-        <v>3072</v>
+        <v>3071</v>
       </c>
       <c r="G67" s="16" t="s">
         <v>4099</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="28" t="s">
-        <v>4188</v>
+        <v>4190</v>
       </c>
       <c r="B68" s="30" t="s">
-        <v>1682</v>
+        <v>4184</v>
       </c>
       <c r="C68" s="28" t="s">
         <v>4063</v>
@@ -41087,19 +41101,18 @@
         <v>4069</v>
       </c>
       <c r="E68" s="18" t="s">
-        <v>2165</v>
-      </c>
-      <c r="F68" s="16"/>
+        <v>3072</v>
+      </c>
       <c r="G68" s="16" t="s">
         <v>4099</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="28" t="s">
-        <v>4187</v>
+        <v>4188</v>
       </c>
       <c r="B69" s="30" t="s">
-        <v>1681</v>
+        <v>1682</v>
       </c>
       <c r="C69" s="28" t="s">
         <v>4063</v>
@@ -41108,19 +41121,19 @@
         <v>4069</v>
       </c>
       <c r="E69" s="18" t="s">
-        <v>2164</v>
+        <v>2165</v>
       </c>
       <c r="F69" s="16"/>
       <c r="G69" s="16" t="s">
         <v>4099</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="28" t="s">
-        <v>4186</v>
+        <v>4187</v>
       </c>
       <c r="B70" s="30" t="s">
-        <v>1582</v>
+        <v>1681</v>
       </c>
       <c r="C70" s="28" t="s">
         <v>4063</v>
@@ -41129,7 +41142,7 @@
         <v>4069</v>
       </c>
       <c r="E70" s="18" t="s">
-        <v>3073</v>
+        <v>2164</v>
       </c>
       <c r="F70" s="16"/>
       <c r="G70" s="16" t="s">
@@ -41138,10 +41151,10 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="28" t="s">
-        <v>4185</v>
+        <v>4186</v>
       </c>
       <c r="B71" s="30" t="s">
-        <v>4044</v>
+        <v>1582</v>
       </c>
       <c r="C71" s="28" t="s">
         <v>4063</v>
@@ -41150,7 +41163,7 @@
         <v>4069</v>
       </c>
       <c r="E71" s="18" t="s">
-        <v>3357</v>
+        <v>3073</v>
       </c>
       <c r="F71" s="16"/>
       <c r="G71" s="16" t="s">
@@ -41159,10 +41172,10 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="28" t="s">
-        <v>4145</v>
+        <v>4185</v>
       </c>
       <c r="B72" s="30" t="s">
-        <v>2520</v>
+        <v>4044</v>
       </c>
       <c r="C72" s="28" t="s">
         <v>4063</v>
@@ -41171,20 +41184,19 @@
         <v>4069</v>
       </c>
       <c r="E72" s="18" t="s">
-        <v>3092</v>
+        <v>3357</v>
       </c>
       <c r="F72" s="16"/>
       <c r="G72" s="16" t="s">
         <v>4099</v>
       </c>
-      <c r="H72" s="16"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="28" t="s">
-        <v>4146</v>
+        <v>4145</v>
       </c>
       <c r="B73" s="30" t="s">
-        <v>2521</v>
+        <v>2520</v>
       </c>
       <c r="C73" s="28" t="s">
         <v>4063</v>
@@ -41193,7 +41205,7 @@
         <v>4069</v>
       </c>
       <c r="E73" s="18" t="s">
-        <v>3093</v>
+        <v>3092</v>
       </c>
       <c r="F73" s="16"/>
       <c r="G73" s="16" t="s">
@@ -41203,10 +41215,10 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="28" t="s">
-        <v>4147</v>
+        <v>4146</v>
       </c>
       <c r="B74" s="30" t="s">
-        <v>2524</v>
+        <v>2521</v>
       </c>
       <c r="C74" s="28" t="s">
         <v>4063</v>
@@ -41215,7 +41227,7 @@
         <v>4069</v>
       </c>
       <c r="E74" s="18" t="s">
-        <v>3096</v>
+        <v>3093</v>
       </c>
       <c r="F74" s="16"/>
       <c r="G74" s="16" t="s">
@@ -41224,11 +41236,11 @@
       <c r="H74" s="16"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" s="18" t="s">
-        <v>4172</v>
+      <c r="A75" s="28" t="s">
+        <v>4147</v>
       </c>
       <c r="B75" s="30" t="s">
-        <v>1609</v>
+        <v>2524</v>
       </c>
       <c r="C75" s="28" t="s">
         <v>4063</v>
@@ -41237,7 +41249,7 @@
         <v>4069</v>
       </c>
       <c r="E75" s="18" t="s">
-        <v>3125</v>
+        <v>3096</v>
       </c>
       <c r="F75" s="16"/>
       <c r="G75" s="16" t="s">
@@ -41247,10 +41259,10 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="18" t="s">
-        <v>4173</v>
+        <v>4172</v>
       </c>
       <c r="B76" s="30" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="C76" s="28" t="s">
         <v>4063</v>
@@ -41259,7 +41271,7 @@
         <v>4069</v>
       </c>
       <c r="E76" s="18" t="s">
-        <v>3126</v>
+        <v>3125</v>
       </c>
       <c r="F76" s="16"/>
       <c r="G76" s="16" t="s">
@@ -41269,10 +41281,10 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="18" t="s">
-        <v>4148</v>
+        <v>4173</v>
       </c>
       <c r="B77" s="30" t="s">
-        <v>1612</v>
+        <v>1610</v>
       </c>
       <c r="C77" s="28" t="s">
         <v>4063</v>
@@ -41281,7 +41293,7 @@
         <v>4069</v>
       </c>
       <c r="E77" s="18" t="s">
-        <v>3128</v>
+        <v>3126</v>
       </c>
       <c r="F77" s="16"/>
       <c r="G77" s="16" t="s">
@@ -41290,11 +41302,11 @@
       <c r="H77" s="16"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A78" s="28" t="s">
-        <v>4174</v>
+      <c r="A78" s="18" t="s">
+        <v>4148</v>
       </c>
       <c r="B78" s="30" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="C78" s="28" t="s">
         <v>4063</v>
@@ -41303,7 +41315,7 @@
         <v>4069</v>
       </c>
       <c r="E78" s="18" t="s">
-        <v>3129</v>
+        <v>3128</v>
       </c>
       <c r="F78" s="16"/>
       <c r="G78" s="16" t="s">
@@ -41313,10 +41325,10 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="28" t="s">
-        <v>4175</v>
+        <v>4174</v>
       </c>
       <c r="B79" s="30" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
       <c r="C79" s="28" t="s">
         <v>4063</v>
@@ -41325,7 +41337,7 @@
         <v>4069</v>
       </c>
       <c r="E79" s="18" t="s">
-        <v>3130</v>
+        <v>3129</v>
       </c>
       <c r="F79" s="16"/>
       <c r="G79" s="16" t="s">
@@ -41335,10 +41347,10 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="28" t="s">
-        <v>4176</v>
+        <v>4175</v>
       </c>
       <c r="B80" s="30" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
       <c r="C80" s="28" t="s">
         <v>4063</v>
@@ -41347,7 +41359,7 @@
         <v>4069</v>
       </c>
       <c r="E80" s="18" t="s">
-        <v>3131</v>
+        <v>3130</v>
       </c>
       <c r="F80" s="16"/>
       <c r="G80" s="16" t="s">
@@ -41357,10 +41369,10 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" s="28" t="s">
-        <v>4149</v>
+        <v>4176</v>
       </c>
       <c r="B81" s="30" t="s">
-        <v>2570</v>
+        <v>1615</v>
       </c>
       <c r="C81" s="28" t="s">
         <v>4063</v>
@@ -41369,7 +41381,7 @@
         <v>4069</v>
       </c>
       <c r="E81" s="18" t="s">
-        <v>3158</v>
+        <v>3131</v>
       </c>
       <c r="F81" s="16"/>
       <c r="G81" s="16" t="s">
@@ -41379,10 +41391,10 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" s="28" t="s">
-        <v>4177</v>
+        <v>4149</v>
       </c>
       <c r="B82" s="30" t="s">
-        <v>4054</v>
+        <v>2570</v>
       </c>
       <c r="C82" s="28" t="s">
         <v>4063</v>
@@ -41391,19 +41403,20 @@
         <v>4069</v>
       </c>
       <c r="E82" s="18" t="s">
-        <v>2103</v>
+        <v>3158</v>
       </c>
       <c r="F82" s="16"/>
       <c r="G82" s="16" t="s">
         <v>4099</v>
       </c>
+      <c r="H82" s="16"/>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A83" s="18" t="s">
-        <v>4178</v>
+      <c r="A83" s="28" t="s">
+        <v>4177</v>
       </c>
       <c r="B83" s="30" t="s">
-        <v>4055</v>
+        <v>4054</v>
       </c>
       <c r="C83" s="28" t="s">
         <v>4063</v>
@@ -41412,20 +41425,19 @@
         <v>4069</v>
       </c>
       <c r="E83" s="18" t="s">
-        <v>2070</v>
+        <v>2103</v>
       </c>
       <c r="F83" s="16"/>
       <c r="G83" s="16" t="s">
         <v>4099</v>
       </c>
-      <c r="H83" s="16"/>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" s="18" t="s">
-        <v>4179</v>
+        <v>4178</v>
       </c>
       <c r="B84" s="30" t="s">
-        <v>4128</v>
+        <v>4055</v>
       </c>
       <c r="C84" s="28" t="s">
         <v>4063</v>
@@ -41434,21 +41446,20 @@
         <v>4069</v>
       </c>
       <c r="E84" s="18" t="s">
-        <v>2071</v>
+        <v>2070</v>
       </c>
       <c r="F84" s="16"/>
       <c r="G84" s="16" t="s">
         <v>4099</v>
       </c>
       <c r="H84" s="16"/>
-      <c r="I84" s="18"/>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" s="18" t="s">
-        <v>4180</v>
+        <v>4179</v>
       </c>
       <c r="B85" s="30" t="s">
-        <v>1594</v>
+        <v>4128</v>
       </c>
       <c r="C85" s="28" t="s">
         <v>4063</v>
@@ -41457,7 +41468,7 @@
         <v>4069</v>
       </c>
       <c r="E85" s="18" t="s">
-        <v>2072</v>
+        <v>2071</v>
       </c>
       <c r="F85" s="16"/>
       <c r="G85" s="16" t="s">
@@ -41468,10 +41479,10 @@
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" s="18" t="s">
-        <v>4150</v>
+        <v>4180</v>
       </c>
       <c r="B86" s="30" t="s">
-        <v>4053</v>
+        <v>1594</v>
       </c>
       <c r="C86" s="28" t="s">
         <v>4063</v>
@@ -41480,7 +41491,7 @@
         <v>4069</v>
       </c>
       <c r="E86" s="18" t="s">
-        <v>2100</v>
+        <v>2072</v>
       </c>
       <c r="F86" s="16"/>
       <c r="G86" s="16" t="s">
@@ -41491,10 +41502,10 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" s="18" t="s">
-        <v>4151</v>
+        <v>4150</v>
       </c>
       <c r="B87" s="30" t="s">
-        <v>4129</v>
+        <v>4053</v>
       </c>
       <c r="C87" s="28" t="s">
         <v>4063</v>
@@ -41503,7 +41514,7 @@
         <v>4069</v>
       </c>
       <c r="E87" s="18" t="s">
-        <v>2101</v>
+        <v>2100</v>
       </c>
       <c r="F87" s="16"/>
       <c r="G87" s="16" t="s">
@@ -41514,10 +41525,10 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" s="18" t="s">
-        <v>4181</v>
+        <v>4151</v>
       </c>
       <c r="B88" s="30" t="s">
-        <v>1680</v>
+        <v>4129</v>
       </c>
       <c r="C88" s="28" t="s">
         <v>4063</v>
@@ -41526,7 +41537,7 @@
         <v>4069</v>
       </c>
       <c r="E88" s="18" t="s">
-        <v>2163</v>
+        <v>2101</v>
       </c>
       <c r="F88" s="16"/>
       <c r="G88" s="16" t="s">
@@ -41535,12 +41546,12 @@
       <c r="H88" s="16"/>
       <c r="I88" s="18"/>
     </row>
-    <row r="89" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" s="18" t="s">
-        <v>4152</v>
+        <v>4181</v>
       </c>
       <c r="B89" s="30" t="s">
-        <v>1619</v>
+        <v>1680</v>
       </c>
       <c r="C89" s="28" t="s">
         <v>4063</v>
@@ -41549,7 +41560,7 @@
         <v>4069</v>
       </c>
       <c r="E89" s="18" t="s">
-        <v>2102</v>
+        <v>2163</v>
       </c>
       <c r="F89" s="16"/>
       <c r="G89" s="16" t="s">
@@ -41558,12 +41569,12 @@
       <c r="H89" s="16"/>
       <c r="I89" s="18"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="18" t="s">
-        <v>4153</v>
+        <v>4152</v>
       </c>
       <c r="B90" s="30" t="s">
-        <v>106</v>
+        <v>1619</v>
       </c>
       <c r="C90" s="28" t="s">
         <v>4063</v>
@@ -41572,7 +41583,7 @@
         <v>4069</v>
       </c>
       <c r="E90" s="18" t="s">
-        <v>1117</v>
+        <v>2102</v>
       </c>
       <c r="F90" s="16"/>
       <c r="G90" s="16" t="s">
@@ -41583,10 +41594,10 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" s="18" t="s">
-        <v>4154</v>
+        <v>4153</v>
       </c>
       <c r="B91" s="30" t="s">
-        <v>4051</v>
+        <v>106</v>
       </c>
       <c r="C91" s="28" t="s">
         <v>4063</v>
@@ -41595,19 +41606,21 @@
         <v>4069</v>
       </c>
       <c r="E91" s="18" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="F91" s="16"/>
       <c r="G91" s="16" t="s">
         <v>4099</v>
       </c>
+      <c r="H91" s="16"/>
+      <c r="I91" s="18"/>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" s="18" t="s">
-        <v>4155</v>
+        <v>4154</v>
       </c>
       <c r="B92" s="30" t="s">
-        <v>4059</v>
+        <v>4051</v>
       </c>
       <c r="C92" s="28" t="s">
         <v>4063</v>
@@ -41616,20 +41629,19 @@
         <v>4069</v>
       </c>
       <c r="E92" s="18" t="s">
-        <v>1101</v>
+        <v>1116</v>
       </c>
       <c r="F92" s="16"/>
       <c r="G92" s="16" t="s">
         <v>4099</v>
       </c>
-      <c r="J92" s="16"/>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" s="18" t="s">
-        <v>4156</v>
+        <v>4155</v>
       </c>
       <c r="B93" s="30" t="s">
-        <v>4060</v>
+        <v>4059</v>
       </c>
       <c r="C93" s="28" t="s">
         <v>4063</v>
@@ -41638,7 +41650,7 @@
         <v>4069</v>
       </c>
       <c r="E93" s="18" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="F93" s="16"/>
       <c r="G93" s="16" t="s">
@@ -41648,10 +41660,10 @@
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" s="18" t="s">
-        <v>4157</v>
+        <v>4156</v>
       </c>
       <c r="B94" s="30" t="s">
-        <v>4049</v>
+        <v>4060</v>
       </c>
       <c r="C94" s="28" t="s">
         <v>4063</v>
@@ -41660,7 +41672,7 @@
         <v>4069</v>
       </c>
       <c r="E94" s="18" t="s">
-        <v>1105</v>
+        <v>1102</v>
       </c>
       <c r="F94" s="16"/>
       <c r="G94" s="16" t="s">
@@ -41670,10 +41682,10 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" s="18" t="s">
-        <v>4158</v>
+        <v>4157</v>
       </c>
       <c r="B95" s="30" t="s">
-        <v>4050</v>
+        <v>4049</v>
       </c>
       <c r="C95" s="28" t="s">
         <v>4063</v>
@@ -41682,7 +41694,7 @@
         <v>4069</v>
       </c>
       <c r="E95" s="18" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="F95" s="16"/>
       <c r="G95" s="16" t="s">
@@ -41692,10 +41704,10 @@
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" s="18" t="s">
-        <v>4159</v>
+        <v>4158</v>
       </c>
       <c r="B96" s="30" t="s">
-        <v>4048</v>
+        <v>4050</v>
       </c>
       <c r="C96" s="28" t="s">
         <v>4063</v>
@@ -41704,7 +41716,7 @@
         <v>4069</v>
       </c>
       <c r="E96" s="18" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="F96" s="16"/>
       <c r="G96" s="16" t="s">
@@ -41714,10 +41726,10 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" s="18" t="s">
-        <v>4160</v>
+        <v>4159</v>
       </c>
       <c r="B97" s="30" t="s">
-        <v>4047</v>
+        <v>4048</v>
       </c>
       <c r="C97" s="28" t="s">
         <v>4063</v>
@@ -41726,7 +41738,7 @@
         <v>4069</v>
       </c>
       <c r="E97" s="18" t="s">
-        <v>1078</v>
+        <v>1107</v>
       </c>
       <c r="F97" s="16"/>
       <c r="G97" s="16" t="s">
@@ -41735,11 +41747,11 @@
       <c r="J97" s="16"/>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A98" s="28" t="s">
-        <v>4161</v>
+      <c r="A98" s="18" t="s">
+        <v>4160</v>
       </c>
       <c r="B98" s="30" t="s">
-        <v>4052</v>
+        <v>4047</v>
       </c>
       <c r="C98" s="28" t="s">
         <v>4063</v>
@@ -41748,7 +41760,7 @@
         <v>4069</v>
       </c>
       <c r="E98" s="18" t="s">
-        <v>1114</v>
+        <v>1078</v>
       </c>
       <c r="F98" s="16"/>
       <c r="G98" s="16" t="s">
@@ -41757,11 +41769,11 @@
       <c r="J98" s="16"/>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A99" s="18" t="s">
-        <v>4162</v>
+      <c r="A99" s="28" t="s">
+        <v>4161</v>
       </c>
       <c r="B99" s="30" t="s">
-        <v>4046</v>
+        <v>4052</v>
       </c>
       <c r="C99" s="28" t="s">
         <v>4063</v>
@@ -41770,7 +41782,7 @@
         <v>4069</v>
       </c>
       <c r="E99" s="18" t="s">
-        <v>1108</v>
+        <v>1114</v>
       </c>
       <c r="F99" s="16"/>
       <c r="G99" s="16" t="s">
@@ -41780,10 +41792,10 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" s="18" t="s">
-        <v>4163</v>
+        <v>4162</v>
       </c>
       <c r="B100" s="30" t="s">
-        <v>108</v>
+        <v>4046</v>
       </c>
       <c r="C100" s="28" t="s">
         <v>4063</v>
@@ -41792,7 +41804,7 @@
         <v>4069</v>
       </c>
       <c r="E100" s="18" t="s">
-        <v>334</v>
+        <v>1108</v>
       </c>
       <c r="F100" s="16"/>
       <c r="G100" s="16" t="s">
@@ -41802,10 +41814,10 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" s="18" t="s">
-        <v>4207</v>
+        <v>4163</v>
       </c>
       <c r="B101" s="30" t="s">
-        <v>4206</v>
+        <v>108</v>
       </c>
       <c r="C101" s="28" t="s">
         <v>4063</v>
@@ -41814,7 +41826,7 @@
         <v>4069</v>
       </c>
       <c r="E101" s="18" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="F101" s="16"/>
       <c r="G101" s="16" t="s">
@@ -41823,11 +41835,11 @@
       <c r="J101" s="16"/>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A102" s="19" t="s">
-        <v>4164</v>
+      <c r="A102" s="18" t="s">
+        <v>4207</v>
       </c>
       <c r="B102" s="30" t="s">
-        <v>4043</v>
+        <v>4206</v>
       </c>
       <c r="C102" s="28" t="s">
         <v>4063</v>
@@ -41835,8 +41847,8 @@
       <c r="D102" s="28" t="s">
         <v>4069</v>
       </c>
-      <c r="E102" s="19" t="s">
-        <v>3881</v>
+      <c r="E102" s="18" t="s">
+        <v>332</v>
       </c>
       <c r="F102" s="16"/>
       <c r="G102" s="16" t="s">
@@ -41846,10 +41858,10 @@
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" s="19" t="s">
-        <v>4192</v>
-      </c>
-      <c r="B103" s="32" t="s">
-        <v>4058</v>
+        <v>4164</v>
+      </c>
+      <c r="B103" s="30" t="s">
+        <v>4043</v>
       </c>
       <c r="C103" s="28" t="s">
         <v>4063</v>
@@ -41858,798 +41870,825 @@
         <v>4069</v>
       </c>
       <c r="E103" s="19" t="s">
-        <v>3883</v>
+        <v>3881</v>
       </c>
       <c r="F103" s="16"/>
       <c r="G103" s="16" t="s">
         <v>4099</v>
       </c>
+      <c r="J103" s="16"/>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J104" s="21"/>
+      <c r="A104" s="19" t="s">
+        <v>4192</v>
+      </c>
+      <c r="B104" s="32" t="s">
+        <v>4058</v>
+      </c>
+      <c r="C104" s="28" t="s">
+        <v>4063</v>
+      </c>
+      <c r="D104" s="28" t="s">
+        <v>4069</v>
+      </c>
+      <c r="E104" s="19" t="s">
+        <v>3883</v>
+      </c>
+      <c r="F104" s="16"/>
+      <c r="G104" s="16" t="s">
+        <v>4099</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J105" s="21"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:B6 A19:A23 A30:A31 A24:B24 B25:B26 B12:B15 B18 A2:A4">
-    <cfRule type="expression" dxfId="160" priority="155">
+  <conditionalFormatting sqref="A20:A24 A31:A32 A25:B25 B26:B27 B13:B16 B19 A2:A4 A5:B7">
+    <cfRule type="expression" dxfId="161" priority="155">
       <formula>$C2="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A55:A57">
-    <cfRule type="expression" dxfId="159" priority="188">
-      <formula>$C8="Y"</formula>
+  <conditionalFormatting sqref="A56:A58">
+    <cfRule type="expression" dxfId="160" priority="188">
+      <formula>$C9="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A32">
-    <cfRule type="expression" dxfId="158" priority="186">
-      <formula>$C46="Y"</formula>
+  <conditionalFormatting sqref="A33">
+    <cfRule type="expression" dxfId="159" priority="186">
+      <formula>$C47="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A36">
-    <cfRule type="expression" dxfId="157" priority="182">
+  <conditionalFormatting sqref="A37">
+    <cfRule type="expression" dxfId="158" priority="182">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A33:A35">
-    <cfRule type="expression" dxfId="156" priority="183">
-      <formula>$C38="Y"</formula>
+  <conditionalFormatting sqref="A34:A36">
+    <cfRule type="expression" dxfId="157" priority="183">
+      <formula>$C39="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A39 H76:H81 E76:E81">
-    <cfRule type="expression" dxfId="155" priority="180">
+  <conditionalFormatting sqref="A40 H77:H82 E77:E82">
+    <cfRule type="expression" dxfId="156" priority="180">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A40">
-    <cfRule type="expression" dxfId="154" priority="181">
+  <conditionalFormatting sqref="A41">
+    <cfRule type="expression" dxfId="155" priority="181">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A16">
-    <cfRule type="expression" dxfId="153" priority="179">
+  <conditionalFormatting sqref="A17">
+    <cfRule type="expression" dxfId="154" priority="179">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A50:A51">
-    <cfRule type="expression" dxfId="152" priority="178">
-      <formula>$C42="Y"</formula>
+  <conditionalFormatting sqref="A51:A52">
+    <cfRule type="expression" dxfId="153" priority="178">
+      <formula>$C43="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A54">
-    <cfRule type="expression" dxfId="151" priority="177">
-      <formula>$C34="Y"</formula>
+  <conditionalFormatting sqref="A55">
+    <cfRule type="expression" dxfId="152" priority="177">
+      <formula>$C35="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B60:B61">
-    <cfRule type="expression" dxfId="150" priority="176">
+  <conditionalFormatting sqref="B61:B62">
+    <cfRule type="expression" dxfId="151" priority="176">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A52">
-    <cfRule type="expression" dxfId="149" priority="190">
-      <formula>$C11="Y"</formula>
+  <conditionalFormatting sqref="A53">
+    <cfRule type="expression" dxfId="150" priority="190">
+      <formula>$C12="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A8:A25 A27:A29">
-    <cfRule type="expression" dxfId="148" priority="175">
+  <conditionalFormatting sqref="A9:A26 A28:A30">
+    <cfRule type="expression" dxfId="149" priority="175">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B95">
-    <cfRule type="expression" dxfId="147" priority="171">
+  <conditionalFormatting sqref="B96">
+    <cfRule type="expression" dxfId="148" priority="171">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B99">
-    <cfRule type="expression" dxfId="146" priority="172">
-      <formula>$C8="Y"</formula>
+  <conditionalFormatting sqref="B100">
+    <cfRule type="expression" dxfId="147" priority="172">
+      <formula>$C9="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B98">
+    <cfRule type="expression" dxfId="146" priority="173">
+      <formula>$C12="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B97">
-    <cfRule type="expression" dxfId="145" priority="173">
-      <formula>$C11="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B96">
-    <cfRule type="expression" dxfId="144" priority="174">
+    <cfRule type="expression" dxfId="145" priority="174">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B88:B89">
-    <cfRule type="expression" dxfId="143" priority="169">
+  <conditionalFormatting sqref="B89:B90">
+    <cfRule type="expression" dxfId="144" priority="169">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B87">
-    <cfRule type="expression" dxfId="142" priority="170">
+  <conditionalFormatting sqref="B88">
+    <cfRule type="expression" dxfId="143" priority="170">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B85">
-    <cfRule type="expression" dxfId="141" priority="167">
+  <conditionalFormatting sqref="B86">
+    <cfRule type="expression" dxfId="142" priority="167">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B84 E99">
-    <cfRule type="expression" dxfId="140" priority="168">
-      <formula>$C12="Y"</formula>
+  <conditionalFormatting sqref="B85 E100">
+    <cfRule type="expression" dxfId="141" priority="168">
+      <formula>$C13="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B76:B81">
-    <cfRule type="expression" dxfId="139" priority="162">
-      <formula>#REF!="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B72 H72 E72">
-    <cfRule type="expression" dxfId="138" priority="163">
-      <formula>#REF!="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B75 H75 E75">
-    <cfRule type="expression" dxfId="137" priority="164">
+  <conditionalFormatting sqref="B77:B82">
+    <cfRule type="expression" dxfId="140" priority="162">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B73 H73 E73">
-    <cfRule type="expression" dxfId="136" priority="165">
+    <cfRule type="expression" dxfId="139" priority="163">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B74">
-    <cfRule type="expression" dxfId="135" priority="166">
-      <formula>$C7="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B94">
-    <cfRule type="expression" dxfId="134" priority="193">
-      <formula>$C89="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A37">
-    <cfRule type="expression" dxfId="133" priority="194">
+  <conditionalFormatting sqref="B76 H76 E76">
+    <cfRule type="expression" dxfId="138" priority="164">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7 B27:B28">
-    <cfRule type="expression" dxfId="132" priority="158">
-      <formula>$C7="Y"</formula>
+  <conditionalFormatting sqref="B74 H74 E74">
+    <cfRule type="expression" dxfId="137" priority="165">
+      <formula>#REF!="Y"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="131" priority="159">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B75">
+    <cfRule type="expression" dxfId="136" priority="166">
+      <formula>$C8="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B95">
+    <cfRule type="expression" dxfId="135" priority="193">
+      <formula>$C90="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A38">
+    <cfRule type="expression" dxfId="134" priority="194">
+      <formula>#REF!="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8 B28:B29">
+    <cfRule type="expression" dxfId="133" priority="158">
+      <formula>$C8="Y"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="132" priority="159">
       <formula>"$C3='Y'"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B8:B10">
-    <cfRule type="expression" dxfId="130" priority="157">
-      <formula>$C8="Y"</formula>
+  <conditionalFormatting sqref="B9:B11">
+    <cfRule type="expression" dxfId="131" priority="157">
+      <formula>$C9="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="129" priority="156">
-      <formula>$C11="Y"</formula>
+  <conditionalFormatting sqref="B12">
+    <cfRule type="expression" dxfId="130" priority="156">
+      <formula>$C12="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A28:A29">
-    <cfRule type="expression" dxfId="128" priority="152">
-      <formula>$C33="Y"</formula>
+  <conditionalFormatting sqref="A29:A30">
+    <cfRule type="expression" dxfId="129" priority="152">
+      <formula>$C34="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A38">
-    <cfRule type="expression" dxfId="127" priority="770">
+  <conditionalFormatting sqref="A39">
+    <cfRule type="expression" dxfId="128" priority="770">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A27">
-    <cfRule type="expression" dxfId="126" priority="771">
-      <formula>$C33="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B29">
-    <cfRule type="expression" dxfId="125" priority="141">
+  <conditionalFormatting sqref="A28">
+    <cfRule type="expression" dxfId="127" priority="771">
       <formula>$C34="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B41">
-    <cfRule type="expression" dxfId="124" priority="138">
-      <formula>$C55="Y"</formula>
+  <conditionalFormatting sqref="B30">
+    <cfRule type="expression" dxfId="126" priority="141">
+      <formula>$C35="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B45">
-    <cfRule type="expression" dxfId="123" priority="136">
+  <conditionalFormatting sqref="B42">
+    <cfRule type="expression" dxfId="125" priority="138">
+      <formula>$C56="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B46">
+    <cfRule type="expression" dxfId="124" priority="136">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B42:B44">
-    <cfRule type="expression" dxfId="122" priority="137">
-      <formula>$C47="Y"</formula>
+  <conditionalFormatting sqref="B43:B45">
+    <cfRule type="expression" dxfId="123" priority="137">
+      <formula>$C48="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B48">
-    <cfRule type="expression" dxfId="121" priority="134">
+  <conditionalFormatting sqref="B49">
+    <cfRule type="expression" dxfId="122" priority="134">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B49">
-    <cfRule type="expression" dxfId="120" priority="135">
-      <formula>#REF!="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B46">
-    <cfRule type="expression" dxfId="119" priority="139">
+  <conditionalFormatting sqref="B50">
+    <cfRule type="expression" dxfId="121" priority="135">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="expression" dxfId="118" priority="140">
+    <cfRule type="expression" dxfId="120" priority="139">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A41">
-    <cfRule type="expression" dxfId="117" priority="133">
-      <formula>$C55="Y"</formula>
+  <conditionalFormatting sqref="B48">
+    <cfRule type="expression" dxfId="119" priority="140">
+      <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42">
-    <cfRule type="expression" dxfId="116" priority="132">
-      <formula>$C42="Y"</formula>
+    <cfRule type="expression" dxfId="118" priority="133">
+      <formula>$C56="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43">
+    <cfRule type="expression" dxfId="117" priority="132">
+      <formula>$C43="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B39">
+    <cfRule type="expression" dxfId="116" priority="131">
+      <formula>$C39="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A50">
+    <cfRule type="expression" dxfId="115" priority="122">
+      <formula>$C50="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B34">
+    <cfRule type="expression" dxfId="114" priority="130">
+      <formula>$C34="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B35">
+    <cfRule type="expression" dxfId="113" priority="129">
+      <formula>$C35="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B33">
+    <cfRule type="expression" dxfId="112" priority="128">
+      <formula>$C33="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="expression" dxfId="115" priority="131">
+    <cfRule type="expression" dxfId="111" priority="127">
       <formula>$C38="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A49">
-    <cfRule type="expression" dxfId="114" priority="122">
-      <formula>$C49="Y"</formula>
+  <conditionalFormatting sqref="A47">
+    <cfRule type="expression" dxfId="110" priority="126">
+      <formula>$C47="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B33">
-    <cfRule type="expression" dxfId="113" priority="130">
+  <conditionalFormatting sqref="B37">
+    <cfRule type="expression" dxfId="109" priority="125">
+      <formula>$C37="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B41">
+    <cfRule type="expression" dxfId="108" priority="124">
+      <formula>$C41="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A48">
+    <cfRule type="expression" dxfId="107" priority="123">
+      <formula>$C48="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26">
+    <cfRule type="expression" dxfId="106" priority="773">
       <formula>$C33="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B34">
-    <cfRule type="expression" dxfId="112" priority="129">
-      <formula>$C34="Y"</formula>
+  <conditionalFormatting sqref="A27">
+    <cfRule type="expression" dxfId="105" priority="121">
+      <formula>$C27="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B32">
-    <cfRule type="expression" dxfId="111" priority="128">
-      <formula>$C32="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B37">
-    <cfRule type="expression" dxfId="110" priority="127">
-      <formula>$C37="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A46">
-    <cfRule type="expression" dxfId="109" priority="126">
-      <formula>$C46="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B36">
-    <cfRule type="expression" dxfId="108" priority="125">
-      <formula>$C36="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B40">
-    <cfRule type="expression" dxfId="107" priority="124">
-      <formula>$C40="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A47">
-    <cfRule type="expression" dxfId="106" priority="123">
-      <formula>$C47="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A25">
-    <cfRule type="expression" dxfId="105" priority="773">
-      <formula>$C32="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A26">
-    <cfRule type="expression" dxfId="104" priority="121">
-      <formula>$C26="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B17">
-    <cfRule type="expression" dxfId="103" priority="120">
+  <conditionalFormatting sqref="B18">
+    <cfRule type="expression" dxfId="104" priority="120">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A17">
-    <cfRule type="expression" dxfId="102" priority="119">
-      <formula>#REF!="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B50">
-    <cfRule type="expression" dxfId="101" priority="118">
+  <conditionalFormatting sqref="A18">
+    <cfRule type="expression" dxfId="103" priority="119">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B51">
-    <cfRule type="expression" dxfId="100" priority="117">
-      <formula>$C43="Y"</formula>
+    <cfRule type="expression" dxfId="102" priority="118">
+      <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A53">
-    <cfRule type="expression" dxfId="99" priority="116">
+  <conditionalFormatting sqref="B52">
+    <cfRule type="expression" dxfId="101" priority="117">
+      <formula>$C44="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A54">
+    <cfRule type="expression" dxfId="100" priority="116">
+      <formula>$C46="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B54">
+    <cfRule type="expression" dxfId="99" priority="115">
+      <formula>$C46="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B53">
+    <cfRule type="expression" dxfId="98" priority="114">
       <formula>$C45="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B53">
-    <cfRule type="expression" dxfId="98" priority="115">
-      <formula>$C45="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B52">
-    <cfRule type="expression" dxfId="97" priority="114">
-      <formula>$C44="Y"</formula>
+  <conditionalFormatting sqref="A77">
+    <cfRule type="expression" dxfId="97" priority="107">
+      <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A76">
-    <cfRule type="expression" dxfId="96" priority="107">
+    <cfRule type="expression" dxfId="96" priority="108">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A75">
-    <cfRule type="expression" dxfId="95" priority="108">
+  <conditionalFormatting sqref="A78">
+    <cfRule type="expression" dxfId="95" priority="106">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A77">
-    <cfRule type="expression" dxfId="94" priority="106">
+  <conditionalFormatting sqref="H89:I91">
+    <cfRule type="expression" dxfId="94" priority="102">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H88:I90">
-    <cfRule type="expression" dxfId="93" priority="102">
+  <conditionalFormatting sqref="H87:I88">
+    <cfRule type="expression" dxfId="93" priority="103">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H86:I87">
-    <cfRule type="expression" dxfId="92" priority="103">
+  <conditionalFormatting sqref="H86:I86">
+    <cfRule type="expression" dxfId="92" priority="104">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H85:I85">
-    <cfRule type="expression" dxfId="91" priority="104">
-      <formula>#REF!="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H84:I84 H83 A83">
-    <cfRule type="expression" dxfId="90" priority="105">
-      <formula>$C38="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A85">
-    <cfRule type="expression" dxfId="89" priority="99">
-      <formula>$C40="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A84">
-    <cfRule type="expression" dxfId="88" priority="100">
+  <conditionalFormatting sqref="H85:I85 H84 A84">
+    <cfRule type="expression" dxfId="91" priority="105">
       <formula>$C39="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A86">
-    <cfRule type="expression" dxfId="87" priority="98">
-      <formula>#REF!="Y"</formula>
+    <cfRule type="expression" dxfId="90" priority="99">
+      <formula>$C41="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A85">
+    <cfRule type="expression" dxfId="89" priority="100">
+      <formula>$C40="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A87">
-    <cfRule type="expression" dxfId="86" priority="97">
+    <cfRule type="expression" dxfId="88" priority="98">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A88">
-    <cfRule type="expression" dxfId="85" priority="96">
+    <cfRule type="expression" dxfId="87" priority="97">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A89">
-    <cfRule type="expression" dxfId="84" priority="95">
+    <cfRule type="expression" dxfId="86" priority="96">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J98 E96 J93 E91">
-    <cfRule type="expression" dxfId="83" priority="85">
+  <conditionalFormatting sqref="A90">
+    <cfRule type="expression" dxfId="85" priority="95">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J92 A90">
-    <cfRule type="expression" dxfId="82" priority="86">
+  <conditionalFormatting sqref="J99 E97 J94 E92">
+    <cfRule type="expression" dxfId="84" priority="85">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A91">
-    <cfRule type="expression" dxfId="81" priority="84">
+  <conditionalFormatting sqref="J93 A91">
+    <cfRule type="expression" dxfId="83" priority="86">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A92 E92">
-    <cfRule type="expression" dxfId="80" priority="83">
-      <formula>$C42="Y"</formula>
+  <conditionalFormatting sqref="A92">
+    <cfRule type="expression" dxfId="82" priority="84">
+      <formula>#REF!="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A93 E93">
+    <cfRule type="expression" dxfId="81" priority="83">
+      <formula>$C43="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A95 E95">
+    <cfRule type="expression" dxfId="80" priority="81">
+      <formula>$C60="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A96">
+    <cfRule type="expression" dxfId="79" priority="80">
+      <formula>$C63="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A97">
+    <cfRule type="expression" dxfId="78" priority="79">
+      <formula>#REF!="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A98 E98">
+    <cfRule type="expression" dxfId="77" priority="78">
+      <formula>$C45="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A100">
+    <cfRule type="expression" dxfId="76" priority="77">
+      <formula>$C28="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J105">
+    <cfRule type="expression" dxfId="75" priority="71">
+      <formula>$C83="Y"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="74" priority="72">
+      <formula>"$C3='Y'"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A103 E103">
+    <cfRule type="expression" dxfId="73" priority="69">
+      <formula>$C83="Y"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="72" priority="70">
+      <formula>"$C3='Y'"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B101:B102">
+    <cfRule type="expression" dxfId="71" priority="774">
+      <formula>$J94="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B94">
+    <cfRule type="expression" dxfId="70" priority="775">
+      <formula>$J93="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J102">
+    <cfRule type="expression" dxfId="69" priority="779">
+      <formula>$C28="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J101">
+    <cfRule type="expression" dxfId="68" priority="781">
+      <formula>$C30="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J96">
+    <cfRule type="expression" dxfId="67" priority="785">
+      <formula>$J102="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J98">
+    <cfRule type="expression" dxfId="66" priority="787">
+      <formula>$J101="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J100">
+    <cfRule type="expression" dxfId="65" priority="789">
+      <formula>$C45="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J97">
+    <cfRule type="expression" dxfId="64" priority="793">
+      <formula>$C60="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A94 E94">
-    <cfRule type="expression" dxfId="79" priority="81">
-      <formula>$C59="Y"</formula>
+    <cfRule type="expression" dxfId="63" priority="794">
+      <formula>$J102="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A95">
-    <cfRule type="expression" dxfId="78" priority="80">
-      <formula>$C62="Y"</formula>
+  <conditionalFormatting sqref="J103">
+    <cfRule type="expression" dxfId="62" priority="795">
+      <formula>$J103="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A96">
-    <cfRule type="expression" dxfId="77" priority="79">
+  <conditionalFormatting sqref="A101 E101">
+    <cfRule type="expression" dxfId="61" priority="797">
+      <formula>$J103="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E99">
+    <cfRule type="expression" dxfId="60" priority="811">
+      <formula>$C30="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E96">
+    <cfRule type="expression" dxfId="59" priority="815">
+      <formula>$J101="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E89:E90 E83">
+    <cfRule type="expression" dxfId="58" priority="65">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A97 E97">
-    <cfRule type="expression" dxfId="76" priority="78">
-      <formula>$C44="Y"</formula>
+  <conditionalFormatting sqref="E87:E88">
+    <cfRule type="expression" dxfId="57" priority="66">
+      <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A99">
-    <cfRule type="expression" dxfId="75" priority="77">
-      <formula>$C27="Y"</formula>
+  <conditionalFormatting sqref="E86">
+    <cfRule type="expression" dxfId="56" priority="67">
+      <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J104">
-    <cfRule type="expression" dxfId="74" priority="71">
-      <formula>$C82="Y"</formula>
+  <conditionalFormatting sqref="E84:E85">
+    <cfRule type="expression" dxfId="55" priority="68">
+      <formula>$C37="Y"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="72">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E91">
+    <cfRule type="expression" dxfId="54" priority="64">
+      <formula>#REF!="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H75 E75">
+    <cfRule type="expression" dxfId="53" priority="816">
+      <formula>$C36="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="expression" dxfId="52" priority="58">
+      <formula>#REF!="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="expression" dxfId="51" priority="818">
+      <formula>$C2="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9:E10">
+    <cfRule type="expression" dxfId="50" priority="57">
+      <formula>$C9="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="expression" dxfId="49" priority="55">
+      <formula>#REF!="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12:E13">
+    <cfRule type="expression" dxfId="48" priority="54">
+      <formula>#REF!="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14">
+    <cfRule type="expression" dxfId="47" priority="52">
+      <formula>$C14="Y"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="46" priority="53">
+      <formula>"$C3='Y'"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15">
+    <cfRule type="expression" dxfId="45" priority="50">
+      <formula>$C15="Y"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="51">
+      <formula>"$C3='Y'"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16">
+    <cfRule type="expression" dxfId="43" priority="48">
+      <formula>$C16="Y"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="42" priority="49">
+      <formula>"$C3='Y'"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E19">
+    <cfRule type="expression" dxfId="41" priority="46">
+      <formula>$C19="Y"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="47">
+      <formula>"$C3='Y'"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17">
+    <cfRule type="expression" dxfId="39" priority="45">
+      <formula>#REF!="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18">
+    <cfRule type="expression" dxfId="38" priority="44">
+      <formula>#REF!="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24">
+    <cfRule type="expression" dxfId="37" priority="43">
+      <formula>$C8="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E26">
+    <cfRule type="expression" dxfId="36" priority="41">
+      <formula>$C28="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27">
+    <cfRule type="expression" dxfId="35" priority="40">
+      <formula>$C29="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28">
+    <cfRule type="expression" dxfId="34" priority="39">
+      <formula>$C19="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E29">
+    <cfRule type="expression" dxfId="33" priority="38">
+      <formula>$C20="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E30">
+    <cfRule type="expression" dxfId="32" priority="37">
+      <formula>$C21="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E72">
+    <cfRule type="expression" dxfId="31" priority="33">
+      <formula>#REF!="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E72">
+    <cfRule type="expression" dxfId="30" priority="34">
+      <formula>#REF!="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E71">
+    <cfRule type="expression" dxfId="29" priority="32">
+      <formula>$C108="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E67">
+    <cfRule type="expression" dxfId="28" priority="31">
+      <formula>$C109="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E68:E70">
+    <cfRule type="expression" dxfId="27" priority="30">
+      <formula>$C72="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J95">
+    <cfRule type="expression" dxfId="26" priority="819">
+      <formula>$C43="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E65">
+    <cfRule type="expression" dxfId="25" priority="29">
+      <formula>$C107="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E69">
+    <cfRule type="expression" dxfId="24" priority="27">
+      <formula>#REF!="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E70">
+    <cfRule type="expression" dxfId="23" priority="26">
+      <formula>#REF!="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E66">
+    <cfRule type="expression" dxfId="22" priority="827">
+      <formula>#REF!="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E104">
+    <cfRule type="expression" dxfId="21" priority="24">
+      <formula>$C60="Y"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="25">
+      <formula>"$C3='Y'"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A104">
+    <cfRule type="expression" dxfId="19" priority="22">
+      <formula>$C42="Y"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="23">
       <formula>"$C3='Y'"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A102 E102">
-    <cfRule type="expression" dxfId="72" priority="69">
-      <formula>$C82="Y"</formula>
+    <cfRule type="expression" dxfId="17" priority="830">
+      <formula>#REF!="Y"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="70">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E55">
+    <cfRule type="expression" dxfId="16" priority="20">
+      <formula>$C46="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E56">
+    <cfRule type="expression" dxfId="15" priority="21">
+      <formula>$C37="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B58">
+    <cfRule type="expression" dxfId="14" priority="19">
+      <formula>$C11="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B57">
+    <cfRule type="expression" dxfId="13" priority="18">
+      <formula>$C37="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E57">
+    <cfRule type="expression" dxfId="12" priority="16">
+      <formula>$C48="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E58">
+    <cfRule type="expression" dxfId="11" priority="17">
+      <formula>$C39="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E63">
+    <cfRule type="expression" dxfId="10" priority="14">
+      <formula>#REF!="Y"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="15">
       <formula>"$C3='Y'"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B100:B101">
-    <cfRule type="expression" dxfId="70" priority="774">
-      <formula>$J93="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B93">
-    <cfRule type="expression" dxfId="69" priority="775">
-      <formula>$J92="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J101">
-    <cfRule type="expression" dxfId="68" priority="779">
-      <formula>$C27="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J100">
-    <cfRule type="expression" dxfId="67" priority="781">
-      <formula>$C29="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J95">
-    <cfRule type="expression" dxfId="66" priority="785">
-      <formula>$J101="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J97">
-    <cfRule type="expression" dxfId="65" priority="787">
-      <formula>$J100="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J99">
-    <cfRule type="expression" dxfId="64" priority="789">
-      <formula>$C44="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J96">
-    <cfRule type="expression" dxfId="63" priority="793">
-      <formula>$C59="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A93 E93">
-    <cfRule type="expression" dxfId="62" priority="794">
-      <formula>$J101="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J102">
-    <cfRule type="expression" dxfId="61" priority="795">
-      <formula>$J102="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A100 E100">
-    <cfRule type="expression" dxfId="60" priority="797">
-      <formula>$J102="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E98">
-    <cfRule type="expression" dxfId="59" priority="811">
-      <formula>$C29="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E95">
-    <cfRule type="expression" dxfId="58" priority="815">
-      <formula>$J100="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E88:E89 E82">
-    <cfRule type="expression" dxfId="57" priority="65">
+  <conditionalFormatting sqref="E64">
+    <cfRule type="expression" dxfId="8" priority="10">
       <formula>#REF!="Y"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E86:E87">
-    <cfRule type="expression" dxfId="56" priority="66">
-      <formula>#REF!="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E85">
-    <cfRule type="expression" dxfId="55" priority="67">
-      <formula>#REF!="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E83:E84">
-    <cfRule type="expression" dxfId="54" priority="68">
-      <formula>$C36="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E90">
-    <cfRule type="expression" dxfId="53" priority="64">
-      <formula>#REF!="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H74 E74">
-    <cfRule type="expression" dxfId="52" priority="816">
-      <formula>$C35="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E7">
-    <cfRule type="expression" dxfId="51" priority="58">
-      <formula>#REF!="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2">
-    <cfRule type="expression" dxfId="50" priority="818">
-      <formula>$C2="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E8:E9">
-    <cfRule type="expression" dxfId="49" priority="57">
-      <formula>$C8="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E10">
-    <cfRule type="expression" dxfId="48" priority="55">
-      <formula>#REF!="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E11:E12">
-    <cfRule type="expression" dxfId="47" priority="54">
-      <formula>#REF!="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="46" priority="52">
-      <formula>$C13="Y"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="45" priority="53">
+    <cfRule type="expression" dxfId="7" priority="11">
       <formula>"$C3='Y'"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="44" priority="50">
-      <formula>$C14="Y"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="43" priority="51">
-      <formula>"$C3='Y'"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="42" priority="48">
-      <formula>$C15="Y"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="41" priority="49">
-      <formula>"$C3='Y'"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E18">
-    <cfRule type="expression" dxfId="40" priority="46">
-      <formula>$C18="Y"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="39" priority="47">
-      <formula>"$C3='Y'"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E16">
-    <cfRule type="expression" dxfId="38" priority="45">
-      <formula>#REF!="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E17">
-    <cfRule type="expression" dxfId="37" priority="44">
-      <formula>#REF!="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E19:E23">
-    <cfRule type="expression" dxfId="36" priority="43">
-      <formula>$C3="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="expression" dxfId="35" priority="41">
-      <formula>$C27="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E26">
-    <cfRule type="expression" dxfId="34" priority="40">
-      <formula>$C28="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E27">
-    <cfRule type="expression" dxfId="33" priority="39">
-      <formula>$C18="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E28">
-    <cfRule type="expression" dxfId="32" priority="38">
-      <formula>$C19="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E29">
-    <cfRule type="expression" dxfId="31" priority="37">
-      <formula>$C20="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E71">
-    <cfRule type="expression" dxfId="30" priority="33">
-      <formula>#REF!="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E71">
-    <cfRule type="expression" dxfId="29" priority="34">
-      <formula>#REF!="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E70">
-    <cfRule type="expression" dxfId="28" priority="32">
-      <formula>$C107="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E66">
-    <cfRule type="expression" dxfId="27" priority="31">
-      <formula>$C108="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E67:E69">
-    <cfRule type="expression" dxfId="26" priority="30">
-      <formula>$C71="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J94">
-    <cfRule type="expression" dxfId="25" priority="819">
-      <formula>$C42="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E64">
-    <cfRule type="expression" dxfId="24" priority="29">
-      <formula>$C106="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E68">
-    <cfRule type="expression" dxfId="23" priority="27">
-      <formula>#REF!="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E69">
-    <cfRule type="expression" dxfId="22" priority="26">
-      <formula>#REF!="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E65">
-    <cfRule type="expression" dxfId="21" priority="827">
-      <formula>#REF!="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E103">
-    <cfRule type="expression" dxfId="20" priority="24">
-      <formula>$C59="Y"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="19" priority="25">
-      <formula>"$C3='Y'"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A103">
-    <cfRule type="expression" dxfId="18" priority="22">
-      <formula>$C41="Y"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="17" priority="23">
-      <formula>"$C3='Y'"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A101 E101">
-    <cfRule type="expression" dxfId="16" priority="830">
-      <formula>#REF!="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E54">
-    <cfRule type="expression" dxfId="15" priority="20">
-      <formula>$C45="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E55">
-    <cfRule type="expression" dxfId="14" priority="21">
-      <formula>$C36="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B57">
-    <cfRule type="expression" dxfId="13" priority="19">
-      <formula>$C10="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B56">
-    <cfRule type="expression" dxfId="12" priority="18">
-      <formula>$C36="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E56">
-    <cfRule type="expression" dxfId="11" priority="16">
-      <formula>$C47="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E57">
-    <cfRule type="expression" dxfId="10" priority="17">
-      <formula>$C38="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E62">
-    <cfRule type="expression" dxfId="9" priority="14">
-      <formula>#REF!="Y"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="15">
-      <formula>"$C3='Y'"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E63">
-    <cfRule type="expression" dxfId="7" priority="10">
-      <formula>#REF!="Y"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="11">
-      <formula>"$C3='Y'"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E58:E59">
-    <cfRule type="expression" dxfId="5" priority="9">
-      <formula>#REF!="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B58">
-    <cfRule type="expression" dxfId="4" priority="8">
+  <conditionalFormatting sqref="E59:E60">
+    <cfRule type="expression" dxfId="6" priority="9">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B59">
-    <cfRule type="expression" dxfId="3" priority="7">
+    <cfRule type="expression" dxfId="5" priority="8">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A60:A61">
-    <cfRule type="expression" dxfId="2" priority="6">
+  <conditionalFormatting sqref="B60">
+    <cfRule type="expression" dxfId="4" priority="7">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E60:E61">
-    <cfRule type="expression" dxfId="1" priority="5">
+  <conditionalFormatting sqref="A61:A62">
+    <cfRule type="expression" dxfId="3" priority="6">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A58:A59">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="E61:E62">
+    <cfRule type="expression" dxfId="2" priority="5">
       <formula>#REF!="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A59:A60">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>#REF!="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E20:E23">
+    <cfRule type="expression" dxfId="0" priority="831">
+      <formula>$C3="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>